<commit_message>
updating dataset to show digital version
</commit_message>
<xml_diff>
--- a/assets/data/BenchInfo.xlsx
+++ b/assets/data/BenchInfo.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fariakn\Research\website\assets\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fariakn\Research\resess.github.io\artifacts\MobileCoverage\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFF7B5E3-4D59-4871-9C17-DF5D99384C5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF31AEB-C2B9-4049-88FA-DC5EB744700C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" xr2:uid="{2D0D9300-A13D-45F3-88AA-A9A4F06330F2}"/>
   </bookViews>
@@ -745,9 +745,6 @@
     <t>Books &amp; Reference</t>
   </si>
   <si>
-    <t>Canva: Design, Photo &amp; Video</t>
-  </si>
-  <si>
     <t>com.canva.editor</t>
   </si>
   <si>
@@ -811,9 +808,6 @@
     <t>Sports</t>
   </si>
   <si>
-    <t>Expedia: Hotels, Flights &amp; Car</t>
-  </si>
-  <si>
     <t>com.expedia.bookings</t>
   </si>
   <si>
@@ -844,9 +838,6 @@
     <t>cn.danatech.xingseus</t>
   </si>
   <si>
-    <t>Ticketmaster－Buy, Sell Tickets</t>
-  </si>
-  <si>
     <t>com.ticketmaster.mobile.android.na</t>
   </si>
   <si>
@@ -862,9 +853,6 @@
     <t>Shopping</t>
   </si>
   <si>
-    <t>Lensa: Avatar Maker, Editor</t>
-  </si>
-  <si>
     <t>com.lensa.app</t>
   </si>
   <si>
@@ -1180,385 +1168,397 @@
     <t>android.permission.READ_CONTACTS</t>
   </si>
   <si>
-    <t>android.hardware.camera implied: requested android.permission.CAMERA permission,android.hardware.screen.portrait implied: one or more activities have specified a portrait orientation,android.hardware.wifi implied: requested android.permission.ACCESS_WIFI_STATE permission,android.hardware.faketouch implied: default feature for all apps</t>
-  </si>
-  <si>
-    <t>com.google.android.gms.permission.AD_ID,android.permission.ACCESS_MEDIA_LOCATION,android.permission.FOREGROUND_SERVICE,android.permission.READ_MEDIA_IMAGES,android.permission.VIBRATE,com.android.vending.BILLING,android.permission.WRITE_EXTERNAL_STORAGE,com.applovin.array.apphub.permission.BIND_APPHUB_SERVICE,android.permission.PHOTOS,android.permission.INTERNET,com.ai.polyverse.mirror.DYNAMIC_RECEIVER_NOT_EXPORTED_PERMISSION,android.permission.ACCESS_NETWORK_STATE,android.permission.WAKE_LOCK,com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE,android.permission.ACCESS_WIFI_STATE,android.permission.CAMERA,android.permission.READ_EXTERNAL_STORAGE</t>
-  </si>
-  <si>
-    <t>android.hardware.bluetooth implied: requested android.permission.BLUETOOTH permission, requested android.permission.BLUETOOTH_ADMIN permission, and targetSdkVersion &gt; 4,android.hardware.screen.portrait implied: one or more activities have specified a portrait orientation,android.hardware.location implied: requested android.permission.ACCESS_COARSE_LOCATION permission, and requested android.permission.ACCESS_FINE_LOCATION permission,android.hardware.faketouch implied: default feature for all apps</t>
-  </si>
-  <si>
-    <t>android.permission.BLUETOOTH_ADMIN' maxSdkVersion='30,com.google.android.gms.permission.AD_ID,android.permission.WRITE_CALENDAR,android.permission.FOREGROUND_SERVICE,android.permission.READ_CALENDAR,android.permission.RECEIVE_BOOT_COMPLETED,android.permission.NFC,android.permission.WRITE_EXTERNAL_STORAGE,android.permission.BLUETOOTH' maxSdkVersion='30,android.permission.ACCESS_FINE_LOCATION,android.permission.ACCESS_COARSE_LOCATION,android.permission.ACCESS_NETWORK_STATE,android.permission.WAKE_LOCK,android.permission.ACCESS_WIFI_STATE,android.permission.USE_FINGERPRINT,android.permission.POST_NOTIFICATIONS,com.google.android.c2dm.permission.RECEIVE,android.permission.BLUETOOTH_SCAN,android.permission.VIBRATE,android.permission.CHANGE_WIFI_STATE,android.permission.INTERNET,android.permission.USE_BIOMETRIC,com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE,android.permission.CAMERA,android.permission.READ_EXTERNAL_STORAGE,android.permission.BLUETOOTH_CONNECT,android.permission.WRITE_SETTINGS</t>
-  </si>
-  <si>
-    <t>android.hardware.screen.landscape implied: one or more activities have specified a landscape orientation,android.hardware.faketouch implied: default feature for all apps</t>
-  </si>
-  <si>
-    <t>com.google.android.gms.permission.AD_ID,android.permission.GET_ACCOUNTS,android.permission.AUTHENTICATE_ACCOUNTS,android.permission.FOREGROUND_SERVICE,com.amazon.dcp.metrics.permission.METRICS_PERMISSION,com.amazon.identity.permission.CAN_CALL_MAP_INFORMATION_PROVIDER,amazon.permission.COLLECT_METRICS,android.permission.RECEIVE_BOOT_COMPLETED,android.permission.BLUETOOTH' maxSdkVersion='30,com.samsung.permission.USE_MHDR_SERVICE,com.amazon.dcp.sso.permission.CUSTOMER_ATTRIBUTE_SERVICE,android.permission.ACCESS_FINE_LOCATION,android.permission.ACCESS_COARSE_LOCATION,android.permission.ACCESS_NETWORK_STATE,android.permission.WAKE_LOCK,android.permission.ACCESS_WIFI_STATE,com.amazon.device.environment.permission.SWITCH_STAGE,com.amazon.appmanager.preload.permission.READ_PRELOAD_DEVICE_INFO_PROVIDER,android.permission.VIBRATE' maxSdkVersion='18,android.permission.MANAGE_ACCOUNTS,com.google.android.c2dm.permission.RECEIVE,com.amazon.dcp.sso.permission.USE_DEVICE_CREDENTIALS,com.amazon.identity.permission.GENERIC_IPC,com.amazon.identity.auth.device.perm.AUTH_SDK,com.amazon.dcp.config.permission.DYN_CONFIG_VALUES_UPDATED,android.permission.CHANGE_WIFI_MULTICAST_STATE,com.amazon.dcp.sso.permission.MANAGE_COR_PFM,com.android.vending.BILLING,com.amazon.avod.SDK_ACCESS,com.amazon.CONTENT_PROVIDER_ACCESS,android.permission.SCHEDULE_EXACT_ALARM,android.permission.INTERNET,android.permission.USE_CREDENTIALS,android.permission.CHANGE_NETWORK_STATE,com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE,android.permission.WRITE_EXTERNAL_STORAGE' maxSdkVersion='28,com.amazon.dcp.sso.permission.AmazonAccountPropertyService.property.changed,android.permission.READ_EXTERNAL_STORAGE,com.amazon.identity.permission.CALL_AMAZON_DEVICE_INFORMATION_PROVIDER,android.permission.READ_PHONE_STATE,com.amazon.dcp.sso.permission.account.changed</t>
-  </si>
-  <si>
-    <t>android.hardware.microphone implied: requested android.permission.RECORD_AUDIO permission,android.hardware.faketouch implied: default feature for all apps</t>
-  </si>
-  <si>
-    <t>com.google.android.gms.permission.AD_ID,android.permission.GET_ACCOUNTS,android.permission.FOREGROUND_SERVICE,com.amazon.dcp.metrics.permission.METRICS_PERMISSION,android.permission.EXPAND_STATUS_BAR,amazon.permission.COLLECT_METRICS,com.amazon.kindle.cms.CMS_ACCESS,android.permission.RECEIVE_BOOT_COMPLETED,android.permission.BLUETOOTH' maxSdkVersion='30,android.permission.READ_PHONE_STATE' maxSdkVersion='22,com.amazon.dcp.sso.permission.CUSTOMER_ATTRIBUTE_SERVICE,com.audible.application.externalmediaplayer.permission.WAKE_UP,android.permission.ACCESS_NETWORK_STATE,android.permission.WAKE_LOCK,android.permission.ACCESS_WIFI_STATE,com.amazon.appmanager.preload.permission.READ_PRELOAD_DEVICE_INFO_PROVIDER,android.permission.POST_NOTIFICATIONS,com.amazon.alexa.handsfree.protocols.permission.DATA_SYNC,com.google.android.c2dm.permission.RECEIVE,com.amazon.dcp.sso.permission.USE_DEVICE_CREDENTIALS,com.amazon.identity.auth.device.perm.AUTH_SDK,com.amazon.dcp.config.permission.DYN_CONFIG_VALUES_UPDATED,android.permission.CHANGE_WIFI_MULTICAST_STATE,com.amazon.dcp.sso.permission.MANAGE_COR_PFM,com.android.vending.BILLING,android.permission.RECORD_AUDIO,com.audible.application.permission.C2D_MESSAGE,android.permission.CHANGE_WIFI_STATE,android.permission.INTERNET,com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE,com.amazon.alexa.externalmediaplayer.permission.WAKE_UP,android.permission.WRITE_EXTERNAL_STORAGE' maxSdkVersion='29,android.permission.MODIFY_AUDIO_SETTINGS,android.permission.BLUETOOTH_CONNECT,com.amazon.identity.permission.CALL_AMAZON_DEVICE_INFORMATION_PROVIDER,android.permission.READ_EXTERNAL_STORAGE,com.amazon.dcp.sso.permission.AmazonAccountPropertyService.property.changed,com.amazon.dcp.sso.permission.account.changed</t>
-  </si>
-  <si>
-    <t>android.hardware.screen.landscape implied: one or more activities have specified a landscape orientation,android.hardware.screen.portrait implied: one or more activities have specified a portrait orientation,android.hardware.wifi implied: requested android.permission.ACCESS_WIFI_STATE permission,android.hardware.faketouch implied: default feature for all apps</t>
-  </si>
-  <si>
-    <t>com.google.android.gms.permission.AD_ID,android.permission.FOREGROUND_SERVICE,android.permission.RECEIVE_BOOT_COMPLETED,android.permission.CAMERA' maxSdkVersion='22,android.permission.ACCESS_FINE_LOCATION,ca.autotrader.userapp.DYNAMIC_RECEIVER_NOT_EXPORTED_PERMISSION,android.permission.ACCESS_COARSE_LOCATION,android.permission.INTERNET,android.permission.ACCESS_NETWORK_STATE,android.permission.WAKE_LOCK,com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE,android.permission.ACCESS_WIFI_STATE,ca.autotrader.userapp.permission.READ_EXTERNAL_STORAGE,android.permission.POST_NOTIFICATIONS,com.google.android.c2dm.permission.RECEIVE</t>
-  </si>
-  <si>
-    <t>android.hardware.camera implied: requested android.permission.CAMERA permission,android.hardware.screen.portrait implied: one or more activities have specified a portrait orientation,android.hardware.location implied: requested android.permission.ACCESS_COARSE_LOCATION permission, and requested android.permission.ACCESS_FINE_LOCATION permission,android.hardware.faketouch implied: default feature for all apps</t>
-  </si>
-  <si>
-    <t>android.permission.READ_CONTACTS,com.google.android.gms.permission.AD_ID,com.sonyericsson.home.permission.BROADCAST_BADGE,com.htc.launcher.permission.READ_SETTINGS,android.permission.FOREGROUND_SERVICE,android.permission.SYSTEM_ALERT_WINDOW,android.permission.READ_PROFILE,android.permission.RECEIVE_BOOT_COMPLETED,android.permission.WRITE_EXTERNAL_STORAGE,com.huawei.android.launcher.permission.WRITE_SETTINGS,android.permission.ACCESS_FINE_LOCATION,me.everything.badger.permission.BADGE_COUNT_READ,android.permission.ACCESS_COARSE_LOCATION,com.sec.android.provider.badge.permission.WRITE,com.sec.android.provider.badge.permission.READ,android.permission.ACCESS_NETWORK_STATE,android.permission.WAKE_LOCK,com.anddoes.launcher.permission.UPDATE_COUNT,android.permission.ACCESS_WIFI_STATE,android.permission.POST_NOTIFICATIONS,com.google.android.c2dm.permission.RECEIVE,com.oppo.launcher.permission.WRITE_SETTINGS,oppo.permission.OPPO_COMPONENT_SAFE,android.permission.READ_APP_BADGE,android.permission.ACCESS_BACKGROUND_LOCATION,android.permission.VIBRATE,com.huawei.android.launcher.permission.CHANGE_BADGE,com.android.vending.BILLING,com.majeur.launcher.permission.UPDATE_BADGE,android.permission.SCHEDULE_EXACT_ALARM,com.sonymobile.home.permission.PROVIDER_INSERT_BADGE,com.htc.launcher.permission.UPDATE_SHORTCUT,android.permission.INTERNET,com.huawei.permission.external_app_settings.USE_COMPONENT,com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE,android.permission.ACTIVITY_RECOGNITION,com.huawei.android.launcher.permission.READ_SETTINGS,android.permission.CAMERA,android.permission.READ_EXTERNAL_STORAGE,me.everything.badger.permission.BADGE_COUNT_WRITE,com.google.android.gms.permission.ACTIVITY_RECOGNITION,com.oppo.launcher.permission.READ_SETTINGS</t>
-  </si>
-  <si>
-    <t>android.hardware.bluetooth implied: requested android.permission.BLUETOOTH permission, and targetSdkVersion &gt; 4,android.hardware.camera,android.hardware.screen.portrait implied: one or more activities have specified a portrait orientation,android.hardware.microphone implied: requested android.permission.RECORD_AUDIO permission,android.hardware.location implied: requested android.permission.ACCESS_COARSE_LOCATION permission, and requested android.permission.ACCESS_FINE_LOCATION permission,android.hardware.wifi implied: requested android.permission.ACCESS_WIFI_STATE permission, and requested android.permission.CHANGE_WIFI_STATE permission,android.hardware.faketouch implied: default feature for all apps</t>
-  </si>
-  <si>
-    <t>com.google.android.gms.permission.AD_ID,com.bumble.app.DYNAMIC_RECEIVER_NOT_EXPORTED_PERMISSION,android.permission.GET_ACCOUNTS,com.sonyericsson.home.permission.BROADCAST_BADGE,com.htc.launcher.permission.READ_SETTINGS,android.permission.FOREGROUND_SERVICE,android.permission.READ_PHONE_NUMBERS,android.permission.RECEIVE_BOOT_COMPLETED,com.huawei.android.launcher.permission.WRITE_SETTINGS,android.permission.ACCESS_FINE_LOCATION,android.permission.ACCESS_COARSE_LOCATION,com.sec.android.provider.badge.permission.WRITE,com.sec.android.provider.badge.permission.READ,android.permission.ACCESS_NETWORK_STATE,android.permission.WAKE_LOCK,com.anddoes.launcher.permission.UPDATE_COUNT,android.permission.ACCESS_WIFI_STATE,android.permission.USE_FINGERPRINT,android.permission.POST_NOTIFICATIONS,com.oppo.launcher.permission.WRITE_SETTINGS,com.google.android.c2dm.permission.RECEIVE,android.permission.DISABLE_KEYGUARD,android.permission.READ_APP_BADGE,android.permission.VIBRATE,com.huawei.android.launcher.permission.CHANGE_BADGE,com.android.vending.BILLING,android.permission.RECORD_AUDIO,com.majeur.launcher.permission.UPDATE_BADGE,com.sonymobile.home.permission.PROVIDER_INSERT_BADGE,com.htc.launcher.permission.UPDATE_SHORTCUT,android.permission.CHANGE_WIFI_STATE,android.permission.INTERNET,android.permission.USE_BIOMETRIC,android.permission.CHANGE_NETWORK_STATE,com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE,android.permission.USE_FULL_SCREEN_INTENT,com.badoo.permission.SignaturePrivileged,com.huawei.android.launcher.permission.READ_SETTINGS,android.permission.CAMERA,android.permission.WRITE_EXTERNAL_STORAGE' maxSdkVersion='28,android.permission.MODIFY_AUDIO_SETTINGS,android.permission.READ_EXTERNAL_STORAGE,android.permission.BLUETOOTH,android.permission.BLUETOOTH_CONNECT,android.permission.READ_PHONE_STATE,com.oppo.launcher.permission.READ_SETTINGS</t>
-  </si>
-  <si>
-    <t>android.hardware.screen.portrait,android.hardware.wifi implied: requested android.permission.ACCESS_WIFI_STATE permission,android.hardware.faketouch implied: default feature for all apps</t>
-  </si>
-  <si>
-    <t>com.google.android.gms.permission.AD_ID,android.permission.FOREGROUND_SERVICE,android.permission.VIBRATE,com.android.vending.BILLING,android.permission.RECEIVE_BOOT_COMPLETED,android.permission.WRITE_EXTERNAL_STORAGE,android.permission.INTERNET,android.permission.ACCESS_NETWORK_STATE,com.huawei.appmarket.service.commondata.permission.GET_COMMON_DATA,android.permission.WAKE_LOCK,com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE,android.permission.ACCESS_WIFI_STATE,android.permission.CAMERA,android.permission.READ_EXTERNAL_STORAGE,android.permission.POST_NOTIFICATIONS,com.google.android.c2dm.permission.RECEIVE</t>
-  </si>
-  <si>
-    <t>android.hardware.screen.portrait implied: one or more activities have specified a portrait orientation,android.hardware.microphone implied: requested android.permission.RECORD_AUDIO permission,android.hardware.wifi implied: requested android.permission.ACCESS_WIFI_STATE permission,android.hardware.faketouch implied: default feature for all apps</t>
-  </si>
-  <si>
-    <t>com.hihonor.android.launcher.permission.CHANGE_BADGE,com.google.android.gms.permission.AD_ID,com.sonyericsson.home.permission.BROADCAST_BADGE,com.htc.launcher.permission.READ_SETTINGS,android.permission.FOREGROUND_SERVICE,android.permission.GET_PACKAGE_SIZE' maxSdkVersion='25,android.permission.RECEIVE_BOOT_COMPLETED,android.permission.WRITE_EXTERNAL_STORAGE,com.huawei.android.launcher.permission.WRITE_SETTINGS,com.android.launcher.permission.UNINSTALL_SHORTCUT,me.everything.badger.permission.BADGE_COUNT_READ,com.sec.android.provider.badge.permission.WRITE,com.sec.android.provider.badge.permission.READ,android.permission.ACCESS_NETWORK_STATE,com.vivo.notification.permission.BADGE_ICON,android.permission.WAKE_LOCK,com.anddoes.launcher.permission.UPDATE_COUNT,android.permission.ACCESS_WIFI_STATE,android.permission.HIGH_SAMPLING_RATE_SENSORS,com.oppo.launcher.permission.WRITE_SETTINGS,com.google.android.c2dm.permission.RECEIVE,com.android.launcher.permission.INSTALL_SHORTCUT,com.android.launcher.permission.READ_SETTINGS,android.permission.READ_APP_BADGE,android.permission.VIBRATE,com.huawei.android.launcher.permission.CHANGE_BADGE,com.android.vending.BILLING,android.permission.RECORD_AUDIO,com.majeur.launcher.permission.UPDATE_BADGE,com.sonymobile.home.permission.PROVIDER_INSERT_BADGE,com.htc.launcher.permission.UPDATE_SHORTCUT,android.permission.INTERNET,com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE,com.huawei.android.launcher.permission.READ_SETTINGS,android.permission.CAMERA,android.permission.READ_EXTERNAL_STORAGE,me.everything.badger.permission.BADGE_COUNT_WRITE,android.permission.UPDATE_APP_BADGE,com.oppo.launcher.permission.READ_SETTINGS,com.android.launcher.permission.WRITE_SETTINGS</t>
-  </si>
-  <si>
-    <t>android.hardware.sensor.gyroscope,android.hardware.sensor.accelerometer,android.hardware.bluetooth implied: requested android.permission.BLUETOOTH permission, requested android.permission.BLUETOOTH_ADMIN permission, and targetSdkVersion &gt; 4,android.hardware.screen.landscape implied: one or more activities have specified a landscape orientation,android.hardware.screen.portrait implied: one or more activities have specified a portrait orientation,android.hardware.location implied: requested android.permission.ACCESS_COARSE_LOCATION permission,android.hardware.wifi implied: requested android.permission.ACCESS_WIFI_STATE permission,android.hardware.faketouch implied: default feature for all apps</t>
-  </si>
-  <si>
-    <t>android.permission.READ_MEDIA_VIDEO,com.google.android.gms.permission.AD_ID,android.permission.READ_MEDIA_IMAGES,android.permission.BLUETOOTH_ADMIN,android.permission.VIBRATE,android.permission.NFC,android.permission.WRITE_EXTERNAL_STORAGE,android.permission.ACCESS_COARSE_LOCATION,android.permission.INTERNET,android.permission.ACCESS_NETWORK_STATE,android.permission.WAKE_LOCK,android.permission.ACCESS_WIFI_STATE,android.permission.CAMERA,android.permission.READ_EXTERNAL_STORAGE,android.permission.BLUETOOTH</t>
-  </si>
-  <si>
-    <t>android.hardware.screen.portrait implied: one or more activities have specified a portrait orientation,android.hardware.wifi,android.hardware.faketouch implied: default feature for all apps</t>
-  </si>
-  <si>
-    <t>com.google.android.gms.permission.AD_ID,android.permission.FOREGROUND_SERVICE,android.permission.VIBRATE,custom.permission.NEWS_CONTENT_PROVIDER,android.permission.RECEIVE_BOOT_COMPLETED,com.android.alarm.permission.SET_ALARM,android.permission.INTERNET,android.permission.ACCESS_NETWORK_STATE,android.permission.WAKE_LOCK,com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE,android.permission.ACCESS_WIFI_STATE,ca.cbc.android.sports.permission.C2D_MESSAGE,com.google.android.c2dm.permission.RECEIVE</t>
-  </si>
-  <si>
-    <t>android.hardware.camera,android.hardware.screen.portrait implied: one or more activities have specified a portrait orientation,android.hardware.microphone implied: requested android.permission.RECORD_AUDIO permission,android.hardware.wifi implied: requested android.permission.ACCESS_WIFI_STATE permission,android.hardware.faketouch implied: default feature for all apps</t>
-  </si>
-  <si>
-    <t>com.google.android.gms.permission.AD_ID,com.sonyericsson.home.permission.BROADCAST_BADGE,com.htc.launcher.permission.READ_SETTINGS,android.permission.FOREGROUND_SERVICE,android.permission.RECEIVE_BOOT_COMPLETED,com.scaleup.chatai.permission.C2D_MESSAGE,com.huawei.android.launcher.permission.WRITE_SETTINGS,me.everything.badger.permission.BADGE_COUNT_READ,com.sec.android.provider.badge.permission.WRITE,com.sec.android.provider.badge.permission.READ,android.permission.ACCESS_NETWORK_STATE,android.permission.WAKE_LOCK,com.anddoes.launcher.permission.UPDATE_COUNT,android.permission.ACCESS_WIFI_STATE,com.scaleup.chatai.DYNAMIC_RECEIVER_NOT_EXPORTED_PERMISSION,android.permission.POST_NOTIFICATIONS,com.google.android.c2dm.permission.RECEIVE,com.oppo.launcher.permission.WRITE_SETTINGS,android.permission.READ_APP_BADGE,android.permission.READ_MEDIA_IMAGES,android.permission.VIBRATE,android.permission.REORDER_TASKS,com.huawei.android.launcher.permission.CHANGE_BADGE,com.android.vending.BILLING,android.permission.RECORD_AUDIO,com.majeur.launcher.permission.UPDATE_BADGE,com.sonymobile.home.permission.PROVIDER_INSERT_BADGE,com.htc.launcher.permission.UPDATE_SHORTCUT,android.permission.INTERNET,com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE,com.huawei.android.launcher.permission.READ_SETTINGS,android.permission.CAMERA,android.permission.READ_EXTERNAL_STORAGE,me.everything.badger.permission.BADGE_COUNT_WRITE,com.oppo.launcher.permission.READ_SETTINGS</t>
-  </si>
-  <si>
-    <t>android.permission.READ_CONTACTS,com.google.android.gms.permission.AD_ID,android.permission.GET_ACCOUNTS,com.sonyericsson.home.permission.BROADCAST_BADGE,com.htc.launcher.permission.READ_SETTINGS,android.permission.FOREGROUND_SERVICE,android.permission.RECEIVE_BOOT_COMPLETED,com.huawei.android.launcher.permission.WRITE_SETTINGS,me.everything.badger.permission.BADGE_COUNT_READ,com.sec.android.provider.badge.permission.WRITE,com.sec.android.provider.badge.permission.READ,android.permission.ACCESS_NETWORK_STATE,android.permission.WAKE_LOCK,com.anddoes.launcher.permission.UPDATE_COUNT,android.permission.POST_NOTIFICATIONS,com.google.android.c2dm.permission.RECEIVE,com.oppo.launcher.permission.WRITE_SETTINGS,android.permission.READ_EXTERNAL_STORAGE' maxSdkVersion='32,android.permission.READ_APP_BADGE,android.permission.READ_MEDIA_IMAGES,android.permission.VIBRATE,com.huawei.android.launcher.permission.CHANGE_BADGE,com.android.vending.BILLING,android.permission.RECORD_AUDIO,com.duolingo.DYNAMIC_RECEIVER_NOT_EXPORTED_PERMISSION,com.majeur.launcher.permission.UPDATE_BADGE,com.sonymobile.home.permission.PROVIDER_INSERT_BADGE,com.htc.launcher.permission.UPDATE_SHORTCUT,android.permission.INTERNET,com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE,com.huawei.android.launcher.permission.READ_SETTINGS,android.permission.WRITE_EXTERNAL_STORAGE' maxSdkVersion='28,me.everything.badger.permission.BADGE_COUNT_WRITE,com.oppo.launcher.permission.READ_SETTINGS</t>
-  </si>
-  <si>
-    <t>android.hardware.screen.portrait implied: one or more activities have specified a portrait orientation,android.hardware.location implied: requested android.permission.ACCESS_COARSE_LOCATION permission, and requested android.permission.ACCESS_FINE_LOCATION permission,android.hardware.wifi implied: requested android.permission.ACCESS_WIFI_STATE permission,android.hardware.faketouch implied: default feature for all apps</t>
-  </si>
-  <si>
-    <t>com.google.android.gms.permission.AD_ID,android.permission.READ_SYNC_SETTINGS,android.permission.GET_ACCOUNTS,android.permission.AUTHENTICATE_ACCOUNTS,android.permission.FOREGROUND_SERVICE,android.permission.RECEIVE_BOOT_COMPLETED,android.permission.WRITE_EXTERNAL_STORAGE,android.permission.WRITE_SYNC_SETTINGS,android.permission.READ_SYNC_STATS,android.permission.ACCESS_FINE_LOCATION,android.permission.ACCESS_COARSE_LOCATION,android.permission.INTERNET,android.permission.USE_CREDENTIALS,android.permission.ACCESS_NETWORK_STATE,android.permission.WAKE_LOCK,com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE,android.permission.ACCESS_WIFI_STATE,android.permission.READ_EXTERNAL_STORAGE,android.permission.MANAGE_ACCOUNTS,com.google.android.c2dm.permission.RECEIVE,com.google.android.providers.gsf.permission.READ_GSERVICES</t>
-  </si>
-  <si>
-    <t>android.hardware.screen.portrait implied: one or more activities have specified a portrait orientation,android.hardware.vulkan.version,android.hardware.wifi implied: requested android.permission.ACCESS_WIFI_STATE permission</t>
-  </si>
-  <si>
-    <t>com.google.android.gms.permission.AD_ID,android.permission.FOREGROUND_SERVICE,android.permission.VIBRATE,com.android.vending.BILLING,android.permission.WRITE_EXTERNAL_STORAGE,com.applovin.array.apphub.permission.BIND_APPHUB_SERVICE,android.permission.SCHEDULE_EXACT_ALARM,android.permission.ACCESS_NOTIFICATION_POLICY,android.permission.INTERNET,android.permission.BROADCAST_CLOSE_SYSTEM_DIALOGS' maxSdkVersion='30,android.permission.ACCESS_NETWORK_STATE,android.permission.WAKE_LOCK,com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE,android.permission.ACCESS_WIFI_STATE,android.permission.USE_FULL_SCREEN_INTENT,android.permission.POST_NOTIFICATIONS,android.permission.READ_EXTERNAL_STORAGE,com.google.android.c2dm.permission.RECEIVE</t>
-  </si>
-  <si>
-    <t>android.hardware.screen.portrait implied: one or more activities have specified a portrait orientation,android.hardware.location implied: requested android.permission.ACCESS_COARSE_LOCATION permission, and requested android.permission.ACCESS_FINE_LOCATION permission,android.hardware.faketouch implied: default feature for all apps</t>
-  </si>
-  <si>
-    <t>android.permission.READ_CONTACTS,com.google.android.gms.permission.AD_ID,com.sonyericsson.home.permission.BROADCAST_BADGE,com.htc.launcher.permission.READ_SETTINGS,com.feverup.fever.BRANCH_SHARE_PERMISSION,android.permission.FOREGROUND_SERVICE,android.permission.RECEIVE_BOOT_COMPLETED,android.permission.WRITE_EXTERNAL_STORAGE,com.feverup.fever.DYNAMIC_RECEIVER_NOT_EXPORTED_PERMISSION,com.huawei.android.launcher.permission.WRITE_SETTINGS,android.permission.ACCESS_FINE_LOCATION,com.feverup.fever.permission.C2D_MESSAGE,me.everything.badger.permission.BADGE_COUNT_READ,android.permission.ACCESS_COARSE_LOCATION,com.sec.android.provider.badge.permission.WRITE,com.sec.android.provider.badge.permission.READ,android.permission.ACCESS_NETWORK_STATE,android.permission.WAKE_LOCK,com.anddoes.launcher.permission.UPDATE_COUNT,android.permission.POST_NOTIFICATIONS,com.google.android.c2dm.permission.RECEIVE,com.oppo.launcher.permission.WRITE_SETTINGS,android.permission.READ_EXTERNAL_STORAGE' maxSdkVersion='32,android.permission.READ_MEDIA_VIDEO,android.permission.READ_MEDIA_AUDIO,android.permission.READ_APP_BADGE,android.permission.READ_MEDIA_IMAGES,android.permission.VIBRATE,com.huawei.android.launcher.permission.CHANGE_BADGE,com.majeur.launcher.permission.UPDATE_BADGE,com.sonymobile.home.permission.PROVIDER_INSERT_BADGE,com.htc.launcher.permission.UPDATE_SHORTCUT,com.feverup.fever.BRANCH_PERMISSION,android.permission.INTERNET,com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE,com.huawei.android.launcher.permission.READ_SETTINGS,android.permission.CAMERA,me.everything.badger.permission.BADGE_COUNT_WRITE,com.oppo.launcher.permission.READ_SETTINGS</t>
-  </si>
-  <si>
-    <t>android.hardware.camera implied: requested android.permission.CAMERA permission,android.hardware.screen.landscape implied: one or more activities have specified a landscape orientation,android.hardware.screen.portrait implied: one or more activities have specified a portrait orientation,android.hardware.microphone implied: requested android.permission.RECORD_AUDIO permission,android.hardware.wifi implied: requested android.permission.ACCESS_WIFI_STATE permission, requested android.permission.CHANGE_WIFI_MULTICAST_STATE permission, and requested android.permission.CHANGE_WIFI_STATE permission</t>
-  </si>
-  <si>
-    <t>com.google.android.gms.permission.AD_ID,android.permission.GET_ACCOUNTS,android.permission.DOWNLOAD_WITHOUT_NOTIFICATION,android.permission.FOREGROUND_SERVICE,android.permission.SYSTEM_ALERT_WINDOW,android.permission.RECEIVE_BOOT_COMPLETED,android.permission.WRITE_EXTERNAL_STORAGE,android.permission.ACCESS_FINE_LOCATION,android.permission.ACCESS_COARSE_LOCATION,android.permission.ACCESS_NETWORK_STATE,android.permission.WAKE_LOCK,android.permission.ACCESS_WIFI_STATE,com.google.android.c2dm.permission.RECEIVE,android.permission.ACCESS_BACKGROUND_LOCATION,android.permission.CHANGE_WIFI_MULTICAST_STATE,android.permission.VIBRATE,com.android.vending.BILLING,android.permission.RECORD_AUDIO,com.app.appname.permission.C2D_MESSAGE,android.permission.CHANGE_WIFI_STATE,android.permission.INTERNET,com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE,android.permission.CAMERA,android.permission.READ_EXTERNAL_STORAGE,android.permission.READ_PHONE_STATE</t>
-  </si>
-  <si>
-    <t>android.hardware.screen.portrait implied: one or more activities have specified a portrait orientation,android.software.device_admin,android.hardware.location implied: requested android.permission.ACCESS_COARSE_LOCATION permission, and requested android.permission.ACCESS_FINE_LOCATION permission,android.hardware.wifi implied: requested android.permission.ACCESS_WIFI_STATE permission,android.hardware.faketouch implied: default feature for all apps</t>
-  </si>
-  <si>
-    <t>android.permission.READ_CONTACTS,com.google.android.gms.permission.AD_ID,android.permission.FOREGROUND_SERVICE,android.permission.NFC,android.permission.RECEIVE_BOOT_COMPLETED,android.permission.WRITE_EXTERNAL_STORAGE,android.permission.ACCESS_FINE_LOCATION,com.felicanetworks.mfc.permission.MFC_ACCESS,android.permission.ACCESS_COARSE_LOCATION,android.permission.ACCESS_NETWORK_STATE,android.permission.WAKE_LOCK,android.permission.ACCESS_WIFI_STATE,android.permission.USE_FINGERPRINT,com.google.android.c2dm.permission.RECEIVE,com.google.android.providers.gsf.permission.READ_GSERVICES,android.permission.GET_ACCOUNTS' maxSdkVersion='22,android.permission.GET_PACKAGE_SIZE,com.google.android.apps.walletnfcrel.permission.C2D_MESSAGE,android.permission.VIBRATE,android.permission.INTERNET,android.permission.USE_BIOMETRIC,com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE,android.permission.CAMERA,android.permission.READ_EXTERNAL_STORAGE,android.permission.READ_PHONE_STATE</t>
-  </si>
-  <si>
-    <t>android.permission.READ_CONTACTS,com.google.android.gms.permission.AD_ID,android.permission.GET_ACCOUNTS,android.permission.ACCESS_MEDIA_LOCATION,com.sonyericsson.home.permission.BROADCAST_BADGE,com.htc.launcher.permission.READ_SETTINGS,android.permission.FOREGROUND_SERVICE,android.permission.READ_PHONE_NUMBERS,com.amazon.device.messaging.permission.RECEIVE,android.permission.READ_PROFILE,android.permission.RECEIVE_BOOT_COMPLETED,android.permission.WRITE_EXTERNAL_STORAGE,android.permission.ACCESS_FINE_LOCATION,com.android.launcher.permission.UNINSTALL_SHORTCUT,com.instagram.android.DYNAMIC_RECEIVER_NOT_EXPORTED_PERMISSION,com.instagram.direct.permission.PROTECTED_DEEPLINKING,android.permission.MANAGE_OWN_CALLS,android.permission.ACCESS_NETWORK_STATE,.permission.RECEIVE_ADM_MESSAGE,android.permission.WAKE_LOCK,android.permission.USE_FINGERPRINT,android.permission.POST_NOTIFICATIONS,com.google.android.c2dm.permission.RECEIVE,com.android.launcher.permission.INSTALL_SHORTCUT,android.permission.READ_MEDIA_VIDEO,android.permission.READ_MEDIA_IMAGES,android.permission.VIBRATE,android.permission.REORDER_TASKS,com.huawei.android.launcher.permission.CHANGE_BADGE,com.android.vending.BILLING,android.permission.RECORD_AUDIO,com.facebook.services.identity.FEO2,com.instagram.direct.permission.DIRECT_APP_THREAD_STORE_SERVICE,com.sonymobile.home.permission.PROVIDER_INSERT_BADGE,com.htc.launcher.permission.UPDATE_SHORTCUT,android.permission.INTERNET,android.permission.USE_CREDENTIALS,android.permission.USE_BIOMETRIC,com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE,android.permission.USE_FULL_SCREEN_INTENT,android.permission.CAMERA,android.permission.MODIFY_AUDIO_SETTINGS,com.facebook.katana.provider.ACCESS,android.permission.BLUETOOTH,android.permission.READ_EXTERNAL_STORAGE,android.permission.READ_PHONE_STATE</t>
-  </si>
-  <si>
-    <t>android.hardware.screen.portrait implied: one or more activities have specified a portrait orientation,android.hardware.wifi implied: requested android.permission.ACCESS_WIFI_STATE permission,android.hardware.faketouch implied: default feature for all apps</t>
-  </si>
-  <si>
-    <t>android.permission.READ_EXTERNAL_STORAGE' maxSdkVersion='32,com.google.android.gms.permission.AD_ID,android.permission.FOREGROUND_SERVICE,android.permission.READ_MEDIA_IMAGES,android.permission.VIBRATE,com.android.vending.BILLING,android.permission.RECEIVE_BOOT_COMPLETED,android.permission.BILLING,android.permission.INTERNET,android.permission.ACCESS_NETWORK_STATE,android.permission.WAKE_LOCK,com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE,android.permission.ACCESS_WIFI_STATE,android.permission.WRITE_EXTERNAL_STORAGE' maxSdkVersion='28,android.permission.POST_NOTIFICATIONS,com.google.android.c2dm.permission.RECEIVE</t>
-  </si>
-  <si>
-    <t>android.hardware.screen.portrait implied: one or more activities have specified a portrait orientation,android.hardware.location.network,android.hardware.location,android.hardware.wifi implied: requested android.permission.ACCESS_WIFI_STATE permission, and requested android.permission.CHANGE_WIFI_STATE permission,android.hardware.faketouch implied: default feature for all apps</t>
-  </si>
-  <si>
-    <t>com.google.android.gms.permission.AD_ID,android.permission.GET_ACCOUNTS,com.sonyericsson.home.permission.BROADCAST_BADGE,com.htc.launcher.permission.READ_SETTINGS,android.permission.FOREGROUND_SERVICE,android.permission.AUTHENTICATE_ACCOUNTS,android.permission.RECEIVE_USER_PRESENT,android.permission.READ_EXTERNAL_STORAGE' maxSdkVersion='29,com.sonyericsson.home.action.UPDATE_BADGE,android.permission.RECEIVE_BOOT_COMPLETED,com.huawei.android.launcher.permission.WRITE_SETTINGS,me.everything.badger.permission.BADGE_COUNT_READ,android.permission.ACCESS_COARSE_LOCATION,com.sec.android.provider.badge.permission.WRITE,com.sec.android.provider.badge.permission.READ,android.permission.ACCESS_NETWORK_STATE,android.permission.REQUEST_IGNORE_BATTERY_OPTIMIZATIONS,com.anddoes.launcher.permission.UPDATE_COUNT,android.permission.WAKE_LOCK,android.permission.ACCESS_WIFI_STATE,android.permission.POST_NOTIFICATIONS,com.oppo.launcher.permission.WRITE_SETTINGS,com.google.android.c2dm.permission.RECEIVE,android.permission.READ_APP_BADGE,com.huawei.android.launcher.permission.CHANGE_BADGE,com.android.vending.BILLING,android.permission.WRITE_SYNC_SETTINGS,com.majeur.launcher.permission.UPDATE_BADGE,com.sonymobile.home.permission.PROVIDER_INSERT_BADGE,com.htc.launcher.permission.UPDATE_SHORTCUT,android.permission.CHANGE_WIFI_STATE,android.permission.INTERNET,com.huawei.permission.external_app_settings.USE_COMPONENT,com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE,android.permission.WRITE_EXTERNAL_STORAGE' maxSdkVersion='29,android.permission.USE_FULL_SCREEN_INTENT,com.huawei.android.launcher.permission.READ_SETTINGS,me.everything.badger.permission.BADGE_COUNT_WRITE,com.oppo.launcher.permission.READ_SETTINGS</t>
-  </si>
-  <si>
-    <t>android.hardware.camera,android.hardware.screen.portrait implied: one or more activities have specified a portrait orientation,android.hardware.location implied: requested android.permission.ACCESS_COARSE_LOCATION permission, and requested android.permission.ACCESS_FINE_LOCATION permission,android.hardware.wifi implied: requested android.permission.ACCESS_WIFI_STATE permission, and requested android.permission.CHANGE_WIFI_STATE permission,android.hardware.faketouch implied: default feature for all apps</t>
-  </si>
-  <si>
-    <t>com.google.android.gms.permission.AD_ID,com.mcdonalds.superapp.permission.MAPS_RECEIVE,android.permission.FOREGROUND_SERVICE,android.permission.VIBRATE,android.permission.RECEIVE_BOOT_COMPLETED,android.permission.WRITE_EXTERNAL_STORAGE,com.android.alarm.permission.SET_ALARM,android.permission.ACCESS_FINE_LOCATION,android.permission.CHANGE_WIFI_STATE,android.permission.ACCESS_COARSE_LOCATION,android.permission.INTERNET,android.permission.USE_CREDENTIALS,android.permission.ACCESS_NETWORK_STATE,android.permission.GET_TASKS,android.permission.WAKE_LOCK,com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE,android.permission.ACCESS_WIFI_STATE,android.permission.CAMERA,android.permission.READ_EXTERNAL_STORAGE,com.google.android.c2dm.permission.RECEIVE,android.permission.READ_PHONE_STATE,com.google.android.providers.gsf.permission.READ_GSERVICES</t>
-  </si>
-  <si>
-    <t>android.hardware.bluetooth implied: requested android.permission.BLUETOOTH permission, requested android.permission.BLUETOOTH_ADMIN permission, and targetSdkVersion &gt; 4,android.hardware.camera,android.hardware.screen.portrait implied: one or more activities have specified a portrait orientation,android.hardware.telephony implied: requested a telephony permission,android.hardware.camera.flash</t>
-  </si>
-  <si>
-    <t>android.permission.REQUEST_DELETE_PACKAGES,net.oneplus.launcher.permission.READ_SETTINGS,com.actionlauncher.playstore.permission.READ_SETTINGS,com.myhomescreen.messenger.home.emoji.lite.permission.WRITE_SETTINGS,org.adw.launcher.one.permission.READ_SETTINGS,com.transsion.hilauncher.permission.READ_SETTINGS,com.google.android.apps.nexuslauncher.permission.READ_SETTINGS,org.adwfreak.launcher.permission.READ_SETTINGS,android.permission.WAKE_LOCK,android.permission.CANCEL_NOTIFICATIONS,com.google.android.c2dm.permission.RECEIVE,android.permission.PACKAGE_USAGE_STATS,com.cyanogenmod.trebuchet.permission.READ_SETTINGS,com.myhomescreen.messenger.home.emoji.lite.permission.READ_SETTINGS,android.permission.SET_WALLPAPER_HINTS,com.motorola.launcher3.permission.READ_SETTINGS,android.permission.INTERNET,com.chrislacy.actionlauncher.permission.READ_SETTINGS,android.permission.SET_WALLPAPER,android.permission.BLUETOOTH_CONNECT,com.oppo.launcher.permission.READ_SETTINGS,android.permission.READ_CONTACTS,com.teslacoilsw.launcher.permission.READ_SETTINGS,com.google.android.gms.permission.AD_ID,android.permission.READ_SMS,android.permission.GET_ACCOUNTS,android.permission.FLASHLIGHT,com.htc.launcher.permission.READ_SETTINGS,android.permission.FOREGROUND_SERVICE,android.permission.EXPAND_STATUS_BAR,android.permission.BLUETOOTH_ADMIN,android.permission.RECEIVE_BOOT_COMPLETED,android.permission.WRITE_EXTERNAL_STORAGE,com.anddoes.launcher.permission.READ_SETTINGS,android.permission.ACCESS_NOTIFICATION_POLICY,com.lge.launcher3.permission.READ_SETTINGS,android.permission.ACCESS_NETWORK_STATE,org.adw.launcher.permission.READ_SETTINGS,com.android.launcher.permission.INSTALL_SHORTCUT,android.permission.SEND_SMS,android.permission.RECEIVE_SMS,android.permission.WRITE_SMS,com.android.launcher.permission.READ_SETTINGS,android.permission.VIBRATE,android.permission.RECEIVE_MMS,com.google.android.launcher.permission.READ_SETTINGS,com.tcl.android.launcher.permission.READ_SETTINGS,com.android.launcher3.permission.READ_SETTINGS,com.samsung.android.launcher.permission.READ_SETTINGS,com.motorola.launcher3.permission.WRITE_SETTINGS,com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE,com.huawei.android.launcher.permission.READ_SETTINGS,android.permission.CAMERA,android.permission.READ_EXTERNAL_STORAGE,android.permission.BLUETOOTH,android.permission.READ_PHONE_STATE,android.permission.WRITE_SETTINGS,com.android.launcher.permission.WRITE_SETTINGS</t>
-  </si>
-  <si>
-    <t>android.hardware.screen.portrait implied: one or more activities have specified a portrait orientation,android.hardware.microphone implied: requested android.permission.RECORD_AUDIO permission,android.hardware.location implied: requested android.permission.ACCESS_COARSE_LOCATION permission, and requested android.permission.ACCESS_FINE_LOCATION permission,android.hardware.wifi implied: requested android.permission.ACCESS_WIFI_STATE permission,android.hardware.faketouch implied: default feature for all apps</t>
-  </si>
-  <si>
-    <t>android.permission.BLUETOOTH_PRIVILEGED,android.permission.DOWNLOAD_WITHOUT_NOTIFICATION,android.permission.BLUETOOTH' maxSdkVersion='30,android.permission.ACCESS_COARSE_LOCATION,com.sec.android.provider.badge.permission.WRITE,com.anddoes.launcher.permission.UPDATE_COUNT,android.permission.WAKE_LOCK,android.permission.ACCESS_WIFI_STATE,android.permission.POST_NOTIFICATIONS,android.permission.MANAGE_ACCOUNTS,com.oppo.launcher.permission.WRITE_SETTINGS,com.google.android.c2dm.permission.RECEIVE,android.permission.DISABLE_KEYGUARD,android.permission.BLUETOOTH_SCAN,android.permission.READ_APP_BADGE,android.permission.ACCESS_BACKGROUND_LOCATION,android.permission.RECORD_AUDIO,android.permission.REQUEST_INSTALL_PACKAGES,com.majeur.launcher.permission.UPDATE_BADGE,android.permission.SCHEDULE_EXACT_ALARM,com.sonymobile.home.permission.PROVIDER_INSERT_BADGE,android.permission.INTERNET,android.permission.USE_FULL_SCREEN_INTENT,android.permission.BLUETOOTH_CONNECT,me.everything.badger.permission.BADGE_COUNT_WRITE,com.oppo.launcher.permission.READ_SETTINGS,android.permission.ACCESS_DOWNLOAD_MANAGER,android.permission.BLUETOOTH_ADMIN' maxSdkVersion='30,android.permission.READ_CONTACTS,android.permission.GET_ACCOUNTS,android.permission.CALL_PHONE,com.sonyericsson.home.permission.BROADCAST_BADGE,com.htc.launcher.permission.READ_SETTINGS,android.permission.FOREGROUND_SERVICE,android.permission.AUTHENTICATE_ACCOUNTS,android.permission.EXPAND_STATUS_BAR,android.permission.SYSTEM_ALERT_WINDOW,android.permission.RECEIVE_BOOT_COMPLETED,android.permission.NFC,android.permission.WRITE_EXTERNAL_STORAGE,com.huawei.android.launcher.permission.WRITE_SETTINGS,android.permission.ACCESS_FINE_LOCATION,me.everything.badger.permission.BADGE_COUNT_READ,baidu.push.permission.WRITE_PUSHINFOPROVIDER.com.microsoft.teams,android.permission.MANAGE_OWN_CALLS,com.sec.android.provider.badge.permission.READ,android.permission.ACCESS_NETWORK_STATE,android.permission.REQUEST_IGNORE_BATTERY_OPTIMIZATIONS,android.permission.USE_FINGERPRINT,android.permission.WRITE_CONTACTS,com.microsoft.teams.permission.MIPUSH_RECEIVE,android.permission.VIBRATE,com.huawei.android.launcher.permission.CHANGE_BADGE,android.permission.RECORD_VIDEO,com.htc.launcher.permission.UPDATE_SHORTCUT,android.permission.USE_CREDENTIALS,android.permission.USE_BIOMETRIC,android.permission.CHANGE_NETWORK_STATE,com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE,com.huawei.android.launcher.permission.READ_SETTINGS,android.permission.CAMERA,android.permission.MODIFY_AUDIO_SETTINGS,android.permissAGE,android.permission.READ_EXTERNAL_STORAGE,android.permission.WRITE_SETTINGS,android.permission.READ_PHONE_STATE</t>
-  </si>
-  <si>
-    <t>android.hardware.bluetooth implied: requested android.permission.BLUETOOTH permission, requested android.permission.BLUETOOTH_ADMIN permission, and targetSdkVersion &gt; 4,android.hardware.camera,android.hardware.screen.portrait implied: one or more activities have specified a portrait orientation,android.hardware.microphone implied: requested android.permission.RECORD_AUDIO permission,android.hardware.location implied: requested android.permission.ACCESS_COARSE_LOCATION permission, and requested android.permission.ACCESS_FINE_LOCATION permission,android.hardware.faketouch implied: default feature for all apps</t>
-  </si>
-  <si>
-    <t>android.permission.BLUETOOTH_ADMIN' maxSdkVersion='30,com.google.android.gms.permission.AD_ID,android.permission.BLUETOOTH_PRIVILEGED,android.permission.FOREGROUND_SERVICE,android.permission.RECEIVE_BOOT_COMPLETED,android.permission.BLUETOOTH' maxSdkVersion='30,android.permission.ACCESS_FINE_LOCATION,android.permission.ACCESS_COARSE_LOCATION,android.permission.ACCESS_NETWORK_STATE,android.permission.WAKE_LOCK,android.permission.ACCESS_WIFI_STATE,android.permission.USE_FINGERPRINT,android.permission.POST_NOTIFICATIONS,com.google.android.c2dm.permission.RECEIVE,android.permission.BLUETOOTH_SCAN,android.permission.VIBRATE,android.permission.RECORD_AUDIO,android.permission.INTERNET,android.permission.USE_BIOMETRIC,com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE,android.permission.ACTIVITY_RECOGNITION,android.permission.WRITE_EXTERNAL_STORAGE' maxSdkVersion='28,android.permission.MODIFY_AUDIO_SETTINGS,android.permission.CAMERA,android.permission.READ_EXTERNAL_STORAGE,android.permission.BLUETOOTH_CONNECT,com.google.android.gms.permission.ACTIVITY_RECOGNITION</t>
-  </si>
-  <si>
-    <t>android.hardware.camera,android.hardware.screen.portrait implied: one or more activities have specified a portrait orientation,android.hardware.wifi implied: requested android.permission.ACCESS_WIFI_STATE permission,android.hardware.faketouch implied: default feature for all apps</t>
-  </si>
-  <si>
-    <t>com.google.android.gms.permission.AD_ID,android.permission.ACCESS_MEDIA_LOCATION,android.permission.FOREGROUND_SERVICE,com.android.vending.BILLING,android.permission.RECEIVE_BOOT_COMPLETED,android.permission.WRITE_EXTERNAL_STORAGE,android.permission.INTERNET,cn.danatech.xingseus.permission.C2D_MESSAGE,android.permission.ACCESS_NETWORK_STATE,android.permission.WAKE_LOCK,com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE,android.permission.ACCESS_WIFI_STATE,android.permission.CAMERA,android.permission.READ_EXTERNAL_STORAGE,com.google.android.c2dm.permission.RECEIVE</t>
-  </si>
-  <si>
-    <t>com.google.android.gms.permission.AD_ID,android.permission.READ_CONTACTS,android.permission.GET_ACCOUNTS,android.permission.FOREGROUND_SERVICE,android.permission.RECEIVE_BOOT_COMPLETED,android.permission.NFC,android.permission.ACCESS_FINE_LOCATION,android.permission.ACCESS_COARSE_LOCATION,com.sec.android.provider.badge.permission.WRITE,com.sec.android.provider.badge.permission.READ,android.permission.ACCESS_NETWORK_STATE,android.permission.WAKE_LOCK,android.permission.ACCESS_WIFI_STATE,android.permission.POST_NOTIFICATIONS,com.google.android.c2dm.permission.RECEIVE,com.google.android.providers.gsf.permission.READ_GSERVICES,android.permission.READ_EXTERNAL_STORAGE' maxSdkVersion='32,android.permission.READ_MEDIA_VIDEO,android.permission.READ_MEDIA_IMAGES,android.permission.SCHEDULE_EXACT_ALARM,android.permission.INTERNET,com.pinterest.account.Credentials,com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE,android.permission.WRITE_EXTERNAL_STORAGE' maxSdkVersion='29,android.permission.CAMERA</t>
-  </si>
-  <si>
-    <t>android.hardware.wifi implied: requested android.permission.ACCESS_WIFI_STATE permission,android.hardware.faketouch implied: default feature for all apps</t>
-  </si>
-  <si>
-    <t>com.google.android.gms.permission.AD_ID,android.permission.INTERNET,com.facebook.everythingtogether.contentprovider.GET_DEFERRED_DEEPLINK,android.permission.FOREGROUND_SERVICE,android.permission.ACCESS_NETWORK_STATE,android.permission.WAKE_LOCK,com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE,android.permission.ACCESS_WIFI_STATE,android.permission.POST_NOTIFICATIONS,android.permission.RECEIVE_BOOT_COMPLETED,com.google.android.c2dm.permission.RECEIVE</t>
-  </si>
-  <si>
-    <t>android.permission.READ_CONTACTS,com.google.android.gms.permission.AD_ID,android.permission.CALL_PHONE,android.permission.FOREGROUND_SERVICE,android.permission.WRITE_CALENDAR,android.permission.VIBRATE,android.permission.SYSTEM_ALERT_WINDOW,ca.crea.app.consumer.DYNAMIC_RECEIVER_NOT_EXPORTED_PERMISSION,android.permission.READ_CALENDAR,android.permission.READ_PROFILE,android.permission.RECEIVE_BOOT_COMPLETED,android.permission.WRITE_EXTERNAL_STORAGE,android.permission.ACCESS_FINE_LOCATION,android.permission.ACCESS_COARSE_LOCATION,android.permission.INTERNET,android.permission.ACCESS_NETWORK_STATE,android.permission.WAKE_LOCK,com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE,android.permission.ACCESS_WIFI_STATE,android.permission.READ_EXTERNAL_STORAGE,android.permission.POST_NOTIFICATIONS,com.google.android.c2dm.permission.RECEIVE</t>
-  </si>
-  <si>
-    <t>android.hardware.bluetooth implied: requested android.permission.BLUETOOTH permission, requested android.permission.BLUETOOTH_ADMIN permission, and targetSdkVersion &gt; 4,android.hardware.screen.landscape,android.hardware.microphone implied: requested android.permission.RECORD_AUDIO permission,android.hardware.location implied: requested android.permission.ACCESS_COARSE_LOCATION permission</t>
-  </si>
-  <si>
-    <t>android.permission.DOWNLOAD_WITHOUT_NOTIFICATION,com.samsung.cmh.data.READ,android.permission.WRITE_CALENDAR,com.sec.android.app.clockpackage.permission.READ_ALARM,com.vlingo.midas.permission.BACKUP_RESTORE,com.sec.android.app.sbrowser.permission.BACKUP_RESTORE,com.sec.mms.permission.BACKUP_RESTORE,android.permission.OVERRIDE_WIFI_CONFIG,android.permission.WAKE_LOCK,com.samsung.inputmethod.permission.BACKUP_RESTORE,com.samsung.android.app.provider.episodes.permission.READ_EPISODES_DB,android.permission.PACKAGE_USAGE_STATS,android.permission.GET_PACKAGE_SIZE,com.sec.android.kies.vzwlocation.BROADCAST_DETECT,android.permission.WRITE_OWNER_DATA,android.permission.CHANGE_WIFI_STATE,com.sec.android.phone.permission.READ_CALL_SETTINGS,android.permission.INTERNET,android.permission.GET_TASKS,com.sec.android.app.clockpackage.permission.READ_TIMER,com.sec.android.app.clockpackage.permission.READ_WCCONTENT,com.samsung.android.app.reminder.permission.READ,android.permission.READ_OWNER_DATA,android.permission.NETWORK_STACK,com.samsung.android.scloud.sync.permission.WRITE,android.permission.READ_CONTACTS,android.permission.READ_LOGS,android.permission.READ_SMS,android.permission.READ_SYNC_SETTINGS,android.permission.UPDATE_APP_OPS_STATS,com.samsung.android.internal.intelligence.useranalysis.permission.WRITE_PLACE,android.permission.BLUETOOTH_ADMIN,com.sec.android.easyMover.permission.RUN_AGENT,com.samsung.android.app.notes.sync.STATE_WRITE,com.samsung.android.app.cocktailbarservice.permission.ACCESS_PANEL,android.permission.READ_PROFILE,com.sec.android.app.clockpackage.permission.BACKUP_RESTORE_ALARM,android.permission.RECEIVE_BOOT_COMPLETED,com.samsung.android.memo.BNR,android.permission.CHANGE_COMPONENT_ENABLED_STATE,com.sec.android.app.fm.BROADCAST_DETECT,android.permission.PEERS_MAC_ADDRESS,android.permission.TETHER_PRIVILEGED,com.sec.android.app.browser.permission.IMPORT_BOOKMARK,com.samsung.android.app.omcagent.permission.READ_PROVIDER,com.sec.permission.WIFI_BACKUP,android.permission.WRITE_SMS,com.android.launcher.permission.READ_SETTINGS,com.samsung.android.app.notes.READ,android.permission.VIBRATE,com.sec.android.permission.KIES_BNR,android.permission.REORDER_TASKS,com.samsung.android.memo.READ,android.permission.READ_CALL_LOG,android.permission.NETWORK_SETTINGS,com.google.android.finsky.permission.INSTANT_APP_STATE,com.samsung.android.scloud.sync.permission.READ,android.permission.BLUETOOTH,com.samsung.voiceserviceplatform.permission.BACKUP_RESTORE,android.permission.READ_CALENDAR,com.sec.android.phone.permission.WRITE_CALL_SETTINGS,android.permission.INSTALL_PACKAGES,android.permission.WRITE_MEDIA_STORAGE,com.samsung.android.app.notes.sync.STATE_READ,com.android.browser.permission.READ_HISTORY_BOOKMARKS,android.permission.WRITE_TASKS,com.sec.android.app.music.permission.WRITE_SETTINGS,android.permission.REBOOT,android.permission.CONNECTIVITY_INTERNAL,android.permission.ACCESS_COARSE_LOCATION,com.sec.permission.BACKUP_RESTORE_HOMESCREEN,android.permission.WRITE_PROFILE,android.permission.WRITE_SECURE_SETTINGS,android.permission.ACCESS_WIFI_STATE,com.sec.android.inputmethod.permission.BACKUP_RESTORE,android.permission.READ_TASKS,com.android.vending.setup.PLAY_SETUP_SERVICE,android.permission.CLEAR_APP_CACHE,com.wssnps.permission.COM_WSSNPS,com.samsung.permission.READ_SM_DATA,com.sec.android.widgetapp.q1_penmemo.permission.WRITE,android.permission.RECORD_AUDIO,com.sec.android.app.safetyassurance.permission.PRIVATE,com.sec.android.provider.logsprovider.permission.READ_LOGS,com.sec.android.app.clockpackage.permission.BACKUP_RESTORE_WORLDCLOCK,com.sec.spp.permission.TOKEN_9d7d0e108b0956dbad83c838c1dc3cdd422696c70a07d965193a2908197b48d72eaad4fa3f4a5cb7a55ea5508008cd3c7c7ef96207215606cd858405b9939c4e645f3ff51dc98f0b1ebcb87c0a1fac1432cb0f6ebcc2e4f7cfe72b7af75a0e836b9a9bec9dd54896807da97b3d66f93feaa7829167a41711983541b34e240c0e,com.infraware.provider.SNoteProvider.permission.READ,com.sec.android.widgetapp.q1_penmemo.permission.READ,android.permission.COM_WSSNPS,android.permission.LOCAL_MAC_ADDRESS,com.sec.android.permission.WRITE_MEMO,com.samsung.android.app.shareaccessibilitysettings.permission.READ_WRITE,android.permission.GET_ACCOUNTS,com.samsung.android.providers.context.permission.WRITE_USE_APP_FEATURE_SURVEY,android.permission.SYSTEM_ALERT_WINDOW,com.sec.android.app.calendar.permission.WRITE_CALENDAR_SETTINGS,android.permission.WRITE_EXTERNAL_STORAGE,com.infraware.provider.SNoteProvider.permission.WRITE,com.sec.permission.OTG_CHARGE_BLOCK,android.permission.ACCESS_NETWORK_STATE,android.permission.WRITE_CONTACTS,com.sec.android.permission.READ_MEMO,com.sec.android.kies.calllog.BROADCAST_DETECT,com.sec.android.app.contact.permission.CONTACT_SETTINGS,android.permission.MANAGE_NETWORK_POLICY,android.permission.BACKUP,com.samsung.android.permission.SSRM_NOTIFICATION_PERMISSION,com.sec.android.email.service.BROADCAST_DETECT,com.samsung.android.telephony.provider.permission.ACCESS_RESTORE_STATE,com.samsung.android.launcher.permission.READ_SETTINGS,com.samsung.kidshome.provider.SETUPWIZARD_READ,android.permission.CHANGE_NETWORK_STATE,android.permission.MODIFY_AUDIO_SETTINGS,android.permission.READ_EXTERNAL_STORAGE,android.permission.WRITE_SETTINGS,android.permission.READ_PHONE_STATE</t>
-  </si>
-  <si>
-    <t>android.hardware.bluetooth implied: requested android.permission.BLUETOOTH permission, requested android.permission.BLUETOOTH_ADMIN permission, and targetSdkVersion &gt; 4,android.hardware.camera,android.hardware.screen.portrait implied: one or more activities have specified a portrait orientation,android.hardware.location implied: requested android.permission.ACCESS_COARSE_LOCATION permission, and requested android.permission.ACCESS_FINE_LOCATION permission,android.hardware.wifi implied: requested android.permission.ACCESS_WIFI_STATE permission,android.hardware.faketouch implied: default feature for all apps</t>
-  </si>
-  <si>
-    <t>android.permission.BLUETOOTH_ADMIN' maxSdkVersion='30,com.google.android.gms.permission.AD_ID,android.permission.FLASHLIGHT,android.permission.FOREGROUND_SERVICE,android.permission.RECEIVE_BOOT_COMPLETED,com.android.vending.CHECK_LICENSE,android.permission.BLUETOOTH' maxSdkVersion='30,android.permission.ACCESS_FINE_LOCATION,android.permission.ACCESS_COARSE_LOCATION,com.sephora.permission.C2D_MESSAGE,android.permission.ACCESS_NETWORK_STATE,android.permission.WAKE_LOCK,android.permission.ACCESS_WIFI_STATE,android.permission.POST_NOTIFICATIONS,com.google.android.c2dm.permission.RECEIVE,android.permission.BLUETOOTH_SCAN,android.permission.ACCESS_BACKGROUND_LOCATION,android.permission.VIBRATE,android.permission.REORDER_TASKS,android.permission.CAMERA2,android.permission.INTERNET,com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE,android.permission.CAMERA,android.permission.WRITE_EXTERNAL_STORAGE' maxSdkVersion='28,android.permission.READ_EXTERNAL_STORAGE,android.permission.READ_PHONE_STATE</t>
-  </si>
-  <si>
-    <t>android.hardware.screen.portrait implied: one or more activities have specified a portrait orientation,android.hardware.location implied: requested android.permission.ACCESS_COARSE_LOCATION permission,android.hardware.wifi implied: requested android.permission.ACCESS_WIFI_STATE permission,android.hardware.faketouch implied: default feature for all apps</t>
-  </si>
-  <si>
-    <t>android.permission.READ_PHONE_NUMBERS,android.permission.VIBRATE,android.permission.STORAGE,android.permission.RECEIVE_BOOT_COMPLETED,android.permission.WRITE_EXTERNAL_STORAGE,android.permission.READ_PHONE_STATE' maxSdkVersion='29,android.permission.SCHEDULE_EXACT_ALARM,android.permission.ACCESS_COARSE_LOCATION,android.permission.INTERNET,android.permission.USE_BIOMETRIC,android.permission.ACCESS_NETWORK_STATE,android.permission.WAKE_LOCK,com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE,android.permission.ACCESS_WIFI_STATE,android.permission.USE_FINGERPRINT,android.permission.USE_CREDENTIALS' maxSdkVersion='22,android.permission.CAMERA,android.permission.POST_NOTIFICATIONS,android.permission.READ_EXTERNAL_STORAGE,com.google.android.c2dm.permission.RECEIVE</t>
-  </si>
-  <si>
-    <t>android.hardware.camera,android.hardware.screen.portrait implied: one or more activities have specified a portrait orientation,android.hardware.location implied: requested android.permission.ACCESS_COARSE_LOCATION permission, and requested android.permission.ACCESS_FINE_LOCATION permission,android.hardware.wifi implied: requested android.permission.ACCESS_WIFI_STATE permission,android.hardware.faketouch implied: default feature for all apps</t>
-  </si>
-  <si>
-    <t>com.google.android.gms.permission.AD_ID,android.permission.FOREGROUND_SERVICE,com.loblaw.shoppersdrugmart.DYNAMIC_RECEIVER_NOT_EXPORTED_PERMISSION,android.permission.RECEIVE_BOOT_COMPLETED,android.permission.WRITE_EXTERNAL_STORAGE,android.permission.ACCESS_FINE_LOCATION,android.permission.ACCESS_COARSE_LOCATION,android.permission.INTERNET,android.permission.USE_BIOMETRIC,android.permission.ACCESS_NETWORK_STATE,android.permission.WAKE_LOCK,com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE,android.permission.USE_FINGERPRINT,android.permission.ACCESS_WIFI_STATE,android.permission.CAMERA,android.permission.POST_NOTIFICATIONS,android.permission.READ_EXTERNAL_STORAGE,com.google.android.c2dm.permission.RECEIVE</t>
-  </si>
-  <si>
-    <t>android.hardware.screen.portrait implied: one or more activities have specified a portrait orientation,android.hardware.microphone implied: requested android.permission.RECORD_AUDIO permission,android.hardware.wifi implied: requested android.permission.ACCESS_WIFI_STATE permission, and requested android.permission.CHANGE_WIFI_MULTICAST_STATE permission,android.hardware.faketouch implied: default feature for all apps</t>
-  </si>
-  <si>
-    <t>com.google.android.gms.permission.AD_ID,com.samsung.android.samsungaccount.permission.ACCOUNT_MANAGER,android.permission.GET_ACCOUNTS,android.permission.FOREGROUND_SERVICE_CONNECTED_DEVICE,android.permission.FOREGROUND_SERVICE,android.permission.BLUETOOTH_ADMIN,com.sec.android.app.clockpackage.permission.READ_ALARM,com.spotify.music.permission.C2D_MESSAGE,android.permission.NFC,android.permission.RECEIVE_BOOT_COMPLETED,android.permission.WRITE_EXTERNAL_STORAGE,android.permission.READ_PHONE_STATE' maxSdkVersion='22,android.permission.BLUETOOTH_ADVERTISE,com.spotify.music.permission.SECURED_BROADCAST,android.permission.ACCESS_NETWORK_STATE,com.samsung.WATCH_APP_TYPE.Companion,android.permission.WAKE_LOCK,android.permission.ACCESS_WIFI_STATE,android.permission.POST_NOTIFICATIONS,android.permission.FOREGROUND_SERVICE_MEDIA_PLAYBACK,com.google.android.c2dm.permission.RECEIVE,com.android.launcher.permission.INSTALL_SHORTCUT,android.permission.READ_MEDIA_AUDIO,com.samsung.android.rubin.context.permission.READ_CONTEXT_MANAGER,com.spotify.music.permission.INTERNAL_BROADCAST,com.google.android.apps.meetings.permission.MEET_LIVE_SHARING,android.permission.BLUETOOTH_SCAN,com.spotify.music.DYNAMIC_RECEIVER_NOT_EXPORTED_PERMISSION,android.permission.READ_MEDIA_IMAGES,android.permission.VIBRATE,android.permission.CHANGE_WIFI_MULTICAST_STATE,com.android.vending.BILLING,android.permission.RECORD_AUDIO,android.permission.BROADCAST_STICKY,android.permission.INTERNET,android.permission.USE_CREDENTIALS,com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE,android.permission.MODIFY_AUDIO_SETTINGS,android.permission.READ_EXTERNAL_STORAGE,android.permission.BLUETOOTH,android.permission.BLUETOOTH_CONNECT,com.sony.snei.np.android.account.provider.permission.DUID_READ_PROVIDER,android.permission.FOREGROUND_SERVICE_DATA_SYNC</t>
-  </si>
-  <si>
-    <t>com.google.android.gms.permission.AD_ID,android.permission.VIBRATE,android.permission.RECEIVE_BOOT_COMPLETED,android.permission.RECORD_AUDIO,android.permission.WRITE_EXTERNAL_STORAGE,com.adjust.preinstall.READ_PERMISSION,android.permission.INTERNET,android.permission.ACCESS_NETWORK_STATE,android.permission.WAKE_LOCK,com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE,android.permission.ACCESS_WIFI_STATE,android.permission.CAMERA,com.einnovation.temu.remote_config,android.permission.READ_EXTERNAL_STORAGE,android.permission.POST_NOTIFICATIONS,com.google.android.c2dm.permission.RECEIVE</t>
-  </si>
-  <si>
-    <t>android.hardware.screen.portrait implied: one or more activities have specified a portrait orientation,android.hardware.location implied: requested android.permission.ACCESS_COARSE_LOCATION permission, and requested android.permission.ACCESS_FINE_LOCATION permission,android.hardware.wifi implied: requested android.permission.ACCESS_WIFI_STATE permission, and requested android.permission.CHANGE_WIFI_STATE permission,android.hardware.faketouch implied: default feature for all apps</t>
-  </si>
-  <si>
-    <t>android.permission.READ_EXTERNAL_STORAGE' maxSdkVersion='32,android.permission.READ_MEDIA_VIDEO,com.google.android.gms.permission.AD_ID,android.permission.WRITE_EXTERNAL_STORAGE' maxSdkVersion='32,android.permission.ACCESS_BACKGROUND_LOCATION,android.permission.FOREGROUND_SERVICE,android.permission.READ_MEDIA_IMAGES,android.permission.REORDER_TASKS,com.android.vending.BILLING,android.permission.RECEIVE_BOOT_COMPLETED,android.permission.ACCESS_FINE_LOCATION,android.permission.SCHEDULE_EXACT_ALARM,android.permission.ACCESS_COARSE_LOCATION,android.permission.CHANGE_WIFI_STATE,android.permission.INTERNET,android.permission.USE_CREDENTIALS,android.permission.ACCESS_NETWORK_STATE,android.permission.WAKE_LOCK,android.permission.ACCESS_WIFI_STATE,android.permission.POST_NOTIFICATIONS,android.permission.MANAGE_ACCOUNTS,com.google.android.c2dm.permission.RECEIVE,com.google.android.gms.permission.ACTIVITY_RECOGNITION</t>
-  </si>
-  <si>
-    <t>android.permission.READ_CONTACTS,com.google.android.gms.permission.AD_ID,android.permission.CALL_PHONE,android.permission.WRITE_CALENDAR,android.permission.FOREGROUND_SERVICE,android.permission.VIBRATE,android.permission.READ_CALENDAR,android.permission.REORDER_TASKS,android.permission.RECEIVE_BOOT_COMPLETED,android.permission.WRITE_EXTERNAL_STORAGE,android.permission.ACCESS_FINE_LOCATION,android.permission.ACCESS_COARSE_LOCATION,android.permission.INTERNET,android.permission.ACCESS_NETWORK_STATE,android.permission.WAKE_LOCK,com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE,android.permission.ACCESS_WIFI_STATE,android.permission.CAMERA,android.permission.READ_EXTERNAL_STORAGE,android.permission.READ_PHONE_STATE,com.google.android.c2dm.permission.RECEIVE,com.google.android.providers.gsf.permission.READ_GSERVICES</t>
-  </si>
-  <si>
-    <t>android.hardware.bluetooth implied: requested android.permission.BLUETOOTH permission, and targetSdkVersion &gt; 4,android.hardware.location implied: requested android.permission.ACCESS_COARSE_LOCATION permission</t>
-  </si>
-  <si>
-    <t>android.permission.READ_CONTACTS,android.permission.FLASHLIGHT,com.vivo.aiengine.permission.READ_AWARE_PROVIDER,android.permission.FOREGROUND_SERVICE,android.permission.SYSTEM_ALERT_WINDOW,com.zhiliao.musically.livewallpaper.permission.wallpaperplugin,com.amazon.device.messaging.permission.RECEIVE,com.zhiliaoapp.musically.permission.READ_ACCOUNT,android.permission.RECEIVE_BOOT_COMPLETED,android.permission.WRITE_EXTERNAL_STORAGE,android.permission.BLUETOOTH' maxSdkVersion='30,com.android.launcher.permission.UNINSTALL_SHORTCUT,android.permission.AUTHENTICATE_ACCOUNTS' maxSdkVersion='22,android.permission.ACCESS_COARSE_LOCATION,com.vivo.aiengine.permission.WRITE_AWARE_PROVIDER,com.sec.android.provider.badge.permission.WRITE,com.sec.android.provider.badge.permission.READ,android.permission.ACCESS_NETWORK_STATE,com.tiktok.preload.permission.IDENTIFY,android.permission.WAKE_LOCK,android.permission.ACCESS_WIFI_STATE,com.zhiliaoapp.musically.permission.RECEIVE_ADM_MESSAGE,com.google.android.c2dm.permission.RECEIVE,com.android.launcher.permission.INSTALL_SHORTCUT,com.android.launcher.permission.READ_SETTINGS,com.samsung.android.mapsagent.permission.READ_APP_INFO,com.orange.update.permission.READ_ATTRIBUTION,android.permission.VIBRATE,android.permission.CHANGE_WIFI_MULTICAST_STATE,com.zhiliaoapp.musically.push.permission.MESSAGE,android.permission.REORDER_TASKS,com.android.vending.BILLING,android.permission.RECORD_AUDIO,android.permission.SCHEDULE_EXACT_ALARM,android.permission.INTERNET,com.zhiliaoapp.musically.permission.WRITE_ACCOUNT,android.permission.CHANGE_NETWORK_STATE,com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE,android.permission.CAMERA,android.permission.SET_WALLPAPER,android.permission.MODIFY_AUDIO_SETTINGS,android.permission.READ_EXTERNAL_STORAGE,android.permission.BLUETOOTH_CONNECT</t>
-  </si>
-  <si>
-    <t>com.google.android.gms.permission.AD_ID,android.permission.READ_CONTACTS,android.permission.CALL_PHONE,android.permission.GET_ACCOUNTS,android.permission.FOREGROUND_SERVICE,com.ubercab.permission.C2D_MESSAGE,android.permission.SYSTEM_ALERT_WINDOW,android.permission.RECEIVE_BOOT_COMPLETED,android.permission.WRITE_EXTERNAL_STORAGE,android.permission.ACCESS_FINE_LOCATION,android.permission.ACCESS_COARSE_LOCATION,android.permission.ACCESS_NETWORK_STATE,android.permission.WAKE_LOCK,android.permission.USE_FINGERPRINT,android.permission.ACCESS_WIFI_STATE,android.permission.BROADCAST_CLOSE_SYSTEM_DIALOGS,android.permission.POST_NOTIFICATIONS,com.google.android.c2dm.permission.RECEIVE,android.permission.MANAGE_ACCOUNTS,com.google.android.providers.gsf.permission.READ_GSERVICES,android.permission.READ_MEDIA_IMAGES,com.ubercab.DYNAMIC_RECEIVER_NOT_EXPORTED_PERMISSION,android.permission.VIBRATE,android.permission.SCHEDULE_EXACT_ALARM,android.permission.INTERNET,android.permission.USE_CREDENTIALS,android.permission.USE_BIOMETRIC,com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE,android.permission.CHANGE_NETWORK_STATE,android.permission.USE_FULL_SCREEN_INTENT,android.permission.CAMERA,android.permission.MODIFY_AUDIO_SETTINGS,android.permission.READ_EXTERNAL_STORAGE,android.permission.BLUETOOTH,android.permission.READ_PHONE_STATE</t>
-  </si>
-  <si>
-    <t>android.hardware.touchscreen,android.hardware.screen.portrait,android.hardware.touchscreen.multitouch</t>
-  </si>
-  <si>
-    <t>android.permission.READ_EXTERNAL_STORAGE' maxSdkVersion='32,com.google.android.gms.permission.AD_ID,android.permission.FOREGROUND_SERVICE,BIND_GET_INSTALL_REFERRER_SERVICE,com.android.vending.BILLING,android.permission.WRITE_EXTERNAL_STORAGE,com.android.vending.CHECK_LICENSE,com.singular.preinstall.READ_PERMISSION_SINGULAR,com.vizmanga.android.DYNAMIC_RECEIVER_NOT_EXPORTED_PERMISSION,android.permission.INTERNET,android.permission.ACCESS_NETWORK_STATE,android.permission.GET_TASKS,android.permission.WAKE_LOCK,com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE,android.permission.POST_NOTIFICATIONS,com.google.android.c2dm.permission.RECEIVE</t>
-  </si>
-  <si>
-    <t>android.hardware.screen.portrait implied: one or more activities have specified a portrait orientation,android.hardware.microphone implied: requested android.permission.RECORD_AUDIO permission,android.hardware.faketouch implied: default feature for all apps</t>
-  </si>
-  <si>
-    <t>com.whatsapp.sticker.READ,android.permission.INSTALL_SHORTCUT,android.permission.READ_PHONE_NUMBERS,com.whatsapp.permission.BROADCAST,android.permission.ACCESS_COARSE_LOCATION,com.sec.android.provider.badge.permission.WRITE,android.permission.WAKE_LOCK,android.permission.ACCESS_WIFI_STATE,android.permission.POST_NOTIFICATIONS,android.permission.MANAGE_ACCOUNTS,com.google.android.c2dm.permission.RECEIVE,android.permission.READ_MEDIA_AUDIO,android.permission.RECORD_AUDIO,com.facebook.services.identity.FEO2,android.permission.REQUEST_INSTALL_PACKAGES,android.permission.BROADCAST_STICKY,android.permission.READ_SYNC_STATS,android.permission.SCHEDULE_EXACT_ALARM,com.sonymobile.home.permission.PROVIDER_INSERT_BADGE,android.permission.CHANGE_WIFI_STATE,android.permission.INTERNET,android.permission.GET_TASKS,android.permission.USE_FULL_SCREEN_INTENT,com.whatsapp.permission.MAPS_RECEIVE,android.permission.READ_CONTACTS,com.google.android.gms.permission.AD_ID,android.permission.GET_ACCOUNTS,android.permission.READ_SYNC_SETTINGS,com.sonyericsson.home.permission.BROADCAST_BADGE,com.htc.launcher.permission.READ_SETTINGS,android.permission.AUTHENTICATE_ACCOUNTS,android.permission.FOREGROUND_SERVICE,android.permission.READ_PROFILE,android.permission.NFC,android.permission.RECEIVE_BOOT_COMPLETED,android.permission.WRITE_EXTERNAL_STORAGE,com.huawei.android.launcher.permission.WRITE_SETTINGS,android.permission.ACCESS_FINE_LOCATION,com.android.launcher.permission.UNINSTALL_SHORTCUT,android.permission.MANAGE_OWN_CALLS,com.sec.android.provider.badge.permission.READ,android.permission.ACCESS_NETWORK_STATE,android.permission.USE_FINGERPRINT,android.permission.NEARBY_WIFI_DEVICES,android.permission.WRITE_CONTACTS,com.android.launcher.permission.INSTALL_SHORTCUT,com.google.android.providers.gsf.permission.READ_GSERVICES,android.permission.RECEIVE_SMS,android.permission.SEND_SMS,android.permission.READ_MEDIA_VIDEO,android.permission.READ_MEDIA_IMAGES,android.permission.VIBRATE,com.huawei.android.launcher.permission.CHANGE_BADGE,android.permission.WRITE_SYNC_SETTINGS,com.whatsapp.permission.REGISTRATION,com.htc.launcher.permission.UPDATE_SHORTCUT,android.permission.USE_CREDENTIALS,android.permission.USE_BIOMETRIC,android.permission.CHANGE_NETWORK_STATE,com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE,com.huawei.android.launcher.permission.READ_SETTINGS,android.permission.CAMERA,android.permission.MODIFY_AUDIO_SETTINGS,android.permission.READ_EXTERNAL_STORAGE,android.permission.BLUETOOTH,android.permission.READ_PHONE_STATE</t>
-  </si>
-  <si>
-    <t>com.google.android.gms.permission.AD_ID,com.sonyericsson.home.permission.BROADCAST_BADGE,com.codeway.wonder.DYNAMIC_RECEIVER_NOT_EXPORTED_PERMISSION,com.htc.launcher.permission.READ_SETTINGS,android.permission.FOREGROUND_SERVICE,android.permission.WRITE_EXTERNAL_STORAGE,com.huawei.android.launcher.permission.WRITE_SETTINGS,me.everything.badger.permission.BADGE_COUNT_READ,com.sec.android.provider.badge.permission.WRITE,com.sec.android.provider.badge.permission.READ,android.permission.ACCESS_NETWORK_STATE,android.permission.WAKE_LOCK,com.anddoes.launcher.permission.UPDATE_COUNT,android.permission.ACCESS_WIFI_STATE,com.codeway.wonder.permission.C2D_MESSAGE,android.permission.POST_NOTIFICATIONS,com.google.android.c2dm.permission.RECEIVE,com.oppo.launcher.permission.WRITE_SETTINGS,android.permission.READ_EXTERNAL_STORAGE' maxSdkVersion='32,android.permission.READ_APP_BADGE,android.permission.READ_MEDIA_IMAGES,android.permission.VIBRATE,com.huawei.android.launcher.permission.CHANGE_BADGE,com.android.vending.BILLING,android.permission.RECORD_AUDIO,com.applovin.array.apphub.permission.BIND_APPHUB_SERVICE,com.majeur.launcher.permission.UPDATE_BADGE,android.permission.SCHEDULE_EXACT_ALARM,com.sonymobile.home.permission.PROVIDER_INSERT_BADGE,com.htc.launcher.permission.UPDATE_SHORTCUT,android.permission.INTERNET,com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE,android.permission.USE_FULL_SCREEN_INTENT,com.huawei.android.launcher.permission.READ_SETTINGS,android.permission.CAMERA,me.everything.badger.permission.BADGE_COUNT_WRITE,android.permission.READ_PHONE_STATE,com.oppo.launcher.permission.READ_SETTINGS</t>
-  </si>
-  <si>
     <t xml:space="preserve">Target SDK </t>
   </si>
   <si>
-    <t>android.hardware.bluetooth implied: requested android.permission.BLUETOOTH permission, requested android.permission.BLUETOOTH_ADMIN permission, and targetSdkVersion &gt; 4,android.hardware.location implied: requested android.permission.ACCESS_COARSE_LOCATION permission, and requested android.permission.ACCESS_FINE_LOCATION permission,android.hardware.wifi implied: requested android.permission.ACCESS_WIFI_STATE permission, and requested android.permission.CHANGE_WIFI_STATE permission,android.hardware.faketouch implied: default feature for all apps</t>
-  </si>
-  <si>
-    <t>com.android.launcher.permission.READ_SETTINGS,android.permission.FOREGROUND_SERVICE,android.permission.BLUETOOTH_ADMIN,android.permission.RECEIVE_BOOT_COMPLETED,android.permission.WRITE_EXTERNAL_STORAGE,android.permission.BROADCAST_STICKY,android.permission.KILL_BACKGROUND_PROCESSES,android.permission.ACCESS_FINE_LOCATION,android.permission.ACCESS_NOTIFICATION_POLICY,android.permission.CHANGE_WIFI_STATE,android.permission.ACCESS_COARSE_LOCATION,android.permission.ACCESS_WIFI_STATE,android.permission.MODIFY_AUDIO_SETTINGS,android.permission.BLUETOOTH,android.permission.READ_EXTERNAL_STORAGE,android.permission.READ_PHONE_STATE,com.android.launcher.permission.INSTALL_SHORTCUT</t>
-  </si>
-  <si>
-    <t>android.permission.INTERNET,android.permission.FOREGROUND_SERVICE,android.permission.READ_EXTERNAL_STORAGE,android.permission.RECORD_AUDIO,android.permission.WRITE_EXTERNAL_STORAGE</t>
-  </si>
-  <si>
-    <t>android.hardware.screen.portrait implied: one or more activities have specified a portrait orientation,android.hardware.faketouch implied: default feature for all apps</t>
-  </si>
-  <si>
-    <t>com.eleybourn.bookcatalogue.DYNAMIC_RECEIVER_NOT_EXPORTED_PERMISSION,android.permission.INTERNET,android.permission.VIBRATE,android.permission.ACCESS_NETWORK_STATE,android.permission.READ_EXTERNAL_STORAGE' maxSdkVersion='29,android.permission.ACCESS_WIFI_STATE,android.permission.WRITE_EXTERNAL_STORAGE' maxSdkVersion='29,android.permission.CAMERA,android.permission.POST_NOTIFICATIONS</t>
-  </si>
-  <si>
-    <t>android.permission.INTERNET,android.permission.BLUETOOTH_ADMIN,android.permission.ACCESS_NETWORK_STATE,android.permission.CHANGE_WIFI_MULTICAST_STATE,android.permission.ACCESS_WIFI_STATE,android.permission.BLUETOOTH</t>
-  </si>
-  <si>
-    <t>android.permission.READ_CONTACTS,android.permission.READ_SYNC_SETTINGS,android.permission.SCHEDULE_EXACT_ALARM,com.fsck.k9.DYNAMIC_RECEIVER_NOT_EXPORTED_PERMISSION,android.permission.INTERNET,android.permission.FOREGROUND_SERVICE,android.permission.USE_BIOMETRIC,android.permission.ACCESS_NETWORK_STATE,android.permission.VIBRATE,android.permission.WAKE_LOCK,android.permission.USE_FINGERPRINT,android.permission.RECEIVE_BOOT_COMPLETED</t>
-  </si>
-  <si>
-    <t>android.permission.USE_BIOMETRIC,android.permission.VIBRATE,android.permission.USE_FINGERPRINT,android.permission.READ_EXTERNAL_STORAGE,android.permission.WRITE_EXTERNAL_STORAGE</t>
-  </si>
-  <si>
-    <t>android.permission.GET_ACCOUNTS' maxSdkVersion='22,android.permission.WAKE_LOCK' maxSdkVersion='25,android.permission.READ_SYNC_SETTINGS,android.permission.WRITE_CALENDAR,android.permission.FOREGROUND_SERVICE,android.permission.MANAGE_ACCOUNTS' maxSdkVersion='22,android.permission.READ_CALENDAR,org.totschnig.myexpenses.DYNAMIC_RECEIVER_NOT_EXPORTED_PERMISSION,android.permission.RECEIVE_BOOT_COMPLETED,android.permission.WRITE_EXTERNAL_STORAGE,android.permission.READ_SYNC_STATS,android.permission.WRITE_SYNC_SETTINGS,android.permission.AUTHENTICATE_ACCOUNTS' maxSdkVersion='22,android.permission.INTERNET,android.permission.ACCESS_NETWORK_STATE,android.permission.ACCESS_WIFI_STATE,android.permission.USE_CREDENTIALS' maxSdkVersion='22,android.permission.POST_NOTIFICATIONS,android.permission.READ_EXTERNAL_STORAGE,com.android.launcher.permission.INSTALL_SHORTCUT</t>
-  </si>
-  <si>
-    <t>com.android.launcher.permission.UNINSTALL_SHORTCUT,android.permission.INTERNET,android.permission.READ_EXTERNAL_STORAGE,android.permission.WRITE_EXTERNAL_STORAGE,com.android.launcher.permission.INSTALL_SHORTCUT</t>
-  </si>
-  <si>
-    <t>android.permission.GET_ACCOUNTS' maxSdkVersion='22,android.permission.FOREGROUND_SERVICE,org.wikipedia.DYNAMIC_RECEIVER_NOT_EXPORTED_PERMISSION,android.permission.VIBRATE,android.permission.MANAGE_ACCOUNTS' maxSdkVersion='22,android.permission.RECEIVE_BOOT_COMPLETED,android.permission.WRITE_EXTERNAL_STORAGE,android.permission.AUTHENTICATE_ACCOUNTS' maxSdkVersion='22,android.permission.INTERNET,android.permission.ACCESS_NETWORK_STATE,android.permission.WAKE_LOCK,com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE,android.permission.POST_NOTIFICATIONS,android.permission.READ_EXTERNAL_STORAGE,com.google.android.c2dm.permission.RECEIVE</t>
-  </si>
-  <si>
-    <t>android.hardware.bluetooth implied: requested android.permission.BLUETOOTH permission, and targetSdkVersion &gt; 4</t>
-  </si>
-  <si>
-    <t>android.permission.READ_EXTERNAL_STORAGE' maxSdkVersion='32,android.permission.READ_MEDIA_VIDEO,android.permission.READ_MEDIA_AUDIO,android.permission.GET_ACCOUNTS,org.wordpress.android.DYNAMIC_RECEIVER_NOT_EXPORTED_PERMISSION,android.permission.FOREGROUND_SERVICE,android.permission.READ_MEDIA_IMAGES,android.permission.VIBRATE,android.permission.RECEIVE_BOOT_COMPLETED,com.android.launcher.permission.UNINSTALL_SHORTCUT,android.permission.INTERNET,android.permission.ACCESS_NETWORK_STATE,android.permission.WAKE_LOCK,com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE,android.permission.WRITE_EXTERNAL_STORAGE' maxSdkVersion='29,android.permission.CAMERA,android.permission.POST_NOTIFICATIONS,android.permission.BLUETOOTH,com.google.android.c2dm.permission.RECEIVE,com.android.launcher.permission.INSTALL_SHORTCUT</t>
-  </si>
-  <si>
-    <t>android.permission.ACCESS_FINE_LOCATION,android.permission.ACCESS_COARSE_LOCATION,android.permission.INTERNET,android.permission.WAKE_LOCK,android.permission.READ_EXTERNAL_STORAGE,android.permission.ACCESS_MOCK_LOCATION,android.permission.ACCESS_LOCATION_EXTRA_COMMANDS,android.permission.WRITE_EXTERNAL_STORAGE</t>
-  </si>
-  <si>
-    <t>android.permission.READ_CONTACTS,android.permission.GET_ACCOUNTS,android.permission.READ_SYNC_SETTINGS,android.permission.WRITE_CALENDAR,android.permission.AUTHENTICATE_ACCOUNTS,android.permission.WRITE_CALL_LOG,android.permission.VIBRATE,android.permission.SYSTEM_ALERT_WINDOW,android.permission.READ_CALENDAR,android.permission.WRITE_EXTERNAL_STORAGE,android.permission.WRITE_SYNC_SETTINGS,android.permission.ACCESS_COARSE_LOCATION,android.permission.INTERNET,android.permission.READ_CALL_LOG,android.permission.PERSISTENT_ACTIVITY,android.permission.ACCESS_NETWORK_STATE,android.permission.WAKE_LOCK,android.permission.ACCESS_WIFI_STATE,android.permission.WRITE_CONTACTS,android.permission.READ_EXTERNAL_STORAGE,android.permission.READ_PHONE_STATE,android.permission.MANAGE_ACCOUNTS</t>
-  </si>
-  <si>
-    <t>android.permission.INTERNET,android.permission.READ_EXTERNAL_STORAGE,android.permission.WRITE_EXTERNAL_STORAGE</t>
-  </si>
-  <si>
-    <t>android.hardware.location.gps implied: requested android.permission.ACCESS_FINE_LOCATION permission, and targetSdkVersion &lt; 21,android.hardware.screen.portrait implied: one or more activities have specified a portrait orientation,android.hardware.location.network implied: requested android.permission.ACCESS_COARSE_LOCATION permission, and targetSdkVersion &lt; 21,android.hardware.location implied: requested android.permission.ACCESS_COARSE_LOCATION permission, requested android.permission.ACCESS_FINE_LOCATION permission, and requested android.permission.ACCESS_MOCK_LOCATION permission,android.hardware.faketouch implied: default feature for all apps</t>
-  </si>
-  <si>
-    <t>android.permission.ACCESS_FINE_LOCATION,android.permission.ACCESS_COARSE_LOCATION,android.permission.INTERNET,android.permission.ACCESS_MOCK_LOCATION</t>
-  </si>
-  <si>
-    <t>android.permission.FOREGROUND_SERVICE,android.permission.VIBRATE,android.permission.WAKE_LOCK,android.permission.USE_FULL_SCREEN_INTENT,android.permission.READ_EXTERNAL_STORAGE,android.permission.RECEIVE_BOOT_COMPLETED</t>
-  </si>
-  <si>
-    <t>android.permission.READ_LOGS,android.permission.WAKE_LOCK,android.permission.READ_EXTERNAL_STORAGE,android.permission.WRITE_EXTERNAL_STORAGE</t>
-  </si>
-  <si>
-    <t>android.permission.READ_EXTERNAL_STORAGE,android.permission.WRITE_EXTERNAL_STORAGE,android.permission.READ_PHONE_STATE</t>
-  </si>
-  <si>
-    <t>android.permission.READ_CONTACTS,android.permission.READ_CALL_LOG,android.permission.READ_EXTERNAL_STORAGE,android.permission.WRITE_EXTERNAL_STORAGE,android.permission.READ_PHONE_STATE,com.android.launcher.permission.INSTALL_SHORTCUT</t>
-  </si>
-  <si>
-    <t>android.hardware.bluetooth implied: requested android.permission.BLUETOOTH permission, and targetSdkVersion &gt; 4,android.hardware.telephony implied: requested a telephony permission,android.hardware.faketouch implied: default feature for all apps</t>
-  </si>
-  <si>
-    <t>android.permission.READ_CONTACTS,android.permission.MODIFY_PHONE_STATE,android.permission.READ_CALL_LOG,android.permission.MODIFY_AUDIO_SETTINGS,android.permission.BLUETOOTH,android.permission.RECEIVE_BOOT_COMPLETED,android.permission.READ_PHONE_STATE</t>
-  </si>
-  <si>
-    <t>android.hardware.telephony implied: requested a telephony permission,android.hardware.faketouch implied: default feature for all apps</t>
-  </si>
-  <si>
-    <t>android.permission.RECEIVE_SMS,android.permission.SEND_SMS,android.permission.READ_EXTERNAL_STORAGE,android.permission.WRITE_EXTERNAL_STORAGE,android.permission.READ_PHONE_STATE</t>
-  </si>
-  <si>
-    <t>android.hardware.touchscreen,android.hardware.screen.portrait</t>
-  </si>
-  <si>
-    <t>android.permission.READ_CONTACTS,android.permission.CALL_PHONE,android.permission.MODIFY_PHONE_STATE,android.permission.CALL_PRIVILEGED,android.permission.READ_CALL_LOG,android.permission.WRITE_CALL_LOG,android.permission.VIBRATE,android.permission.WRITE_CONTACTS</t>
-  </si>
-  <si>
-    <t>android.permission.VIBRATE,android.permission.READ_EXTERNAL_STORAGE,android.permission.WRITE_EXTERNAL_STORAGE,android.permission.READ_PHONE_STATE</t>
-  </si>
-  <si>
-    <t>android.permission.READ_CONTACTS,android.permission.READ_CALL_LOG,android.permission.WRITE_CALL_LOG,android.permission.WRITE_CONTACTS,android.permission.READ_EXTERNAL_STORAGE,android.permission.WRITE_EXTERNAL_STORAGE,android.permission.READ_PHONE_STATE</t>
-  </si>
-  <si>
-    <t>android.hardware.microphone implied: requested android.permission.RECORD_AUDIO permission,android.hardware.wifi implied: requested android.permission.ACCESS_WIFI_STATE permission,android.hardware.faketouch implied: default feature for all apps</t>
-  </si>
-  <si>
-    <t>android.permission.INTERNET,android.permission.WAKE_LOCK,android.permission.ACCESS_WIFI_STATE,android.permission.MODIFY_AUDIO_SETTINGS,android.permission.RECORD_AUDIO,android.permission.READ_EXTERNAL_STORAGE,android.permission.READ_PHONE_STATE,android.permission.WRITE_EXTERNAL_STORAGE</t>
-  </si>
-  <si>
-    <t>android.permission.INTERNET,android.permission.ACCESS_NETWORK_STATE,android.permission.READ_EXTERNAL_STORAGE,android.permission.WRITE_EXTERNAL_STORAGE</t>
-  </si>
-  <si>
-    <t>android.hardware.location.network implied: requested android.permission.ACCESS_COARSE_LOCATION permission, and targetSdkVersion &lt; 21,android.hardware.location implied: requested android.permission.ACCESS_COARSE_LOCATION permission,android.hardware.faketouch implied: default feature for all apps</t>
-  </si>
-  <si>
-    <t>android.permission.ACCESS_COARSE_LOCATION,android.permission.VIBRATE,android.permission.READ_EXTERNAL_STORAGE,android.permission.WRITE_EXTERNAL_STORAGE</t>
-  </si>
-  <si>
-    <t>android.permission.READ_EXTERNAL_STORAGE,android.permission.WRITE_EXTERNAL_STORAGE</t>
-  </si>
-  <si>
-    <t>android.permission.SEND_SMS,android.permission.RECEIVE_SMS,android.permission.READ_CONTACTS,android.permission.WRITE_SMS,android.permission.READ_SMS,android.permission.READ_CALL_LOG,android.permission.READ_PHONE_STATE</t>
-  </si>
-  <si>
-    <t>android.permission.INTERNET,android.permission.ACCESS_NETWORK_STATE,android.permission.WAKE_LOCK</t>
-  </si>
-  <si>
-    <t>android.permission.WAKE_LOCK,android.permission.ACCESS_WIFI_STATE,android.permission.RECEIVE_BOOT_COMPLETED,android.permission.READ_EXTERNAL_STORAGE,android.permission.WRITE_EXTERNAL_STORAGE</t>
-  </si>
-  <si>
-    <t>android.permission.INTERNET,android.permission.VIBRATE,android.permission.SET_WALLPAPER,android.permission.RECEIVE_BOOT_COMPLETED,android.permission.READ_EXTERNAL_STORAGE,android.permission.WRITE_EXTERNAL_STORAGE,android.permission.READ_PHONE_STATE</t>
-  </si>
-  <si>
-    <t>android.hardware.screen.portrait implied: one or more activities have specified a portrait orientation,android.hardware.wifi implied: requested android.permission.ACCESS_WIFI_STATE permission, and requested android.permission.CHANGE_WIFI_STATE permission,android.hardware.faketouch implied: default feature for all apps</t>
-  </si>
-  <si>
-    <t>android.permission.WRITE_APN_SETTINGS,android.permission.READ_SYNC_SETTINGS,android.permission.GET_ACCOUNTS,android.permission.FLASHLIGHT,android.permission.MODIFY_PHONE_STATE,android.permission.ACCESS_WIMAX_STATE,android.permission.BLUETOOTH_ADMIN,android.permission.VIBRATE,android.permission.RECEIVE_BOOT_COMPLETED,android.permission.WRITE_SYNC_SETTINGS,android.permission.CHANGE_WIMAX_STATE,android.permission.ACCESS_FINE_LOCATION,android.permission.CHANGE_WIFI_STATE,android.permission.HARDWARE_TEST,android.permission.ACCESS_NETWORK_STATE,android.permission.READ_SECURE_SETTINGS,android.permission.WAKE_LOCK,android.permission.WRITE_SECURE_SETTINGS,android.permission.ACCESS_WIFI_STATE,android.permission.CAMERA,android.permission.BLUETOOTH,android.permission.WRITE_SETTINGS</t>
-  </si>
-  <si>
-    <t>android.permission.READ_CONTACTS,android.permission.WRITE_CONTACTS,android.permission.RECORD_AUDIO,android.permission.READ_EXTERNAL_STORAGE,android.permission.WRITE_SETTINGS,android.permission.WRITE_EXTERNAL_STORAGE</t>
-  </si>
-  <si>
-    <t>android.hardware.location.gps implied: requested android.permission.ACCESS_FINE_LOCATION permission, and targetSdkVersion &lt; 21,android.hardware.bluetooth implied: requested android.permission.BLUETOOTH permission, requested android.permission.BLUETOOTH_ADMIN permission, and targetSdkVersion &gt; 4,android.hardware.microphone implied: requested android.permission.RECORD_AUDIO permission,android.hardware.telephony implied: requested a telephony permission,android.hardware.location implied: requested android.permission.ACCESS_FINE_LOCATION permission,android.hardware.wifi implied: requested android.permission.ACCESS_WIFI_STATE permission, and requested android.permission.CHANGE_WIFI_STATE permission,android.hardware.faketouch implied: default feature for all apps</t>
-  </si>
-  <si>
-    <t>android.permission.READ_CONTACTS,android.permission.READ_LOGS,android.permission.CALL_PHONE,android.permission.GET_ACCOUNTS,android.permission.MODIFY_PHONE_STATE,android.permission.BLUETOOTH_ADMIN,android.permission.RECEIVE_BOOT_COMPLETED,android.permission.WRITE_EXTERNAL_STORAGE,android.permission.ACCESS_FINE_LOCATION,android.permission.ACCESS_NETWORK_STATE,android.permission.PROCESS_OUTGOING_CALLS,android.permission.WAKE_LOCK,android.permission.ACCESS_WIFI_STATE,android.permission.RECEIVE_SMS,android.permission.DISABLE_KEYGUARD,android.permission.VIBRATE,android.permission.RECORD_AUDIO,android.permission.CHANGE_WIFI_STATE,android.permission.READ_CALL_LOG,android.permission.CHANGE_NETWORK_STATE,android.permission.MODIFY_AUDIO_SETTINGS,android.permission.BLUETOOTH,android.permission.READ_EXTERNAL_STORAGE,android.permission.READ_PHONE_STATE,android.permission.WRITE_SETTINGS</t>
-  </si>
-  <si>
-    <t>android.hardware.wifi implied: requested android.permission.ACCESS_WIFI_STATE permission, and requested android.permission.CHANGE_WIFI_STATE permission,android.hardware.faketouch implied: default feature for all apps</t>
-  </si>
-  <si>
-    <t>android.permission.CHANGE_WIFI_STATE,android.permission.INTERNET,android.permission.WAKE_LOCK,android.permission.ACCESS_WIFI_STATE,android.permission.READ_EXTERNAL_STORAGE,android.permission.READ_PHONE_STATE,android.permission.WRITE_EXTERNAL_STORAGE</t>
-  </si>
-  <si>
-    <t>android.permission.INTERNET,android.permission.SET_WALLPAPER,android.permission.RECEIVE_BOOT_COMPLETED,android.permission.READ_EXTERNAL_STORAGE,android.permission.WRITE_EXTERNAL_STORAGE</t>
-  </si>
-  <si>
-    <t>android.permission.INTERNET,android.permission.WAKE_LOCK</t>
-  </si>
-  <si>
-    <t>android.permission.INTERNET,android.permission.READ_CONTACTS,android.permission.WRITE_CONTACTS,android.permission.RECEIVE_BOOT_COMPLETED,android.permission.ACCESS_NETWORK_STATE,android.permission.WAKE_LOCK,android.permission.WRITE_EXTERNAL_STORAGE</t>
+    <t>android.permission.ACCESS_FINE_LOCATION; android.permission.ACCESS_COARSE_LOCATION; android.permission.INTERNET; android.permission.WAKE_LOCK; android.permission.READ_EXTERNAL_STORAGE; android.permission.ACCESS_MOCK_LOCATION; android.permission.ACCESS_LOCATION_EXTRA_COMMANDS; android.permission.WRITE_EXTERNAL_STORAGE</t>
+  </si>
+  <si>
+    <t>android.permission.READ_CONTACTS; android.permission.GET_ACCOUNTS; android.permission.READ_SYNC_SETTINGS; android.permission.WRITE_CALENDAR; android.permission.AUTHENTICATE_ACCOUNTS; android.permission.WRITE_CALL_LOG; android.permission.VIBRATE; android.permission.SYSTEM_ALERT_WINDOW; android.permission.READ_CALENDAR; android.permission.WRITE_EXTERNAL_STORAGE; android.permission.WRITE_SYNC_SETTINGS; android.permission.ACCESS_COARSE_LOCATION; android.permission.INTERNET; android.permission.READ_CALL_LOG; android.permission.PERSISTENT_ACTIVITY; android.permission.ACCESS_NETWORK_STATE; android.permission.WAKE_LOCK; android.permission.ACCESS_WIFI_STATE; android.permission.WRITE_CONTACTS; android.permission.READ_EXTERNAL_STORAGE; android.permission.READ_PHONE_STATE; android.permission.MANAGE_ACCOUNTS</t>
+  </si>
+  <si>
+    <t>android.permission.INTERNET; android.permission.READ_EXTERNAL_STORAGE; android.permission.WRITE_EXTERNAL_STORAGE</t>
+  </si>
+  <si>
+    <t>android.permission.ACCESS_FINE_LOCATION; android.permission.ACCESS_COARSE_LOCATION; android.permission.INTERNET; android.permission.ACCESS_MOCK_LOCATION</t>
+  </si>
+  <si>
+    <t>android.hardware.screen.portrait implied: one or more activities have specified a portrait orientation; android.hardware.faketouch implied: default feature for all apps</t>
+  </si>
+  <si>
+    <t>android.permission.FOREGROUND_SERVICE; android.permission.VIBRATE; android.permission.WAKE_LOCK; android.permission.USE_FULL_SCREEN_INTENT; android.permission.READ_EXTERNAL_STORAGE; android.permission.RECEIVE_BOOT_COMPLETED</t>
+  </si>
+  <si>
+    <t>android.permission.READ_LOGS; android.permission.WAKE_LOCK; android.permission.READ_EXTERNAL_STORAGE; android.permission.WRITE_EXTERNAL_STORAGE</t>
+  </si>
+  <si>
+    <t>android.permission.READ_EXTERNAL_STORAGE; android.permission.WRITE_EXTERNAL_STORAGE; android.permission.READ_PHONE_STATE</t>
+  </si>
+  <si>
+    <t>android.permission.READ_CONTACTS; android.permission.READ_CALL_LOG; android.permission.READ_EXTERNAL_STORAGE; android.permission.WRITE_EXTERNAL_STORAGE; android.permission.READ_PHONE_STATE; com.android.launcher.permission.INSTALL_SHORTCUT</t>
+  </si>
+  <si>
+    <t>android.permission.READ_CONTACTS; android.permission.MODIFY_PHONE_STATE; android.permission.READ_CALL_LOG; android.permission.MODIFY_AUDIO_SETTINGS; android.permission.BLUETOOTH; android.permission.RECEIVE_BOOT_COMPLETED; android.permission.READ_PHONE_STATE</t>
+  </si>
+  <si>
+    <t>android.hardware.telephony implied: requested a telephony permission; android.hardware.faketouch implied: default feature for all apps</t>
+  </si>
+  <si>
+    <t>android.permission.RECEIVE_SMS; android.permission.SEND_SMS; android.permission.READ_EXTERNAL_STORAGE; android.permission.WRITE_EXTERNAL_STORAGE; android.permission.READ_PHONE_STATE</t>
+  </si>
+  <si>
+    <t>android.hardware.touchscreen; android.hardware.screen.portrait</t>
+  </si>
+  <si>
+    <t>android.permission.READ_CONTACTS; android.permission.CALL_PHONE; android.permission.MODIFY_PHONE_STATE; android.permission.CALL_PRIVILEGED; android.permission.READ_CALL_LOG; android.permission.WRITE_CALL_LOG; android.permission.VIBRATE; android.permission.WRITE_CONTACTS</t>
+  </si>
+  <si>
+    <t>android.permission.VIBRATE; android.permission.READ_EXTERNAL_STORAGE; android.permission.WRITE_EXTERNAL_STORAGE; android.permission.READ_PHONE_STATE</t>
+  </si>
+  <si>
+    <t>android.permission.READ_CONTACTS; android.permission.READ_CALL_LOG; android.permission.WRITE_CALL_LOG; android.permission.WRITE_CONTACTS; android.permission.READ_EXTERNAL_STORAGE; android.permission.WRITE_EXTERNAL_STORAGE; android.permission.READ_PHONE_STATE</t>
+  </si>
+  <si>
+    <t>android.hardware.microphone implied: requested android.permission.RECORD_AUDIO permission; android.hardware.wifi implied: requested android.permission.ACCESS_WIFI_STATE permission; android.hardware.faketouch implied: default feature for all apps</t>
+  </si>
+  <si>
+    <t>android.permission.INTERNET; android.permission.WAKE_LOCK; android.permission.ACCESS_WIFI_STATE; android.permission.MODIFY_AUDIO_SETTINGS; android.permission.RECORD_AUDIO; android.permission.READ_EXTERNAL_STORAGE; android.permission.READ_PHONE_STATE; android.permission.WRITE_EXTERNAL_STORAGE</t>
+  </si>
+  <si>
+    <t>android.permission.INTERNET; android.permission.ACCESS_NETWORK_STATE; android.permission.READ_EXTERNAL_STORAGE; android.permission.WRITE_EXTERNAL_STORAGE</t>
+  </si>
+  <si>
+    <t>android.permission.ACCESS_COARSE_LOCATION; android.permission.VIBRATE; android.permission.READ_EXTERNAL_STORAGE; android.permission.WRITE_EXTERNAL_STORAGE</t>
+  </si>
+  <si>
+    <t>android.permission.READ_EXTERNAL_STORAGE; android.permission.WRITE_EXTERNAL_STORAGE</t>
+  </si>
+  <si>
+    <t>android.permission.SEND_SMS; android.permission.RECEIVE_SMS; android.permission.READ_CONTACTS; android.permission.WRITE_SMS; android.permission.READ_SMS; android.permission.READ_CALL_LOG; android.permission.READ_PHONE_STATE</t>
+  </si>
+  <si>
+    <t>android.permission.INTERNET; android.permission.ACCESS_NETWORK_STATE; android.permission.WAKE_LOCK</t>
+  </si>
+  <si>
+    <t>android.hardware.wifi implied: requested android.permission.ACCESS_WIFI_STATE permission; android.hardware.faketouch implied: default feature for all apps</t>
+  </si>
+  <si>
+    <t>android.permission.WAKE_LOCK; android.permission.ACCESS_WIFI_STATE; android.permission.RECEIVE_BOOT_COMPLETED; android.permission.READ_EXTERNAL_STORAGE; android.permission.WRITE_EXTERNAL_STORAGE</t>
+  </si>
+  <si>
+    <t>android.permission.INTERNET; android.permission.VIBRATE; android.permission.SET_WALLPAPER; android.permission.RECEIVE_BOOT_COMPLETED; android.permission.READ_EXTERNAL_STORAGE; android.permission.WRITE_EXTERNAL_STORAGE; android.permission.READ_PHONE_STATE</t>
+  </si>
+  <si>
+    <t>android.permission.WRITE_APN_SETTINGS; android.permission.READ_SYNC_SETTINGS; android.permission.GET_ACCOUNTS; android.permission.FLASHLIGHT; android.permission.MODIFY_PHONE_STATE; android.permission.ACCESS_WIMAX_STATE; android.permission.BLUETOOTH_ADMIN; android.permission.VIBRATE; android.permission.RECEIVE_BOOT_COMPLETED; android.permission.WRITE_SYNC_SETTINGS; android.permission.CHANGE_WIMAX_STATE; android.permission.ACCESS_FINE_LOCATION; android.permission.CHANGE_WIFI_STATE; android.permission.HARDWARE_TEST; android.permission.ACCESS_NETWORK_STATE; android.permission.READ_SECURE_SETTINGS; android.permission.WAKE_LOCK; android.permission.WRITE_SECURE_SETTINGS; android.permission.ACCESS_WIFI_STATE; android.permission.CAMERA; android.permission.BLUETOOTH; android.permission.WRITE_SETTINGS</t>
+  </si>
+  <si>
+    <t>android.permission.INTERNET; android.permission.WAKE_LOCK</t>
+  </si>
+  <si>
+    <t>android.hardware.microphone implied: requested android.permission.RECORD_AUDIO permission; android.hardware.faketouch implied: default feature for all apps</t>
+  </si>
+  <si>
+    <t>android.permission.READ_CONTACTS; android.permission.WRITE_CONTACTS; android.permission.RECORD_AUDIO; android.permission.READ_EXTERNAL_STORAGE; android.permission.WRITE_SETTINGS; android.permission.WRITE_EXTERNAL_STORAGE</t>
+  </si>
+  <si>
+    <t>android.permission.READ_CONTACTS; android.permission.READ_LOGS; android.permission.CALL_PHONE; android.permission.GET_ACCOUNTS; android.permission.MODIFY_PHONE_STATE; android.permission.BLUETOOTH_ADMIN; android.permission.RECEIVE_BOOT_COMPLETED; android.permission.WRITE_EXTERNAL_STORAGE; android.permission.ACCESS_FINE_LOCATION; android.permission.ACCESS_NETWORK_STATE; android.permission.PROCESS_OUTGOING_CALLS; android.permission.WAKE_LOCK; android.permission.ACCESS_WIFI_STATE; android.permission.RECEIVE_SMS; android.permission.DISABLE_KEYGUARD; android.permission.VIBRATE; android.permission.RECORD_AUDIO; android.permission.CHANGE_WIFI_STATE; android.permission.READ_CALL_LOG; android.permission.CHANGE_NETWORK_STATE; android.permission.MODIFY_AUDIO_SETTINGS; android.permission.BLUETOOTH; android.permission.READ_EXTERNAL_STORAGE; android.permission.READ_PHONE_STATE; android.permission.WRITE_SETTINGS</t>
+  </si>
+  <si>
+    <t>android.permission.CHANGE_WIFI_STATE; android.permission.INTERNET; android.permission.WAKE_LOCK; android.permission.ACCESS_WIFI_STATE; android.permission.READ_EXTERNAL_STORAGE; android.permission.READ_PHONE_STATE; android.permission.WRITE_EXTERNAL_STORAGE</t>
+  </si>
+  <si>
+    <t>android.permission.INTERNET; android.permission.READ_CONTACTS; android.permission.WRITE_CONTACTS; android.permission.RECEIVE_BOOT_COMPLETED; android.permission.ACCESS_NETWORK_STATE; android.permission.WAKE_LOCK; android.permission.WRITE_EXTERNAL_STORAGE</t>
+  </si>
+  <si>
+    <t>android.hardware.screen.landscape implied: one or more activities have specified a landscape orientation; android.hardware.faketouch implied: default feature for all apps</t>
+  </si>
+  <si>
+    <t>android.permission.INTERNET; android.permission.SET_WALLPAPER; android.permission.RECEIVE_BOOT_COMPLETED; android.permission.READ_EXTERNAL_STORAGE; android.permission.WRITE_EXTERNAL_STORAGE</t>
+  </si>
+  <si>
+    <t>com.android.launcher.permission.UNINSTALL_SHORTCUT; android.permission.INTERNET; android.permission.READ_EXTERNAL_STORAGE; android.permission.WRITE_EXTERNAL_STORAGE; com.android.launcher.permission.INSTALL_SHORTCUT</t>
+  </si>
+  <si>
+    <t>android.permission.INTERNET; android.permission.BLUETOOTH_ADMIN; android.permission.ACCESS_NETWORK_STATE; android.permission.CHANGE_WIFI_MULTICAST_STATE; android.permission.ACCESS_WIFI_STATE; android.permission.BLUETOOTH</t>
+  </si>
+  <si>
+    <t>com.android.launcher.permission.READ_SETTINGS; android.permission.FOREGROUND_SERVICE; android.permission.BLUETOOTH_ADMIN; android.permission.RECEIVE_BOOT_COMPLETED; android.permission.WRITE_EXTERNAL_STORAGE; android.permission.BROADCAST_STICKY; android.permission.KILL_BACKGROUND_PROCESSES; android.permission.ACCESS_FINE_LOCATION; android.permission.ACCESS_NOTIFICATION_POLICY; android.permission.CHANGE_WIFI_STATE; android.permission.ACCESS_COARSE_LOCATION; android.permission.ACCESS_WIFI_STATE; android.permission.MODIFY_AUDIO_SETTINGS; android.permission.BLUETOOTH; android.permission.READ_EXTERNAL_STORAGE; android.permission.READ_PHONE_STATE; com.android.launcher.permission.INSTALL_SHORTCUT</t>
+  </si>
+  <si>
+    <t>android.hardware.screen.portrait implied: one or more activities have specified a portrait orientation; android.hardware.wifi implied: requested android.permission.ACCESS_WIFI_STATE permission; android.hardware.faketouch implied: default feature for all apps</t>
+  </si>
+  <si>
+    <t>com.eleybourn.bookcatalogue.DYNAMIC_RECEIVER_NOT_EXPORTED_PERMISSION; android.permission.INTERNET; android.permission.VIBRATE; android.permission.ACCESS_NETWORK_STATE; android.permission.READ_EXTERNAL_STORAGE' maxSdkVersion='29; android.permission.ACCESS_WIFI_STATE; android.permission.WRITE_EXTERNAL_STORAGE' maxSdkVersion='29; android.permission.CAMERA; android.permission.POST_NOTIFICATIONS</t>
+  </si>
+  <si>
+    <t>android.permission.INTERNET; android.permission.FOREGROUND_SERVICE; android.permission.READ_EXTERNAL_STORAGE; android.permission.RECORD_AUDIO; android.permission.WRITE_EXTERNAL_STORAGE</t>
+  </si>
+  <si>
+    <t>android.permission.USE_BIOMETRIC; android.permission.VIBRATE; android.permission.USE_FINGERPRINT; android.permission.READ_EXTERNAL_STORAGE; android.permission.WRITE_EXTERNAL_STORAGE</t>
+  </si>
+  <si>
+    <t>android.permission.READ_CONTACTS; android.permission.READ_SYNC_SETTINGS; android.permission.SCHEDULE_EXACT_ALARM; com.fsck.k9.DYNAMIC_RECEIVER_NOT_EXPORTED_PERMISSION; android.permission.INTERNET; android.permission.FOREGROUND_SERVICE; android.permission.USE_BIOMETRIC; android.permission.ACCESS_NETWORK_STATE; android.permission.VIBRATE; android.permission.WAKE_LOCK; android.permission.USE_FINGERPRINT; android.permission.RECEIVE_BOOT_COMPLETED</t>
+  </si>
+  <si>
+    <t>android.permission.GET_ACCOUNTS' maxSdkVersion='22; android.permission.WAKE_LOCK' maxSdkVersion='25; android.permission.READ_SYNC_SETTINGS; android.permission.WRITE_CALENDAR; android.permission.FOREGROUND_SERVICE; android.permission.MANAGE_ACCOUNTS' maxSdkVersion='22; android.permission.READ_CALENDAR; org.totschnig.myexpenses.DYNAMIC_RECEIVER_NOT_EXPORTED_PERMISSION; android.permission.RECEIVE_BOOT_COMPLETED; android.permission.WRITE_EXTERNAL_STORAGE; android.permission.READ_SYNC_STATS; android.permission.WRITE_SYNC_SETTINGS; android.permission.AUTHENTICATE_ACCOUNTS' maxSdkVersion='22; android.permission.INTERNET; android.permission.ACCESS_NETWORK_STATE; android.permission.ACCESS_WIFI_STATE; android.permission.USE_CREDENTIALS' maxSdkVersion='22; android.permission.POST_NOTIFICATIONS; android.permission.READ_EXTERNAL_STORAGE; com.android.launcher.permission.INSTALL_SHORTCUT</t>
+  </si>
+  <si>
+    <t>android.permission.GET_ACCOUNTS' maxSdkVersion='22; android.permission.FOREGROUND_SERVICE; org.wikipedia.DYNAMIC_RECEIVER_NOT_EXPORTED_PERMISSION; android.permission.VIBRATE; android.permission.MANAGE_ACCOUNTS' maxSdkVersion='22; android.permission.RECEIVE_BOOT_COMPLETED; android.permission.WRITE_EXTERNAL_STORAGE; android.permission.AUTHENTICATE_ACCOUNTS' maxSdkVersion='22; android.permission.INTERNET; android.permission.ACCESS_NETWORK_STATE; android.permission.WAKE_LOCK; com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE; android.permission.POST_NOTIFICATIONS; android.permission.READ_EXTERNAL_STORAGE; com.google.android.c2dm.permission.RECEIVE</t>
+  </si>
+  <si>
+    <t>android.hardware.bluetooth implied: requested android.permission.BLUETOOTH permission;  and targetSdkVersion &gt; 4</t>
+  </si>
+  <si>
+    <t>android.permission.READ_EXTERNAL_STORAGE' maxSdkVersion='32; android.permission.READ_MEDIA_VIDEO; android.permission.READ_MEDIA_AUDIO; android.permission.GET_ACCOUNTS; org.wordpress.android.DYNAMIC_RECEIVER_NOT_EXPORTED_PERMISSION; android.permission.FOREGROUND_SERVICE; android.permission.READ_MEDIA_IMAGES; android.permission.VIBRATE; android.permission.RECEIVE_BOOT_COMPLETED; com.android.launcher.permission.UNINSTALL_SHORTCUT; android.permission.INTERNET; android.permission.ACCESS_NETWORK_STATE; android.permission.WAKE_LOCK; com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE; android.permission.WRITE_EXTERNAL_STORAGE' maxSdkVersion='29; android.permission.CAMERA; android.permission.POST_NOTIFICATIONS; android.permission.BLUETOOTH; com.google.android.c2dm.permission.RECEIVE; com.android.launcher.permission.INSTALL_SHORTCUT</t>
+  </si>
+  <si>
+    <t>android.hardware.screen.portrait implied: one or more activities have specified a portrait orientation; android.hardware.microphone implied: requested android.permission.RECORD_AUDIO permission; android.hardware.faketouch implied: default feature for all apps</t>
+  </si>
+  <si>
+    <t>com.whatsapp.sticker.READ; android.permission.INSTALL_SHORTCUT; android.permission.READ_PHONE_NUMBERS; com.whatsapp.permission.BROADCAST; android.permission.ACCESS_COARSE_LOCATION; com.sec.android.provider.badge.permission.WRITE; android.permission.WAKE_LOCK; android.permission.ACCESS_WIFI_STATE; android.permission.POST_NOTIFICATIONS; android.permission.MANAGE_ACCOUNTS; com.google.android.c2dm.permission.RECEIVE; android.permission.READ_MEDIA_AUDIO; android.permission.RECORD_AUDIO; com.facebook.services.identity.FEO2; android.permission.REQUEST_INSTALL_PACKAGES; android.permission.BROADCAST_STICKY; android.permission.READ_SYNC_STATS; android.permission.SCHEDULE_EXACT_ALARM; com.sonymobile.home.permission.PROVIDER_INSERT_BADGE; android.permission.CHANGE_WIFI_STATE; android.permission.INTERNET; android.permission.GET_TASKS; android.permission.USE_FULL_SCREEN_INTENT; com.whatsapp.permission.MAPS_RECEIVE; android.permission.READ_CONTACTS; com.google.android.gms.permission.AD_ID; android.permission.GET_ACCOUNTS; android.permission.READ_SYNC_SETTINGS; com.sonyericsson.home.permission.BROADCAST_BADGE; com.htc.launcher.permission.READ_SETTINGS; android.permission.AUTHENTICATE_ACCOUNTS; android.permission.FOREGROUND_SERVICE; android.permission.READ_PROFILE; android.permission.NFC; android.permission.RECEIVE_BOOT_COMPLETED; android.permission.WRITE_EXTERNAL_STORAGE; com.huawei.android.launcher.permission.WRITE_SETTINGS; android.permission.ACCESS_FINE_LOCATION; com.android.launcher.permission.UNINSTALL_SHORTCUT; android.permission.MANAGE_OWN_CALLS; com.sec.android.provider.badge.permission.READ; android.permission.ACCESS_NETWORK_STATE; android.permission.USE_FINGERPRINT; android.permission.NEARBY_WIFI_DEVICES; android.permission.WRITE_CONTACTS; com.android.launcher.permission.INSTALL_SHORTCUT; com.google.android.providers.gsf.permission.READ_GSERVICES; android.permission.RECEIVE_SMS; android.permission.SEND_SMS; android.permission.READ_MEDIA_VIDEO; android.permission.READ_MEDIA_IMAGES; android.permission.VIBRATE; com.huawei.android.launcher.permission.CHANGE_BADGE; android.permission.WRITE_SYNC_SETTINGS; com.whatsapp.permission.REGISTRATION; com.htc.launcher.permission.UPDATE_SHORTCUT; android.permission.USE_CREDENTIALS; android.permission.USE_BIOMETRIC; android.permission.CHANGE_NETWORK_STATE; com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE; com.huawei.android.launcher.permission.READ_SETTINGS; android.permission.CAMERA; android.permission.MODIFY_AUDIO_SETTINGS; android.permission.READ_EXTERNAL_STORAGE; android.permission.BLUETOOTH; android.permission.READ_PHONE_STATE</t>
+  </si>
+  <si>
+    <t>com.google.android.gms.permission.AD_ID; com.samsung.android.samsungaccount.permission.ACCOUNT_MANAGER; android.permission.GET_ACCOUNTS; android.permission.FOREGROUND_SERVICE_CONNECTED_DEVICE; android.permission.FOREGROUND_SERVICE; android.permission.BLUETOOTH_ADMIN; com.sec.android.app.clockpackage.permission.READ_ALARM; com.spotify.music.permission.C2D_MESSAGE; android.permission.NFC; android.permission.RECEIVE_BOOT_COMPLETED; android.permission.WRITE_EXTERNAL_STORAGE; android.permission.READ_PHONE_STATE' maxSdkVersion='22; android.permission.BLUETOOTH_ADVERTISE; com.spotify.music.permission.SECURED_BROADCAST; android.permission.ACCESS_NETWORK_STATE; com.samsung.WATCH_APP_TYPE.Companion; android.permission.WAKE_LOCK; android.permission.ACCESS_WIFI_STATE; android.permission.POST_NOTIFICATIONS; android.permission.FOREGROUND_SERVICE_MEDIA_PLAYBACK; com.google.android.c2dm.permission.RECEIVE; com.android.launcher.permission.INSTALL_SHORTCUT; android.permission.READ_MEDIA_AUDIO; com.samsung.android.rubin.context.permission.READ_CONTEXT_MANAGER; com.spotify.music.permission.INTERNAL_BROADCAST; com.google.android.apps.meetings.permission.MEET_LIVE_SHARING; android.permission.BLUETOOTH_SCAN; com.spotify.music.DYNAMIC_RECEIVER_NOT_EXPORTED_PERMISSION; android.permission.READ_MEDIA_IMAGES; android.permission.VIBRATE; android.permission.CHANGE_WIFI_MULTICAST_STATE; com.android.vending.BILLING; android.permission.RECORD_AUDIO; android.permission.BROADCAST_STICKY; android.permission.INTERNET; android.permission.USE_CREDENTIALS; com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE; android.permission.MODIFY_AUDIO_SETTINGS; android.permission.READ_EXTERNAL_STORAGE; android.permission.BLUETOOTH; android.permission.BLUETOOTH_CONNECT; com.sony.snei.np.android.account.provider.permission.DUID_READ_PROVIDER; android.permission.FOREGROUND_SERVICE_DATA_SYNC</t>
+  </si>
+  <si>
+    <t>android.permission.READ_CONTACTS; com.google.android.gms.permission.AD_ID; android.permission.GET_ACCOUNTS; android.permission.ACCESS_MEDIA_LOCATION; com.sonyericsson.home.permission.BROADCAST_BADGE; com.htc.launcher.permission.READ_SETTINGS; android.permission.FOREGROUND_SERVICE; android.permission.READ_PHONE_NUMBERS; com.amazon.device.messaging.permission.RECEIVE; android.permission.READ_PROFILE; android.permission.RECEIVE_BOOT_COMPLETED; android.permission.WRITE_EXTERNAL_STORAGE; android.permission.ACCESS_FINE_LOCATION; com.android.launcher.permission.UNINSTALL_SHORTCUT; com.instagram.android.DYNAMIC_RECEIVER_NOT_EXPORTED_PERMISSION; com.instagram.direct.permission.PROTECTED_DEEPLINKING; android.permission.MANAGE_OWN_CALLS; android.permission.ACCESS_NETWORK_STATE; .permission.RECEIVE_ADM_MESSAGE; android.permission.WAKE_LOCK; android.permission.USE_FINGERPRINT; android.permission.POST_NOTIFICATIONS; com.google.android.c2dm.permission.RECEIVE; com.android.launcher.permission.INSTALL_SHORTCUT; android.permission.READ_MEDIA_VIDEO; android.permission.READ_MEDIA_IMAGES; android.permission.VIBRATE; android.permission.REORDER_TASKS; com.huawei.android.launcher.permission.CHANGE_BADGE; com.android.vending.BILLING; android.permission.RECORD_AUDIO; com.facebook.services.identity.FEO2; com.instagram.direct.permission.DIRECT_APP_THREAD_STORE_SERVICE; com.sonymobile.home.permission.PROVIDER_INSERT_BADGE; com.htc.launcher.permission.UPDATE_SHORTCUT; android.permission.INTERNET; android.permission.USE_CREDENTIALS; android.permission.USE_BIOMETRIC; com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE; android.permission.USE_FULL_SCREEN_INTENT; android.permission.CAMERA; android.permission.MODIFY_AUDIO_SETTINGS; com.facebook.katana.provider.ACCESS; android.permission.BLUETOOTH; android.permission.READ_EXTERNAL_STORAGE; android.permission.READ_PHONE_STATE</t>
+  </si>
+  <si>
+    <t>android.permission.READ_CONTACTS; android.permission.FLASHLIGHT; com.vivo.aiengine.permission.READ_AWARE_PROVIDER; android.permission.FOREGROUND_SERVICE; android.permission.SYSTEM_ALERT_WINDOW; com.zhiliao.musically.livewallpaper.permission.wallpaperplugin; com.amazon.device.messaging.permission.RECEIVE; com.zhiliaoapp.musically.permission.READ_ACCOUNT; android.permission.RECEIVE_BOOT_COMPLETED; android.permission.WRITE_EXTERNAL_STORAGE; android.permission.BLUETOOTH' maxSdkVersion='30; com.android.launcher.permission.UNINSTALL_SHORTCUT; android.permission.AUTHENTICATE_ACCOUNTS' maxSdkVersion='22; android.permission.ACCESS_COARSE_LOCATION; com.vivo.aiengine.permission.WRITE_AWARE_PROVIDER; com.sec.android.provider.badge.permission.WRITE; com.sec.android.provider.badge.permission.READ; android.permission.ACCESS_NETWORK_STATE; com.tiktok.preload.permission.IDENTIFY; android.permission.WAKE_LOCK; android.permission.ACCESS_WIFI_STATE; com.zhiliaoapp.musically.permission.RECEIVE_ADM_MESSAGE; com.google.android.c2dm.permission.RECEIVE; com.android.launcher.permission.INSTALL_SHORTCUT; com.android.launcher.permission.READ_SETTINGS; com.samsung.android.mapsagent.permission.READ_APP_INFO; com.orange.update.permission.READ_ATTRIBUTION; android.permission.VIBRATE; android.permission.CHANGE_WIFI_MULTICAST_STATE; com.zhiliaoapp.musically.push.permission.MESSAGE; android.permission.REORDER_TASKS; com.android.vending.BILLING; android.permission.RECORD_AUDIO; android.permission.SCHEDULE_EXACT_ALARM; android.permission.INTERNET; com.zhiliaoapp.musically.permission.WRITE_ACCOUNT; android.permission.CHANGE_NETWORK_STATE; com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE; android.permission.CAMERA; android.permission.SET_WALLPAPER; android.permission.MODIFY_AUDIO_SETTINGS; android.permission.READ_EXTERNAL_STORAGE; android.permission.BLUETOOTH_CONNECT</t>
+  </si>
+  <si>
+    <t>com.google.android.gms.permission.AD_ID; android.permission.READ_CONTACTS; android.permission.GET_ACCOUNTS; android.permission.FOREGROUND_SERVICE; android.permission.RECEIVE_BOOT_COMPLETED; android.permission.NFC; android.permission.ACCESS_FINE_LOCATION; android.permission.ACCESS_COARSE_LOCATION; com.sec.android.provider.badge.permission.WRITE; com.sec.android.provider.badge.permission.READ; android.permission.ACCESS_NETWORK_STATE; android.permission.WAKE_LOCK; android.permission.ACCESS_WIFI_STATE; android.permission.POST_NOTIFICATIONS; com.google.android.c2dm.permission.RECEIVE; com.google.android.providers.gsf.permission.READ_GSERVICES; android.permission.READ_EXTERNAL_STORAGE' maxSdkVersion='32; android.permission.READ_MEDIA_VIDEO; android.permission.READ_MEDIA_IMAGES; android.permission.SCHEDULE_EXACT_ALARM; android.permission.INTERNET; com.pinterest.account.Credentials; com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE; android.permission.WRITE_EXTERNAL_STORAGE' maxSdkVersion='29; android.permission.CAMERA</t>
+  </si>
+  <si>
+    <t>com.google.android.gms.permission.AD_ID; android.permission.READ_CONTACTS; android.permission.CALL_PHONE; android.permission.GET_ACCOUNTS; android.permission.FOREGROUND_SERVICE; com.ubercab.permission.C2D_MESSAGE; android.permission.SYSTEM_ALERT_WINDOW; android.permission.RECEIVE_BOOT_COMPLETED; android.permission.WRITE_EXTERNAL_STORAGE; android.permission.ACCESS_FINE_LOCATION; android.permission.ACCESS_COARSE_LOCATION; android.permission.ACCESS_NETWORK_STATE; android.permission.WAKE_LOCK; android.permission.USE_FINGERPRINT; android.permission.ACCESS_WIFI_STATE; android.permission.BROADCAST_CLOSE_SYSTEM_DIALOGS; android.permission.POST_NOTIFICATIONS; com.google.android.c2dm.permission.RECEIVE; android.permission.MANAGE_ACCOUNTS; com.google.android.providers.gsf.permission.READ_GSERVICES; android.permission.READ_MEDIA_IMAGES; com.ubercab.DYNAMIC_RECEIVER_NOT_EXPORTED_PERMISSION; android.permission.VIBRATE; android.permission.SCHEDULE_EXACT_ALARM; android.permission.INTERNET; android.permission.USE_CREDENTIALS; android.permission.USE_BIOMETRIC; com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE; android.permission.CHANGE_NETWORK_STATE; android.permission.USE_FULL_SCREEN_INTENT; android.permission.CAMERA; android.permission.MODIFY_AUDIO_SETTINGS; android.permission.READ_EXTERNAL_STORAGE; android.permission.BLUETOOTH; android.permission.READ_PHONE_STATE</t>
+  </si>
+  <si>
+    <t>com.google.android.gms.permission.AD_ID; android.permission.GET_ACCOUNTS; android.permission.AUTHENTICATE_ACCOUNTS; android.permission.FOREGROUND_SERVICE; com.amazon.dcp.metrics.permission.METRICS_PERMISSION; com.amazon.identity.permission.CAN_CALL_MAP_INFORMATION_PROVIDER; amazon.permission.COLLECT_METRICS; android.permission.RECEIVE_BOOT_COMPLETED; android.permission.BLUETOOTH' maxSdkVersion='30; com.samsung.permission.USE_MHDR_SERVICE; com.amazon.dcp.sso.permission.CUSTOMER_ATTRIBUTE_SERVICE; android.permission.ACCESS_FINE_LOCATION; android.permission.ACCESS_COARSE_LOCATION; android.permission.ACCESS_NETWORK_STATE; android.permission.WAKE_LOCK; android.permission.ACCESS_WIFI_STATE; com.amazon.device.environment.permission.SWITCH_STAGE; com.amazon.appmanager.preload.permission.READ_PRELOAD_DEVICE_INFO_PROVIDER; android.permission.VIBRATE' maxSdkVersion='18; android.permission.MANAGE_ACCOUNTS; com.google.android.c2dm.permission.RECEIVE; com.amazon.dcp.sso.permission.USE_DEVICE_CREDENTIALS; com.amazon.identity.permission.GENERIC_IPC; com.amazon.identity.auth.device.perm.AUTH_SDK; com.amazon.dcp.config.permission.DYN_CONFIG_VALUES_UPDATED; android.permission.CHANGE_WIFI_MULTICAST_STATE; com.amazon.dcp.sso.permission.MANAGE_COR_PFM; com.android.vending.BILLING; com.amazon.avod.SDK_ACCESS; com.amazon.CONTENT_PROVIDER_ACCESS; android.permission.SCHEDULE_EXACT_ALARM; android.permission.INTERNET; android.permission.USE_CREDENTIALS; android.permission.CHANGE_NETWORK_STATE; com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE; android.permission.WRITE_EXTERNAL_STORAGE' maxSdkVersion='28; com.amazon.dcp.sso.permission.AmazonAccountPropertyService.property.changed; android.permission.READ_EXTERNAL_STORAGE; com.amazon.identity.permission.CALL_AMAZON_DEVICE_INFORMATION_PROVIDER; android.permission.READ_PHONE_STATE; com.amazon.dcp.sso.permission.account.changed</t>
+  </si>
+  <si>
+    <t>android.permission.READ_CONTACTS; com.google.android.gms.permission.AD_ID; android.permission.FOREGROUND_SERVICE; android.permission.NFC; android.permission.RECEIVE_BOOT_COMPLETED; android.permission.WRITE_EXTERNAL_STORAGE; android.permission.ACCESS_FINE_LOCATION; com.felicanetworks.mfc.permission.MFC_ACCESS; android.permission.ACCESS_COARSE_LOCATION; android.permission.ACCESS_NETWORK_STATE; android.permission.WAKE_LOCK; android.permission.ACCESS_WIFI_STATE; android.permission.USE_FINGERPRINT; com.google.android.c2dm.permission.RECEIVE; com.google.android.providers.gsf.permission.READ_GSERVICES; android.permission.GET_ACCOUNTS' maxSdkVersion='22; android.permission.GET_PACKAGE_SIZE; com.google.android.apps.walletnfcrel.permission.C2D_MESSAGE; android.permission.VIBRATE; android.permission.INTERNET; android.permission.USE_BIOMETRIC; com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE; android.permission.CAMERA; android.permission.READ_EXTERNAL_STORAGE; android.permission.READ_PHONE_STATE</t>
+  </si>
+  <si>
+    <t>android.hardware.screen.portrait implied: one or more activities have specified a portrait orientation; android.hardware.microphone implied: requested android.permission.RECORD_AUDIO permission; android.hardware.wifi implied: requested android.permission.ACCESS_WIFI_STATE permission; android.hardware.faketouch implied: default feature for all apps</t>
+  </si>
+  <si>
+    <t>com.hihonor.android.launcher.permission.CHANGE_BADGE; com.google.android.gms.permission.AD_ID; com.sonyericsson.home.permission.BROADCAST_BADGE; com.htc.launcher.permission.READ_SETTINGS; android.permission.FOREGROUND_SERVICE; android.permission.GET_PACKAGE_SIZE' maxSdkVersion='25; android.permission.RECEIVE_BOOT_COMPLETED; android.permission.WRITE_EXTERNAL_STORAGE; com.huawei.android.launcher.permission.WRITE_SETTINGS; com.android.launcher.permission.UNINSTALL_SHORTCUT; me.everything.badger.permission.BADGE_COUNT_READ; com.sec.android.provider.badge.permission.WRITE; com.sec.android.provider.badge.permission.READ; android.permission.ACCESS_NETWORK_STATE; com.vivo.notification.permission.BADGE_ICON; android.permission.WAKE_LOCK; com.anddoes.launcher.permission.UPDATE_COUNT; android.permission.ACCESS_WIFI_STATE; android.permission.HIGH_SAMPLING_RATE_SENSORS; com.oppo.launcher.permission.WRITE_SETTINGS; com.google.android.c2dm.permission.RECEIVE; com.android.launcher.permission.INSTALL_SHORTCUT; com.android.launcher.permission.READ_SETTINGS; android.permission.READ_APP_BADGE; android.permission.VIBRATE; com.huawei.android.launcher.permission.CHANGE_BADGE; com.android.vending.BILLING; android.permission.RECORD_AUDIO; com.majeur.launcher.permission.UPDATE_BADGE; com.sonymobile.home.permission.PROVIDER_INSERT_BADGE; com.htc.launcher.permission.UPDATE_SHORTCUT; android.permission.INTERNET; com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE; com.huawei.android.launcher.permission.READ_SETTINGS; android.permission.CAMERA; android.permission.READ_EXTERNAL_STORAGE; me.everything.badger.permission.BADGE_COUNT_WRITE; android.permission.UPDATE_APP_BADGE; com.oppo.launcher.permission.READ_SETTINGS; com.android.launcher.permission.WRITE_SETTINGS</t>
+  </si>
+  <si>
+    <t>android.permission.DOWNLOAD_WITHOUT_NOTIFICATION; com.samsung.cmh.data.READ; android.permission.WRITE_CALENDAR; com.sec.android.app.clockpackage.permission.READ_ALARM; com.vlingo.midas.permission.BACKUP_RESTORE; com.sec.android.app.sbrowser.permission.BACKUP_RESTORE; com.sec.mms.permission.BACKUP_RESTORE; android.permission.OVERRIDE_WIFI_CONFIG; android.permission.WAKE_LOCK; com.samsung.inputmethod.permission.BACKUP_RESTORE; com.samsung.android.app.provider.episodes.permission.READ_EPISODES_DB; android.permission.PACKAGE_USAGE_STATS; android.permission.GET_PACKAGE_SIZE; com.sec.android.kies.vzwlocation.BROADCAST_DETECT; android.permission.WRITE_OWNER_DATA; android.permission.CHANGE_WIFI_STATE; com.sec.android.phone.permission.READ_CALL_SETTINGS; android.permission.INTERNET; android.permission.GET_TASKS; com.sec.android.app.clockpackage.permission.READ_TIMER; com.sec.android.app.clockpackage.permission.READ_WCCONTENT; com.samsung.android.app.reminder.permission.READ; android.permission.READ_OWNER_DATA; android.permission.NETWORK_STACK; com.samsung.android.scloud.sync.permission.WRITE; android.permission.READ_CONTACTS; android.permission.READ_LOGS; android.permission.READ_SMS; android.permission.READ_SYNC_SETTINGS; android.permission.UPDATE_APP_OPS_STATS; com.samsung.android.internal.intelligence.useranalysis.permission.WRITE_PLACE; android.permission.BLUETOOTH_ADMIN; com.sec.android.easyMover.permission.RUN_AGENT; com.samsung.android.app.notes.sync.STATE_WRITE; com.samsung.android.app.cocktailbarservice.permission.ACCESS_PANEL; android.permission.READ_PROFILE; com.sec.android.app.clockpackage.permission.BACKUP_RESTORE_ALARM; android.permission.RECEIVE_BOOT_COMPLETED; com.samsung.android.memo.BNR; android.permission.CHANGE_COMPONENT_ENABLED_STATE; com.sec.android.app.fm.BROADCAST_DETECT; android.permission.PEERS_MAC_ADDRESS; android.permission.TETHER_PRIVILEGED; com.sec.android.app.browser.permission.IMPORT_BOOKMARK; com.samsung.android.app.omcagent.permission.READ_PROVIDER; com.sec.permission.WIFI_BACKUP; android.permission.WRITE_SMS; com.android.launcher.permission.READ_SETTINGS; com.samsung.android.app.notes.READ; android.permission.VIBRATE; com.sec.android.permission.KIES_BNR; android.permission.REORDER_TASKS; com.samsung.android.memo.READ; android.permission.READ_CALL_LOG; android.permission.NETWORK_SETTINGS; com.google.android.finsky.permission.INSTANT_APP_STATE; com.samsung.android.scloud.sync.permission.READ; android.permission.BLUETOOTH; com.samsung.voiceserviceplatform.permission.BACKUP_RESTORE; android.permission.READ_CALENDAR; com.sec.android.phone.permission.WRITE_CALL_SETTINGS; android.permission.INSTALL_PACKAGES; android.permission.WRITE_MEDIA_STORAGE; com.samsung.android.app.notes.sync.STATE_READ; com.android.browser.permission.READ_HISTORY_BOOKMARKS; android.permission.WRITE_TASKS; com.sec.android.app.music.permission.WRITE_SETTINGS; android.permission.REBOOT; android.permission.CONNECTIVITY_INTERNAL; android.permission.ACCESS_COARSE_LOCATION; com.sec.permission.BACKUP_RESTORE_HOMESCREEN; android.permission.WRITE_PROFILE; android.permission.WRITE_SECURE_SETTINGS; android.permission.ACCESS_WIFI_STATE; com.sec.android.inputmethod.permission.BACKUP_RESTORE; android.permission.READ_TASKS; com.android.vending.setup.PLAY_SETUP_SERVICE; android.permission.CLEAR_APP_CACHE; com.wssnps.permission.COM_WSSNPS; com.samsung.permission.READ_SM_DATA; com.sec.android.widgetapp.q1_penmemo.permission.WRITE; android.permission.RECORD_AUDIO; com.sec.android.app.safetyassurance.permission.PRIVATE; com.sec.android.provider.logsprovider.permission.READ_LOGS; com.sec.android.app.clockpackage.permission.BACKUP_RESTORE_WORLDCLOCK; com.sec.spp.permission.TOKEN_9d7d0e108b0956dbad83c838c1dc3cdd422696c70a07d965193a2908197b48d72eaad4fa3f4a5cb7a55ea5508008cd3c7c7ef96207215606cd858405b9939c4e645f3ff51dc98f0b1ebcb87c0a1fac1432cb0f6ebcc2e4f7cfe72b7af75a0e836b9a9bec9dd54896807da97b3d66f93feaa7829167a41711983541b34e240c0e; com.infraware.provider.SNoteProvider.permission.READ; com.sec.android.widgetapp.q1_penmemo.permission.READ; android.permission.COM_WSSNPS; android.permission.LOCAL_MAC_ADDRESS; com.sec.android.permission.WRITE_MEMO; com.samsung.android.app.shareaccessibilitysettings.permission.READ_WRITE; android.permission.GET_ACCOUNTS; com.samsung.android.providers.context.permission.WRITE_USE_APP_FEATURE_SURVEY; android.permission.SYSTEM_ALERT_WINDOW; com.sec.android.app.calendar.permission.WRITE_CALENDAR_SETTINGS; android.permission.WRITE_EXTERNAL_STORAGE; com.infraware.provider.SNoteProvider.permission.WRITE; com.sec.permission.OTG_CHARGE_BLOCK; android.permission.ACCESS_NETWORK_STATE; android.permission.WRITE_CONTACTS; com.sec.android.permission.READ_MEMO; com.sec.android.kies.calllog.BROADCAST_DETECT; com.sec.android.app.contact.permission.CONTACT_SETTINGS; android.permission.MANAGE_NETWORK_POLICY; android.permission.BACKUP; com.samsung.android.permission.SSRM_NOTIFICATION_PERMISSION; com.sec.android.email.service.BROADCAST_DETECT; com.samsung.android.telephony.provider.permission.ACCESS_RESTORE_STATE; com.samsung.android.launcher.permission.READ_SETTINGS; com.samsung.kidshome.provider.SETUPWIZARD_READ; android.permission.CHANGE_NETWORK_STATE; android.permission.MODIFY_AUDIO_SETTINGS; android.permission.READ_EXTERNAL_STORAGE; android.permission.WRITE_SETTINGS; android.permission.READ_PHONE_STATE</t>
+  </si>
+  <si>
+    <t>android.permission.READ_CONTACTS; com.google.android.gms.permission.AD_ID; android.permission.GET_ACCOUNTS; com.sonyericsson.home.permission.BROADCAST_BADGE; com.htc.launcher.permission.READ_SETTINGS; android.permission.FOREGROUND_SERVICE; android.permission.RECEIVE_BOOT_COMPLETED; com.huawei.android.launcher.permission.WRITE_SETTINGS; me.everything.badger.permission.BADGE_COUNT_READ; com.sec.android.provider.badge.permission.WRITE; com.sec.android.provider.badge.permission.READ; android.permission.ACCESS_NETWORK_STATE; android.permission.WAKE_LOCK; com.anddoes.launcher.permission.UPDATE_COUNT; android.permission.POST_NOTIFICATIONS; com.google.android.c2dm.permission.RECEIVE; com.oppo.launcher.permission.WRITE_SETTINGS; android.permission.READ_EXTERNAL_STORAGE' maxSdkVersion='32; android.permission.READ_APP_BADGE; android.permission.READ_MEDIA_IMAGES; android.permission.VIBRATE; com.huawei.android.launcher.permission.CHANGE_BADGE; com.android.vending.BILLING; android.permission.RECORD_AUDIO; com.duolingo.DYNAMIC_RECEIVER_NOT_EXPORTED_PERMISSION; com.majeur.launcher.permission.UPDATE_BADGE; com.sonymobile.home.permission.PROVIDER_INSERT_BADGE; com.htc.launcher.permission.UPDATE_SHORTCUT; android.permission.INTERNET; com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE; com.huawei.android.launcher.permission.READ_SETTINGS; android.permission.WRITE_EXTERNAL_STORAGE' maxSdkVersion='28; me.everything.badger.permission.BADGE_COUNT_WRITE; com.oppo.launcher.permission.READ_SETTINGS</t>
+  </si>
+  <si>
+    <t>com.google.android.gms.permission.AD_ID; android.permission.GET_ACCOUNTS; android.permission.FOREGROUND_SERVICE; com.amazon.dcp.metrics.permission.METRICS_PERMISSION; android.permission.EXPAND_STATUS_BAR; amazon.permission.COLLECT_METRICS; com.amazon.kindle.cms.CMS_ACCESS; android.permission.RECEIVE_BOOT_COMPLETED; android.permission.BLUETOOTH' maxSdkVersion='30; android.permission.READ_PHONE_STATE' maxSdkVersion='22; com.amazon.dcp.sso.permission.CUSTOMER_ATTRIBUTE_SERVICE; com.audible.application.externalmediaplayer.permission.WAKE_UP; android.permission.ACCESS_NETWORK_STATE; android.permission.WAKE_LOCK; android.permission.ACCESS_WIFI_STATE; com.amazon.appmanager.preload.permission.READ_PRELOAD_DEVICE_INFO_PROVIDER; android.permission.POST_NOTIFICATIONS; com.amazon.alexa.handsfree.protocols.permission.DATA_SYNC; com.google.android.c2dm.permission.RECEIVE; com.amazon.dcp.sso.permission.USE_DEVICE_CREDENTIALS; com.amazon.identity.auth.device.perm.AUTH_SDK; com.amazon.dcp.config.permission.DYN_CONFIG_VALUES_UPDATED; android.permission.CHANGE_WIFI_MULTICAST_STATE; com.amazon.dcp.sso.permission.MANAGE_COR_PFM; com.android.vending.BILLING; android.permission.RECORD_AUDIO; com.audible.application.permission.C2D_MESSAGE; android.permission.CHANGE_WIFI_STATE; android.permission.INTERNET; com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE; com.amazon.alexa.externalmediaplayer.permission.WAKE_UP; android.permission.WRITE_EXTERNAL_STORAGE' maxSdkVersion='29; android.permission.MODIFY_AUDIO_SETTINGS; android.permission.BLUETOOTH_CONNECT; com.amazon.identity.permission.CALL_AMAZON_DEVICE_INFORMATION_PROVIDER; android.permission.READ_EXTERNAL_STORAGE; com.amazon.dcp.sso.permission.AmazonAccountPropertyService.property.changed; com.amazon.dcp.sso.permission.account.changed</t>
+  </si>
+  <si>
+    <t>Canva: Design;  Photo &amp; Video</t>
+  </si>
+  <si>
+    <t>android.hardware.screen.portrait; android.hardware.wifi implied: requested android.permission.ACCESS_WIFI_STATE permission; android.hardware.faketouch implied: default feature for all apps</t>
+  </si>
+  <si>
+    <t>com.google.android.gms.permission.AD_ID; android.permission.FOREGROUND_SERVICE; android.permission.VIBRATE; com.android.vending.BILLING; android.permission.RECEIVE_BOOT_COMPLETED; android.permission.WRITE_EXTERNAL_STORAGE; android.permission.INTERNET; android.permission.ACCESS_NETWORK_STATE; com.huawei.appmarket.service.commondata.permission.GET_COMMON_DATA; android.permission.WAKE_LOCK; com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE; android.permission.ACCESS_WIFI_STATE; android.permission.CAMERA; android.permission.READ_EXTERNAL_STORAGE; android.permission.POST_NOTIFICATIONS; com.google.android.c2dm.permission.RECEIVE</t>
+  </si>
+  <si>
+    <t>android.permission.BLUETOOTH_PRIVILEGED; android.permission.DOWNLOAD_WITHOUT_NOTIFICATION; android.permission.BLUETOOTH' maxSdkVersion='30; android.permission.ACCESS_COARSE_LOCATION; com.sec.android.provider.badge.permission.WRITE; com.anddoes.launcher.permission.UPDATE_COUNT; android.permission.WAKE_LOCK; android.permission.ACCESS_WIFI_STATE; android.permission.POST_NOTIFICATIONS; android.permission.MANAGE_ACCOUNTS; com.oppo.launcher.permission.WRITE_SETTINGS; com.google.android.c2dm.permission.RECEIVE; android.permission.DISABLE_KEYGUARD; android.permission.BLUETOOTH_SCAN; android.permission.READ_APP_BADGE; android.permission.ACCESS_BACKGROUND_LOCATION; android.permission.RECORD_AUDIO; android.permission.REQUEST_INSTALL_PACKAGES; com.majeur.launcher.permission.UPDATE_BADGE; android.permission.SCHEDULE_EXACT_ALARM; com.sonymobile.home.permission.PROVIDER_INSERT_BADGE; android.permission.INTERNET; android.permission.USE_FULL_SCREEN_INTENT; android.permission.BLUETOOTH_CONNECT; me.everything.badger.permission.BADGE_COUNT_WRITE; com.oppo.launcher.permission.READ_SETTINGS; android.permission.ACCESS_DOWNLOAD_MANAGER; android.permission.BLUETOOTH_ADMIN' maxSdkVersion='30; android.permission.READ_CONTACTS; android.permission.GET_ACCOUNTS; android.permission.CALL_PHONE; com.sonyericsson.home.permission.BROADCAST_BADGE; com.htc.launcher.permission.READ_SETTINGS; android.permission.FOREGROUND_SERVICE; android.permission.AUTHENTICATE_ACCOUNTS; android.permission.EXPAND_STATUS_BAR; android.permission.SYSTEM_ALERT_WINDOW; android.permission.RECEIVE_BOOT_COMPLETED; android.permission.NFC; android.permission.WRITE_EXTERNAL_STORAGE; com.huawei.android.launcher.permission.WRITE_SETTINGS; android.permission.ACCESS_FINE_LOCATION; me.everything.badger.permission.BADGE_COUNT_READ; baidu.push.permission.WRITE_PUSHINFOPROVIDER.com.microsoft.teams; android.permission.MANAGE_OWN_CALLS; com.sec.android.provider.badge.permission.READ; android.permission.ACCESS_NETWORK_STATE; android.permission.REQUEST_IGNORE_BATTERY_OPTIMIZATIONS; android.permission.USE_FINGERPRINT; android.permission.WRITE_CONTACTS; com.microsoft.teams.permission.MIPUSH_RECEIVE; android.permission.VIBRATE; com.huawei.android.launcher.permission.CHANGE_BADGE; android.permission.RECORD_VIDEO; com.htc.launcher.permission.UPDATE_SHORTCUT; android.permission.USE_CREDENTIALS; android.permission.USE_BIOMETRIC; android.permission.CHANGE_NETWORK_STATE; com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE; com.huawei.android.launcher.permission.READ_SETTINGS; android.permission.CAMERA; android.permission.MODIFY_AUDIO_SETTINGS; android.permissAGE; android.permission.READ_EXTERNAL_STORAGE; android.permission.WRITE_SETTINGS; android.permission.READ_PHONE_STATE</t>
+  </si>
+  <si>
+    <t>com.google.android.gms.permission.AD_ID; android.permission.INTERNET; com.facebook.everythingtogether.contentprovider.GET_DEFERRED_DEEPLINK; android.permission.FOREGROUND_SERVICE; android.permission.ACCESS_NETWORK_STATE; android.permission.WAKE_LOCK; com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE; android.permission.ACCESS_WIFI_STATE; android.permission.POST_NOTIFICATIONS; android.permission.RECEIVE_BOOT_COMPLETED; com.google.android.c2dm.permission.RECEIVE</t>
+  </si>
+  <si>
+    <t>com.google.android.gms.permission.AD_ID; com.bumble.app.DYNAMIC_RECEIVER_NOT_EXPORTED_PERMISSION; android.permission.GET_ACCOUNTS; com.sonyericsson.home.permission.BROADCAST_BADGE; com.htc.launcher.permission.READ_SETTINGS; android.permission.FOREGROUND_SERVICE; android.permission.READ_PHONE_NUMBERS; android.permission.RECEIVE_BOOT_COMPLETED; com.huawei.android.launcher.permission.WRITE_SETTINGS; android.permission.ACCESS_FINE_LOCATION; android.permission.ACCESS_COARSE_LOCATION; com.sec.android.provider.badge.permission.WRITE; com.sec.android.provider.badge.permission.READ; android.permission.ACCESS_NETWORK_STATE; android.permission.WAKE_LOCK; com.anddoes.launcher.permission.UPDATE_COUNT; android.permission.ACCESS_WIFI_STATE; android.permission.USE_FINGERPRINT; android.permission.POST_NOTIFICATIONS; com.oppo.launcher.permission.WRITE_SETTINGS; com.google.android.c2dm.permission.RECEIVE; android.permission.DISABLE_KEYGUARD; android.permission.READ_APP_BADGE; android.permission.VIBRATE; com.huawei.android.launcher.permission.CHANGE_BADGE; com.android.vending.BILLING; android.permission.RECORD_AUDIO; com.majeur.launcher.permission.UPDATE_BADGE; com.sonymobile.home.permission.PROVIDER_INSERT_BADGE; com.htc.launcher.permission.UPDATE_SHORTCUT; android.permission.CHANGE_WIFI_STATE; android.permission.INTERNET; android.permission.USE_BIOMETRIC; android.permission.CHANGE_NETWORK_STATE; com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE; android.permission.USE_FULL_SCREEN_INTENT; com.badoo.permission.SignaturePrivileged; com.huawei.android.launcher.permission.READ_SETTINGS; android.permission.CAMERA; android.permission.WRITE_EXTERNAL_STORAGE' maxSdkVersion='28; android.permission.MODIFY_AUDIO_SETTINGS; android.permission.READ_EXTERNAL_STORAGE; android.permission.BLUETOOTH; android.permission.BLUETOOTH_CONNECT; android.permission.READ_PHONE_STATE; com.oppo.launcher.permission.READ_SETTINGS</t>
+  </si>
+  <si>
+    <t>android.permission.READ_CONTACTS; com.google.android.gms.permission.AD_ID; com.sonyericsson.home.permission.BROADCAST_BADGE; com.htc.launcher.permission.READ_SETTINGS; android.permission.FOREGROUND_SERVICE; android.permission.SYSTEM_ALERT_WINDOW; android.permission.READ_PROFILE; android.permission.RECEIVE_BOOT_COMPLETED; android.permission.WRITE_EXTERNAL_STORAGE; com.huawei.android.launcher.permission.WRITE_SETTINGS; android.permission.ACCESS_FINE_LOCATION; me.everything.badger.permission.BADGE_COUNT_READ; android.permission.ACCESS_COARSE_LOCATION; com.sec.android.provider.badge.permission.WRITE; com.sec.android.provider.badge.permission.READ; android.permission.ACCESS_NETWORK_STATE; android.permission.WAKE_LOCK; com.anddoes.launcher.permission.UPDATE_COUNT; android.permission.ACCESS_WIFI_STATE; android.permission.POST_NOTIFICATIONS; com.google.android.c2dm.permission.RECEIVE; com.oppo.launcher.permission.WRITE_SETTINGS; oppo.permission.OPPO_COMPONENT_SAFE; android.permission.READ_APP_BADGE; android.permission.ACCESS_BACKGROUND_LOCATION; android.permission.VIBRATE; com.huawei.android.launcher.permission.CHANGE_BADGE; com.android.vending.BILLING; com.majeur.launcher.permission.UPDATE_BADGE; android.permission.SCHEDULE_EXACT_ALARM; com.sonymobile.home.permission.PROVIDER_INSERT_BADGE; com.htc.launcher.permission.UPDATE_SHORTCUT; android.permission.INTERNET; com.huawei.permission.external_app_settings.USE_COMPONENT; com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE; android.permission.ACTIVITY_RECOGNITION; com.huawei.android.launcher.permission.READ_SETTINGS; android.permission.CAMERA; android.permission.READ_EXTERNAL_STORAGE; me.everything.badger.permission.BADGE_COUNT_WRITE; com.google.android.gms.permission.ACTIVITY_RECOGNITION; com.oppo.launcher.permission.READ_SETTINGS</t>
+  </si>
+  <si>
+    <t>android.permission.READ_MEDIA_VIDEO; com.google.android.gms.permission.AD_ID; android.permission.READ_MEDIA_IMAGES; android.permission.BLUETOOTH_ADMIN; android.permission.VIBRATE; android.permission.NFC; android.permission.WRITE_EXTERNAL_STORAGE; android.permission.ACCESS_COARSE_LOCATION; android.permission.INTERNET; android.permission.ACCESS_NETWORK_STATE; android.permission.WAKE_LOCK; android.permission.ACCESS_WIFI_STATE; android.permission.CAMERA; android.permission.READ_EXTERNAL_STORAGE; android.permission.BLUETOOTH</t>
+  </si>
+  <si>
+    <t>com.google.android.gms.permission.AD_ID; android.permission.GET_ACCOUNTS; android.permission.DOWNLOAD_WITHOUT_NOTIFICATION; android.permission.FOREGROUND_SERVICE; android.permission.SYSTEM_ALERT_WINDOW; android.permission.RECEIVE_BOOT_COMPLETED; android.permission.WRITE_EXTERNAL_STORAGE; android.permission.ACCESS_FINE_LOCATION; android.permission.ACCESS_COARSE_LOCATION; android.permission.ACCESS_NETWORK_STATE; android.permission.WAKE_LOCK; android.permission.ACCESS_WIFI_STATE; com.google.android.c2dm.permission.RECEIVE; android.permission.ACCESS_BACKGROUND_LOCATION; android.permission.CHANGE_WIFI_MULTICAST_STATE; android.permission.VIBRATE; com.android.vending.BILLING; android.permission.RECORD_AUDIO; com.app.appname.permission.C2D_MESSAGE; android.permission.CHANGE_WIFI_STATE; android.permission.INTERNET; com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE; android.permission.CAMERA; android.permission.READ_EXTERNAL_STORAGE; android.permission.READ_PHONE_STATE</t>
+  </si>
+  <si>
+    <t>Expedia: Hotels;  Flights &amp; Car</t>
+  </si>
+  <si>
+    <t>com.google.android.gms.permission.AD_ID; android.permission.READ_SYNC_SETTINGS; android.permission.GET_ACCOUNTS; android.permission.AUTHENTICATE_ACCOUNTS; android.permission.FOREGROUND_SERVICE; android.permission.RECEIVE_BOOT_COMPLETED; android.permission.WRITE_EXTERNAL_STORAGE; android.permission.WRITE_SYNC_SETTINGS; android.permission.READ_SYNC_STATS; android.permission.ACCESS_FINE_LOCATION; android.permission.ACCESS_COARSE_LOCATION; android.permission.INTERNET; android.permission.USE_CREDENTIALS; android.permission.ACCESS_NETWORK_STATE; android.permission.WAKE_LOCK; com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE; android.permission.ACCESS_WIFI_STATE; android.permission.READ_EXTERNAL_STORAGE; android.permission.MANAGE_ACCOUNTS; com.google.android.c2dm.permission.RECEIVE; com.google.android.providers.gsf.permission.READ_GSERVICES</t>
+  </si>
+  <si>
+    <t>com.google.android.gms.permission.AD_ID; android.permission.VIBRATE; android.permission.RECEIVE_BOOT_COMPLETED; android.permission.RECORD_AUDIO; android.permission.WRITE_EXTERNAL_STORAGE; com.adjust.preinstall.READ_PERMISSION; android.permission.INTERNET; android.permission.ACCESS_NETWORK_STATE; android.permission.WAKE_LOCK; com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE; android.permission.ACCESS_WIFI_STATE; android.permission.CAMERA; com.einnovation.temu.remote_config; android.permission.READ_EXTERNAL_STORAGE; android.permission.POST_NOTIFICATIONS; com.google.android.c2dm.permission.RECEIVE</t>
+  </si>
+  <si>
+    <t>android.permission.READ_EXTERNAL_STORAGE' maxSdkVersion='32; android.permission.READ_MEDIA_VIDEO; com.google.android.gms.permission.AD_ID; android.permission.WRITE_EXTERNAL_STORAGE' maxSdkVersion='32; android.permission.ACCESS_BACKGROUND_LOCATION; android.permission.FOREGROUND_SERVICE; android.permission.READ_MEDIA_IMAGES; android.permission.REORDER_TASKS; com.android.vending.BILLING; android.permission.RECEIVE_BOOT_COMPLETED; android.permission.ACCESS_FINE_LOCATION; android.permission.SCHEDULE_EXACT_ALARM; android.permission.ACCESS_COARSE_LOCATION; android.permission.CHANGE_WIFI_STATE; android.permission.INTERNET; android.permission.USE_CREDENTIALS; android.permission.ACCESS_NETWORK_STATE; android.permission.WAKE_LOCK; android.permission.ACCESS_WIFI_STATE; android.permission.POST_NOTIFICATIONS; android.permission.MANAGE_ACCOUNTS; com.google.android.c2dm.permission.RECEIVE; com.google.android.gms.permission.ACTIVITY_RECOGNITION</t>
+  </si>
+  <si>
+    <t>android.hardware.camera; android.hardware.screen.portrait implied: one or more activities have specified a portrait orientation; android.hardware.wifi implied: requested android.permission.ACCESS_WIFI_STATE permission; android.hardware.faketouch implied: default feature for all apps</t>
+  </si>
+  <si>
+    <t>com.google.android.gms.permission.AD_ID; android.permission.ACCESS_MEDIA_LOCATION; android.permission.FOREGROUND_SERVICE; com.android.vending.BILLING; android.permission.RECEIVE_BOOT_COMPLETED; android.permission.WRITE_EXTERNAL_STORAGE; android.permission.INTERNET; cn.danatech.xingseus.permission.C2D_MESSAGE; android.permission.ACCESS_NETWORK_STATE; android.permission.WAKE_LOCK; com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE; android.permission.ACCESS_WIFI_STATE; android.permission.CAMERA; android.permission.READ_EXTERNAL_STORAGE; com.google.android.c2dm.permission.RECEIVE</t>
+  </si>
+  <si>
+    <t>Ticketmaster－Buy;  Sell Tickets</t>
+  </si>
+  <si>
+    <t>android.permission.READ_CONTACTS; com.google.android.gms.permission.AD_ID; android.permission.CALL_PHONE; android.permission.WRITE_CALENDAR; android.permission.FOREGROUND_SERVICE; android.permission.VIBRATE; android.permission.READ_CALENDAR; android.permission.REORDER_TASKS; android.permission.RECEIVE_BOOT_COMPLETED; android.permission.WRITE_EXTERNAL_STORAGE; android.permission.ACCESS_FINE_LOCATION; android.permission.ACCESS_COARSE_LOCATION; android.permission.INTERNET; android.permission.ACCESS_NETWORK_STATE; android.permission.WAKE_LOCK; com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE; android.permission.ACCESS_WIFI_STATE; android.permission.CAMERA; android.permission.READ_EXTERNAL_STORAGE; android.permission.READ_PHONE_STATE; com.google.android.c2dm.permission.RECEIVE; com.google.android.providers.gsf.permission.READ_GSERVICES</t>
+  </si>
+  <si>
+    <t>android.hardware.screen.portrait implied: one or more activities have specified a portrait orientation; android.hardware.location implied: requested android.permission.ACCESS_COARSE_LOCATION permission; android.hardware.wifi implied: requested android.permission.ACCESS_WIFI_STATE permission; android.hardware.faketouch implied: default feature for all apps</t>
+  </si>
+  <si>
+    <t>android.permission.READ_PHONE_NUMBERS; android.permission.VIBRATE; android.permission.STORAGE; android.permission.RECEIVE_BOOT_COMPLETED; android.permission.WRITE_EXTERNAL_STORAGE; android.permission.READ_PHONE_STATE' maxSdkVersion='29; android.permission.SCHEDULE_EXACT_ALARM; android.permission.ACCESS_COARSE_LOCATION; android.permission.INTERNET; android.permission.USE_BIOMETRIC; android.permission.ACCESS_NETWORK_STATE; android.permission.WAKE_LOCK; com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE; android.permission.ACCESS_WIFI_STATE; android.permission.USE_FINGERPRINT; android.permission.USE_CREDENTIALS' maxSdkVersion='22; android.permission.CAMERA; android.permission.POST_NOTIFICATIONS; android.permission.READ_EXTERNAL_STORAGE; com.google.android.c2dm.permission.RECEIVE</t>
+  </si>
+  <si>
+    <t>Lensa: Avatar Maker;  Editor</t>
+  </si>
+  <si>
+    <t>android.permission.READ_EXTERNAL_STORAGE' maxSdkVersion='32; com.google.android.gms.permission.AD_ID; android.permission.FOREGROUND_SERVICE; android.permission.READ_MEDIA_IMAGES; android.permission.VIBRATE; com.android.vending.BILLING; android.permission.RECEIVE_BOOT_COMPLETED; android.permission.BILLING; android.permission.INTERNET; android.permission.ACCESS_NETWORK_STATE; android.permission.WAKE_LOCK; com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE; android.permission.ACCESS_WIFI_STATE; android.permission.WRITE_EXTERNAL_STORAGE' maxSdkVersion='28; android.permission.POST_NOTIFICATIONS; com.google.android.c2dm.permission.RECEIVE</t>
+  </si>
+  <si>
+    <t>com.google.android.gms.permission.AD_ID; com.mcdonalds.superapp.permission.MAPS_RECEIVE; android.permission.FOREGROUND_SERVICE; android.permission.VIBRATE; android.permission.RECEIVE_BOOT_COMPLETED; android.permission.WRITE_EXTERNAL_STORAGE; com.android.alarm.permission.SET_ALARM; android.permission.ACCESS_FINE_LOCATION; android.permission.CHANGE_WIFI_STATE; android.permission.ACCESS_COARSE_LOCATION; android.permission.INTERNET; android.permission.USE_CREDENTIALS; android.permission.ACCESS_NETWORK_STATE; android.permission.GET_TASKS; android.permission.WAKE_LOCK; com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE; android.permission.ACCESS_WIFI_STATE; android.permission.CAMERA; android.permission.READ_EXTERNAL_STORAGE; com.google.android.c2dm.permission.RECEIVE; android.permission.READ_PHONE_STATE; com.google.android.providers.gsf.permission.READ_GSERVICES</t>
+  </si>
+  <si>
+    <t>android.permission.READ_CONTACTS; com.google.android.gms.permission.AD_ID; com.sonyericsson.home.permission.BROADCAST_BADGE; com.htc.launcher.permission.READ_SETTINGS; com.feverup.fever.BRANCH_SHARE_PERMISSION; android.permission.FOREGROUND_SERVICE; android.permission.RECEIVE_BOOT_COMPLETED; android.permission.WRITE_EXTERNAL_STORAGE; com.feverup.fever.DYNAMIC_RECEIVER_NOT_EXPORTED_PERMISSION; com.huawei.android.launcher.permission.WRITE_SETTINGS; android.permission.ACCESS_FINE_LOCATION; com.feverup.fever.permission.C2D_MESSAGE; me.everything.badger.permission.BADGE_COUNT_READ; android.permission.ACCESS_COARSE_LOCATION; com.sec.android.provider.badge.permission.WRITE; com.sec.android.provider.badge.permission.READ; android.permission.ACCESS_NETWORK_STATE; android.permission.WAKE_LOCK; com.anddoes.launcher.permission.UPDATE_COUNT; android.permission.POST_NOTIFICATIONS; com.google.android.c2dm.permission.RECEIVE; com.oppo.launcher.permission.WRITE_SETTINGS; android.permission.READ_EXTERNAL_STORAGE' maxSdkVersion='32; android.permission.READ_MEDIA_VIDEO; android.permission.READ_MEDIA_AUDIO; android.permission.READ_APP_BADGE; android.permission.READ_MEDIA_IMAGES; android.permission.VIBRATE; com.huawei.android.launcher.permission.CHANGE_BADGE; com.majeur.launcher.permission.UPDATE_BADGE; com.sonymobile.home.permission.PROVIDER_INSERT_BADGE; com.htc.launcher.permission.UPDATE_SHORTCUT; com.feverup.fever.BRANCH_PERMISSION; android.permission.INTERNET; com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE; com.huawei.android.launcher.permission.READ_SETTINGS; android.permission.CAMERA; me.everything.badger.permission.BADGE_COUNT_WRITE; com.oppo.launcher.permission.READ_SETTINGS</t>
+  </si>
+  <si>
+    <t>android.permission.BLUETOOTH_ADMIN' maxSdkVersion='30; com.google.android.gms.permission.AD_ID; android.permission.FLASHLIGHT; android.permission.FOREGROUND_SERVICE; android.permission.RECEIVE_BOOT_COMPLETED; com.android.vending.CHECK_LICENSE; android.permission.BLUETOOTH' maxSdkVersion='30; android.permission.ACCESS_FINE_LOCATION; android.permission.ACCESS_COARSE_LOCATION; com.sephora.permission.C2D_MESSAGE; android.permission.ACCESS_NETWORK_STATE; android.permission.WAKE_LOCK; android.permission.ACCESS_WIFI_STATE; android.permission.POST_NOTIFICATIONS; com.google.android.c2dm.permission.RECEIVE; android.permission.BLUETOOTH_SCAN; android.permission.ACCESS_BACKGROUND_LOCATION; android.permission.VIBRATE; android.permission.REORDER_TASKS; android.permission.CAMERA2; android.permission.INTERNET; com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE; android.permission.CAMERA; android.permission.WRITE_EXTERNAL_STORAGE' maxSdkVersion='28; android.permission.READ_EXTERNAL_STORAGE; android.permission.READ_PHONE_STATE</t>
+  </si>
+  <si>
+    <t>com.google.android.gms.permission.AD_ID; com.sonyericsson.home.permission.BROADCAST_BADGE; com.codeway.wonder.DYNAMIC_RECEIVER_NOT_EXPORTED_PERMISSION; com.htc.launcher.permission.READ_SETTINGS; android.permission.FOREGROUND_SERVICE; android.permission.WRITE_EXTERNAL_STORAGE; com.huawei.android.launcher.permission.WRITE_SETTINGS; me.everything.badger.permission.BADGE_COUNT_READ; com.sec.android.provider.badge.permission.WRITE; com.sec.android.provider.badge.permission.READ; android.permission.ACCESS_NETWORK_STATE; android.permission.WAKE_LOCK; com.anddoes.launcher.permission.UPDATE_COUNT; android.permission.ACCESS_WIFI_STATE; com.codeway.wonder.permission.C2D_MESSAGE; android.permission.POST_NOTIFICATIONS; com.google.android.c2dm.permission.RECEIVE; com.oppo.launcher.permission.WRITE_SETTINGS; android.permission.READ_EXTERNAL_STORAGE' maxSdkVersion='32; android.permission.READ_APP_BADGE; android.permission.READ_MEDIA_IMAGES; android.permission.VIBRATE; com.huawei.android.launcher.permission.CHANGE_BADGE; com.android.vending.BILLING; android.permission.RECORD_AUDIO; com.applovin.array.apphub.permission.BIND_APPHUB_SERVICE; com.majeur.launcher.permission.UPDATE_BADGE; android.permission.SCHEDULE_EXACT_ALARM; com.sonymobile.home.permission.PROVIDER_INSERT_BADGE; com.htc.launcher.permission.UPDATE_SHORTCUT; android.permission.INTERNET; com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE; android.permission.USE_FULL_SCREEN_INTENT; com.huawei.android.launcher.permission.READ_SETTINGS; android.permission.CAMERA; me.everything.badger.permission.BADGE_COUNT_WRITE; android.permission.READ_PHONE_STATE; com.oppo.launcher.permission.READ_SETTINGS</t>
+  </si>
+  <si>
+    <t>android.hardware.screen.landscape implied: one or more activities have specified a landscape orientation; android.hardware.screen.portrait implied: one or more activities have specified a portrait orientation; android.hardware.wifi implied: requested android.permission.ACCESS_WIFI_STATE permission; android.hardware.faketouch implied: default feature for all apps</t>
+  </si>
+  <si>
+    <t>com.google.android.gms.permission.AD_ID; android.permission.FOREGROUND_SERVICE; android.permission.RECEIVE_BOOT_COMPLETED; android.permission.CAMERA' maxSdkVersion='22; android.permission.ACCESS_FINE_LOCATION; ca.autotrader.userapp.DYNAMIC_RECEIVER_NOT_EXPORTED_PERMISSION; android.permission.ACCESS_COARSE_LOCATION; android.permission.INTERNET; android.permission.ACCESS_NETWORK_STATE; android.permission.WAKE_LOCK; com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE; android.permission.ACCESS_WIFI_STATE; ca.autotrader.userapp.permission.READ_EXTERNAL_STORAGE; android.permission.POST_NOTIFICATIONS; com.google.android.c2dm.permission.RECEIVE</t>
+  </si>
+  <si>
+    <t>android.permission.REQUEST_DELETE_PACKAGES; net.oneplus.launcher.permission.READ_SETTINGS; com.actionlauncher.playstore.permission.READ_SETTINGS; com.myhomescreen.messenger.home.emoji.lite.permission.WRITE_SETTINGS; org.adw.launcher.one.permission.READ_SETTINGS; com.transsion.hilauncher.permission.READ_SETTINGS; com.google.android.apps.nexuslauncher.permission.READ_SETTINGS; org.adwfreak.launcher.permission.READ_SETTINGS; android.permission.WAKE_LOCK; android.permission.CANCEL_NOTIFICATIONS; com.google.android.c2dm.permission.RECEIVE; android.permission.PACKAGE_USAGE_STATS; com.cyanogenmod.trebuchet.permission.READ_SETTINGS; com.myhomescreen.messenger.home.emoji.lite.permission.READ_SETTINGS; android.permission.SET_WALLPAPER_HINTS; com.motorola.launcher3.permission.READ_SETTINGS; android.permission.INTERNET; com.chrislacy.actionlauncher.permission.READ_SETTINGS; android.permission.SET_WALLPAPER; android.permission.BLUETOOTH_CONNECT; com.oppo.launcher.permission.READ_SETTINGS; android.permission.READ_CONTACTS; com.teslacoilsw.launcher.permission.READ_SETTINGS; com.google.android.gms.permission.AD_ID; android.permission.READ_SMS; android.permission.GET_ACCOUNTS; android.permission.FLASHLIGHT; com.htc.launcher.permission.READ_SETTINGS; android.permission.FOREGROUND_SERVICE; android.permission.EXPAND_STATUS_BAR; android.permission.BLUETOOTH_ADMIN; android.permission.RECEIVE_BOOT_COMPLETED; android.permission.WRITE_EXTERNAL_STORAGE; com.anddoes.launcher.permission.READ_SETTINGS; android.permission.ACCESS_NOTIFICATION_POLICY; com.lge.launcher3.permission.READ_SETTINGS; android.permission.ACCESS_NETWORK_STATE; org.adw.launcher.permission.READ_SETTINGS; com.android.launcher.permission.INSTALL_SHORTCUT; android.permission.SEND_SMS; android.permission.RECEIVE_SMS; android.permission.WRITE_SMS; com.android.launcher.permission.READ_SETTINGS; android.permission.VIBRATE; android.permission.RECEIVE_MMS; com.google.android.launcher.permission.READ_SETTINGS; com.tcl.android.launcher.permission.READ_SETTINGS; com.android.launcher3.permission.READ_SETTINGS; com.samsung.android.launcher.permission.READ_SETTINGS; com.motorola.launcher3.permission.WRITE_SETTINGS; com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE; com.huawei.android.launcher.permission.READ_SETTINGS; android.permission.CAMERA; android.permission.READ_EXTERNAL_STORAGE; android.permission.BLUETOOTH; android.permission.READ_PHONE_STATE; android.permission.WRITE_SETTINGS; com.android.launcher.permission.WRITE_SETTINGS</t>
+  </si>
+  <si>
+    <t>com.google.android.gms.permission.AD_ID; android.permission.GET_ACCOUNTS; com.sonyericsson.home.permission.BROADCAST_BADGE; com.htc.launcher.permission.READ_SETTINGS; android.permission.FOREGROUND_SERVICE; android.permission.AUTHENTICATE_ACCOUNTS; android.permission.RECEIVE_USER_PRESENT; android.permission.READ_EXTERNAL_STORAGE' maxSdkVersion='29; com.sonyericsson.home.action.UPDATE_BADGE; android.permission.RECEIVE_BOOT_COMPLETED; com.huawei.android.launcher.permission.WRITE_SETTINGS; me.everything.badger.permission.BADGE_COUNT_READ; android.permission.ACCESS_COARSE_LOCATION; com.sec.android.provider.badge.permission.WRITE; com.sec.android.provider.badge.permission.READ; android.permission.ACCESS_NETWORK_STATE; android.permission.REQUEST_IGNORE_BATTERY_OPTIMIZATIONS; com.anddoes.launcher.permission.UPDATE_COUNT; android.permission.WAKE_LOCK; android.permission.ACCESS_WIFI_STATE; android.permission.POST_NOTIFICATIONS; com.oppo.launcher.permission.WRITE_SETTINGS; com.google.android.c2dm.permission.RECEIVE; android.permission.READ_APP_BADGE; com.huawei.android.launcher.permission.CHANGE_BADGE; com.android.vending.BILLING; android.permission.WRITE_SYNC_SETTINGS; com.majeur.launcher.permission.UPDATE_BADGE; com.sonymobile.home.permission.PROVIDER_INSERT_BADGE; com.htc.launcher.permission.UPDATE_SHORTCUT; android.permission.CHANGE_WIFI_STATE; android.permission.INTERNET; com.huawei.permission.external_app_settings.USE_COMPONENT; com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE; android.permission.WRITE_EXTERNAL_STORAGE' maxSdkVersion='29; android.permission.USE_FULL_SCREEN_INTENT; com.huawei.android.launcher.permission.READ_SETTINGS; me.everything.badger.permission.BADGE_COUNT_WRITE; com.oppo.launcher.permission.READ_SETTINGS</t>
+  </si>
+  <si>
+    <t>android.hardware.camera implied: requested android.permission.CAMERA permission; android.hardware.screen.portrait implied: one or more activities have specified a portrait orientation; android.hardware.wifi implied: requested android.permission.ACCESS_WIFI_STATE permission; android.hardware.faketouch implied: default feature for all apps</t>
+  </si>
+  <si>
+    <t>com.google.android.gms.permission.AD_ID; android.permission.ACCESS_MEDIA_LOCATION; android.permission.FOREGROUND_SERVICE; android.permission.READ_MEDIA_IMAGES; android.permission.VIBRATE; com.android.vending.BILLING; android.permission.WRITE_EXTERNAL_STORAGE; com.applovin.array.apphub.permission.BIND_APPHUB_SERVICE; android.permission.PHOTOS; android.permission.INTERNET; com.ai.polyverse.mirror.DYNAMIC_RECEIVER_NOT_EXPORTED_PERMISSION; android.permission.ACCESS_NETWORK_STATE; android.permission.WAKE_LOCK; com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE; android.permission.ACCESS_WIFI_STATE; android.permission.CAMERA; android.permission.READ_EXTERNAL_STORAGE</t>
+  </si>
+  <si>
+    <t>android.permission.BLUETOOTH_ADMIN' maxSdkVersion='30; com.google.android.gms.permission.AD_ID; android.permission.WRITE_CALENDAR; android.permission.FOREGROUND_SERVICE; android.permission.READ_CALENDAR; android.permission.RECEIVE_BOOT_COMPLETED; android.permission.NFC; android.permission.WRITE_EXTERNAL_STORAGE; android.permission.BLUETOOTH' maxSdkVersion='30; android.permission.ACCESS_FINE_LOCATION; android.permission.ACCESS_COARSE_LOCATION; android.permission.ACCESS_NETWORK_STATE; android.permission.WAKE_LOCK; android.permission.ACCESS_WIFI_STATE; android.permission.USE_FINGERPRINT; android.permission.POST_NOTIFICATIONS; com.google.android.c2dm.permission.RECEIVE; android.permission.BLUETOOTH_SCAN; android.permission.VIBRATE; android.permission.CHANGE_WIFI_STATE; android.permission.INTERNET; android.permission.USE_BIOMETRIC; com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE; android.permission.CAMERA; android.permission.READ_EXTERNAL_STORAGE; android.permission.BLUETOOTH_CONNECT; android.permission.WRITE_SETTINGS</t>
+  </si>
+  <si>
+    <t>android.hardware.screen.portrait implied: one or more activities have specified a portrait orientation; android.hardware.vulkan.version; android.hardware.wifi implied: requested android.permission.ACCESS_WIFI_STATE permission</t>
+  </si>
+  <si>
+    <t>com.google.android.gms.permission.AD_ID; android.permission.FOREGROUND_SERVICE; android.permission.VIBRATE; com.android.vending.BILLING; android.permission.WRITE_EXTERNAL_STORAGE; com.applovin.array.apphub.permission.BIND_APPHUB_SERVICE; android.permission.SCHEDULE_EXACT_ALARM; android.permission.ACCESS_NOTIFICATION_POLICY; android.permission.INTERNET; android.permission.BROADCAST_CLOSE_SYSTEM_DIALOGS' maxSdkVersion='30; android.permission.ACCESS_NETWORK_STATE; android.permission.WAKE_LOCK; com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE; android.permission.ACCESS_WIFI_STATE; android.permission.USE_FULL_SCREEN_INTENT; android.permission.POST_NOTIFICATIONS; android.permission.READ_EXTERNAL_STORAGE; com.google.android.c2dm.permission.RECEIVE</t>
+  </si>
+  <si>
+    <t>android.hardware.camera; android.hardware.screen.portrait implied: one or more activities have specified a portrait orientation; android.hardware.microphone implied: requested android.permission.RECORD_AUDIO permission; android.hardware.wifi implied: requested android.permission.ACCESS_WIFI_STATE permission; android.hardware.faketouch implied: default feature for all apps</t>
+  </si>
+  <si>
+    <t>com.google.android.gms.permission.AD_ID; com.sonyericsson.home.permission.BROADCAST_BADGE; com.htc.launcher.permission.READ_SETTINGS; android.permission.FOREGROUND_SERVICE; android.permission.RECEIVE_BOOT_COMPLETED; com.scaleup.chatai.permission.C2D_MESSAGE; com.huawei.android.launcher.permission.WRITE_SETTINGS; me.everything.badger.permission.BADGE_COUNT_READ; com.sec.android.provider.badge.permission.WRITE; com.sec.android.provider.badge.permission.READ; android.permission.ACCESS_NETWORK_STATE; android.permission.WAKE_LOCK; com.anddoes.launcher.permission.UPDATE_COUNT; android.permission.ACCESS_WIFI_STATE; com.scaleup.chatai.DYNAMIC_RECEIVER_NOT_EXPORTED_PERMISSION; android.permission.POST_NOTIFICATIONS; com.google.android.c2dm.permission.RECEIVE; com.oppo.launcher.permission.WRITE_SETTINGS; android.permission.READ_APP_BADGE; android.permission.READ_MEDIA_IMAGES; android.permission.VIBRATE; android.permission.REORDER_TASKS; com.huawei.android.launcher.permission.CHANGE_BADGE; com.android.vending.BILLING; android.permission.RECORD_AUDIO; com.majeur.launcher.permission.UPDATE_BADGE; com.sonymobile.home.permission.PROVIDER_INSERT_BADGE; com.htc.launcher.permission.UPDATE_SHORTCUT; android.permission.INTERNET; com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE; com.huawei.android.launcher.permission.READ_SETTINGS; android.permission.CAMERA; android.permission.READ_EXTERNAL_STORAGE; me.everything.badger.permission.BADGE_COUNT_WRITE; com.oppo.launcher.permission.READ_SETTINGS</t>
+  </si>
+  <si>
+    <t>android.permission.READ_CONTACTS; com.google.android.gms.permission.AD_ID; android.permission.CALL_PHONE; android.permission.FOREGROUND_SERVICE; android.permission.WRITE_CALENDAR; android.permission.VIBRATE; android.permission.SYSTEM_ALERT_WINDOW; ca.crea.app.consumer.DYNAMIC_RECEIVER_NOT_EXPORTED_PERMISSION; android.permission.READ_CALENDAR; android.permission.READ_PROFILE; android.permission.RECEIVE_BOOT_COMPLETED; android.permission.WRITE_EXTERNAL_STORAGE; android.permission.ACCESS_FINE_LOCATION; android.permission.ACCESS_COARSE_LOCATION; android.permission.INTERNET; android.permission.ACCESS_NETWORK_STATE; android.permission.WAKE_LOCK; com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE; android.permission.ACCESS_WIFI_STATE; android.permission.READ_EXTERNAL_STORAGE; android.permission.POST_NOTIFICATIONS; com.google.android.c2dm.permission.RECEIVE</t>
+  </si>
+  <si>
+    <t>com.google.android.gms.permission.AD_ID; android.permission.FOREGROUND_SERVICE; com.loblaw.shoppersdrugmart.DYNAMIC_RECEIVER_NOT_EXPORTED_PERMISSION; android.permission.RECEIVE_BOOT_COMPLETED; android.permission.WRITE_EXTERNAL_STORAGE; android.permission.ACCESS_FINE_LOCATION; android.permission.ACCESS_COARSE_LOCATION; android.permission.INTERNET; android.permission.USE_BIOMETRIC; android.permission.ACCESS_NETWORK_STATE; android.permission.WAKE_LOCK; com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE; android.permission.USE_FINGERPRINT; android.permission.ACCESS_WIFI_STATE; android.permission.CAMERA; android.permission.POST_NOTIFICATIONS; android.permission.READ_EXTERNAL_STORAGE; com.google.android.c2dm.permission.RECEIVE</t>
+  </si>
+  <si>
+    <t>android.hardware.touchscreen; android.hardware.screen.portrait; android.hardware.touchscreen.multitouch</t>
+  </si>
+  <si>
+    <t>android.permission.READ_EXTERNAL_STORAGE' maxSdkVersion='32; com.google.android.gms.permission.AD_ID; android.permission.FOREGROUND_SERVICE; BIND_GET_INSTALL_REFERRER_SERVICE; com.android.vending.BILLING; android.permission.WRITE_EXTERNAL_STORAGE; com.android.vending.CHECK_LICENSE; com.singular.preinstall.READ_PERMISSION_SINGULAR; com.vizmanga.android.DYNAMIC_RECEIVER_NOT_EXPORTED_PERMISSION; android.permission.INTERNET; android.permission.ACCESS_NETWORK_STATE; android.permission.GET_TASKS; android.permission.WAKE_LOCK; com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE; android.permission.POST_NOTIFICATIONS; com.google.android.c2dm.permission.RECEIVE</t>
+  </si>
+  <si>
+    <t>android.hardware.screen.portrait implied: one or more activities have specified a portrait orientation; android.hardware.wifi; android.hardware.faketouch implied: default feature for all apps</t>
+  </si>
+  <si>
+    <t>com.google.android.gms.permission.AD_ID; android.permission.FOREGROUND_SERVICE; android.permission.VIBRATE; custom.permission.NEWS_CONTENT_PROVIDER; android.permission.RECEIVE_BOOT_COMPLETED; com.android.alarm.permission.SET_ALARM; android.permission.INTERNET; android.permission.ACCESS_NETWORK_STATE; android.permission.WAKE_LOCK; com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE; android.permission.ACCESS_WIFI_STATE; ca.cbc.android.sports.permission.C2D_MESSAGE; com.google.android.c2dm.permission.RECEIVE</t>
+  </si>
+  <si>
+    <t>android.permission.BLUETOOTH_ADMIN' maxSdkVersion='30; com.google.android.gms.permission.AD_ID; android.permission.BLUETOOTH_PRIVILEGED; android.permission.FOREGROUND_SERVICE; android.permission.RECEIVE_BOOT_COMPLETED; android.permission.BLUETOOTH' maxSdkVersion='30; android.permission.ACCESS_FINE_LOCATION; android.permission.ACCESS_COARSE_LOCATION; android.permission.ACCESS_NETWORK_STATE; android.permission.WAKE_LOCK; android.permission.ACCESS_WIFI_STATE; android.permission.USE_FINGERPRINT; android.permission.POST_NOTIFICATIONS; com.google.android.c2dm.permission.RECEIVE; android.permission.BLUETOOTH_SCAN; android.permission.VIBRATE; android.permission.RECORD_AUDIO; android.permission.INTERNET; android.permission.USE_BIOMETRIC; com.google.android.finsky.permission.BIND_GET_INSTALL_REFERRER_SERVICE; android.permission.ACTIVITY_RECOGNITION; android.permission.WRITE_EXTERNAL_STORAGE' maxSdkVersion='28; android.permission.MODIFY_AUDIO_SETTINGS; android.permission.CAMERA; android.permission.READ_EXTERNAL_STORAGE; android.permission.BLUETOOTH_CONNECT; com.google.android.gms.permission.ACTIVITY_RECOGNITION</t>
+  </si>
+  <si>
+    <t>android.hardware.screen.portrait implied: one or more activities have specified a portrait orientation; android.hardware.microphone implied: requested android.permission.RECORD_AUDIO permission; android.hardware.wifi implied: requested android.permission.ACCESS_WIFI_STATE permission and android.permission.CHANGE_WIFI_MULTICAST_STATE permission; android.hardware.faketouch implied: default feature for all apps</t>
+  </si>
+  <si>
+    <t>android.hardware.screen.portrait implied: one or more activities have specified a portrait orientation; android.hardware.location implied: requested android.permission.ACCESS_COARSE_LOCATION permission and android.permission.ACCESS_FINE_LOCATION permission; android.hardware.wifi implied: requested android.permission.ACCESS_WIFI_STATE permission; android.hardware.faketouch implied: default feature for all apps</t>
+  </si>
+  <si>
+    <t>android.hardware.screen.portrait implied: one or more activities have specified a portrait orientation; android.software.device_admin; android.hardware.location implied: requested android.permission.ACCESS_COARSE_LOCATION permission and android.permission.ACCESS_FINE_LOCATION permission; android.hardware.wifi implied: requested android.permission.ACCESS_WIFI_STATE permission; android.hardware.faketouch implied: default feature for all apps</t>
+  </si>
+  <si>
+    <t>android.hardware.screen.portrait implied: one or more activities have specified a portrait orientation; android.hardware.microphone implied: requested android.permission.RECORD_AUDIO permission; android.hardware.location implied: requested android.permission.ACCESS_COARSE_LOCATION permission and android.permission.ACCESS_FINE_LOCATION permission; android.hardware.wifi implied: requested android.permission.ACCESS_WIFI_STATE permission; android.hardware.faketouch implied: default feature for all apps</t>
+  </si>
+  <si>
+    <t>android.hardware.camera implied: requested android.permission.CAMERA permission; android.hardware.screen.portrait implied: one or more activities have specified a portrait orientation; android.hardware.location implied: requested android.permission.ACCESS_COARSE_LOCATION permission and android.permission.ACCESS_FINE_LOCATION permission; android.hardware.faketouch implied: default feature for all apps</t>
+  </si>
+  <si>
+    <t>android.hardware.camera implied: requested android.permission.CAMERA permission; android.hardware.screen.landscape implied: one or more activities have specified a landscape orientation; android.hardware.screen.portrait implied: one or more activities have specified a portrait orientation; android.hardware.microphone implied: requested android.permission.RECORD_AUDIO permission; android.hardware.wifi implied: requested android.permission.ACCESS_WIFI_STATE permission and android.permission.CHANGE_WIFI_MULTICAST_STATE permission and android.permission.CHANGE_WIFI_STATE permission</t>
+  </si>
+  <si>
+    <t>android.hardware.screen.portrait implied: one or more activities have specified a portrait orientation; android.hardware.location implied: requested android.permission.ACCESS_COARSE_LOCATION permission and android.permission.ACCESS_FINE_LOCATION permission; android.hardware.wifi implied: requested android.permission.ACCESS_WIFI_STATE permission and android.permission.CHANGE_WIFI_STATE permission; android.hardware.faketouch implied: default feature for all apps</t>
+  </si>
+  <si>
+    <t>android.hardware.camera; android.hardware.screen.portrait implied: one or more activities have specified a portrait orientation; android.hardware.location implied: requested android.permission.ACCESS_COARSE_LOCATION permission and android.permission.ACCESS_FINE_LOCATION permission; android.hardware.wifi implied: requested android.permission.ACCESS_WIFI_STATE permission and android.permission.CHANGE_WIFI_STATE permission; android.hardware.faketouch implied: default feature for all apps</t>
+  </si>
+  <si>
+    <t>android.hardware.screen.portrait implied: one or more activities have specified a portrait orientation; android.hardware.location implied: requested android.permission.ACCESS_COARSE_LOCATION permission and android.permission.ACCESS_FINE_LOCATION permission; android.hardware.faketouch implied: default feature for all apps</t>
+  </si>
+  <si>
+    <t>android.hardware.screen.portrait implied: one or more activities have specified a portrait orientation; android.hardware.location.network; android.hardware.location; android.hardware.wifi implied: requested android.permission.ACCESS_WIFI_STATE permission and android.permission.CHANGE_WIFI_STATE permission; android.hardware.faketouch implied: default feature for all apps</t>
+  </si>
+  <si>
+    <t>android.hardware.camera; android.hardware.screen.portrait implied: one or more activities have specified a portrait orientation; android.hardware.location implied: requested android.permission.ACCESS_COARSE_LOCATION permission and android.permission.ACCESS_FINE_LOCATION permission; android.hardware.wifi implied: requested android.permission.ACCESS_WIFI_STATE permission; android.hardware.faketouch implied: default feature for all apps</t>
+  </si>
+  <si>
+    <t>android.hardware.bluetooth implied: requested android.permission.BLUETOOTH permission and targetSdkVersion &gt; 4; android.hardware.location implied: requested android.permission.ACCESS_COARSE_LOCATION permission</t>
+  </si>
+  <si>
+    <t>android.hardware.bluetooth implied: requested android.permission.BLUETOOTH permission and android.permission.BLUETOOTH_ADMIN permission and targetSdkVersion &gt; 4; android.hardware.camera; android.hardware.screen.portrait implied: one or more activities have specified a portrait orientation; android.hardware.location implied: requested android.permission.ACCESS_COARSE_LOCATION permission and android.permission.ACCESS_FINE_LOCATION permission; android.hardware.wifi implied: requested android.permission.ACCESS_WIFI_STATE permission; android.hardware.faketouch implied: default feature for all apps</t>
+  </si>
+  <si>
+    <t>android.hardware.bluetooth implied: requested android.permission.BLUETOOTH permission and android.permission.BLUETOOTH_ADMIN permission and targetSdkVersion &gt; 4; android.hardware.screen.landscape; android.hardware.microphone implied: requested android.permission.RECORD_AUDIO permission; android.hardware.location implied: requested android.permission.ACCESS_COARSE_LOCATION permission</t>
+  </si>
+  <si>
+    <t>android.hardware.bluetooth implied: requested android.permission.BLUETOOTH permission and targetSdkVersion &gt; 4; android.hardware.camera; android.hardware.screen.portrait implied: one or more activities have specified a portrait orientation; android.hardware.microphone implied: requested android.permission.RECORD_AUDIO permission; android.hardware.location implied: requested android.permission.ACCESS_COARSE_LOCATION permission and android.permission.ACCESS_FINE_LOCATION permission; android.hardware.wifi implied: requested android.permission.ACCESS_WIFI_STATE permission and android.permission.CHANGE_WIFI_STATE permission; android.hardware.faketouch implied: default feature for all apps</t>
+  </si>
+  <si>
+    <t>android.hardware.sensor.gyroscope; android.hardware.sensor.accelerometer; android.hardware.bluetooth implied: requested android.permission.BLUETOOTH permission and android.permission.BLUETOOTH_ADMIN permission and targetSdkVersion &gt; 4; android.hardware.screen.landscape implied: one or more activities have specified a landscape orientation; android.hardware.screen.portrait implied: one or more activities have specified a portrait orientation; android.hardware.location implied: requested android.permission.ACCESS_COARSE_LOCATION permission; android.hardware.wifi implied: requested android.permission.ACCESS_WIFI_STATE permission; android.hardware.faketouch implied: default feature for all apps</t>
+  </si>
+  <si>
+    <t>android.hardware.bluetooth implied: requested android.permission.BLUETOOTH permission and android.permission.BLUETOOTH_ADMIN permission and targetSdkVersion &gt; 4; android.hardware.camera; android.hardware.screen.portrait implied: one or more activities have specified a portrait orientation; android.hardware.telephony implied: requested a telephony permission; android.hardware.camera.flash</t>
+  </si>
+  <si>
+    <t>android.hardware.bluetooth implied: requested android.permission.BLUETOOTH permission and android.permission.BLUETOOTH_ADMIN permission and targetSdkVersion &gt; 4; android.hardware.screen.portrait implied: one or more activities have specified a portrait orientation; android.hardware.location implied: requested android.permission.ACCESS_COARSE_LOCATION permission and android.permission.ACCESS_FINE_LOCATION permission; android.hardware.faketouch implied: default feature for all apps</t>
+  </si>
+  <si>
+    <t>android.hardware.bluetooth implied: requested android.permission.BLUETOOTH permission and android.permission.BLUETOOTH_ADMIN permission and targetSdkVersion &gt; 4; android.hardware.camera; android.hardware.screen.portrait implied: one or more activities have specified a portrait orientation; android.hardware.microphone implied: requested android.permission.RECORD_AUDIO permission; android.hardware.location implied: requested android.permission.ACCESS_COARSE_LOCATION permission and android.permission.ACCESS_FINE_LOCATION permission; android.hardware.faketouch implied: default feature for all apps</t>
+  </si>
+  <si>
+    <t>android.hardware.bluetooth implied: requested android.permission.BLUETOOTH permission and targetSdkVersion &gt; 4; android.hardware.telephony implied: requested a telephony permission; android.hardware.faketouch implied: default feature for all apps</t>
+  </si>
+  <si>
+    <t>android.hardware.location.network implied: requested android.permission.ACCESS_COARSE_LOCATION permission and targetSdkVersion &lt; 21; android.hardware.location implied: requested android.permission.ACCESS_COARSE_LOCATION permission; android.hardware.faketouch implied: default feature for all apps</t>
+  </si>
+  <si>
+    <t>android.hardware.screen.portrait implied: one or more activities have specified a portrait orientation; android.hardware.wifi implied: requested android.permission.ACCESS_WIFI_STATE permission and requested android.permission.CHANGE_WIFI_STATE permission; android.hardware.faketouch implied: default feature for all apps</t>
+  </si>
+  <si>
+    <t>android.hardware.wifi implied: requested android.permission.ACCESS_WIFI_STATE permission and requested android.permission.CHANGE_WIFI_STATE permission; android.hardware.faketouch implied: default feature for all apps</t>
+  </si>
+  <si>
+    <t>android.hardware.location.gps implied: requested android.permission.ACCESS_FINE_LOCATION permission and targetSdkVersion &lt; 21; android.hardware.screen.portrait implied: one or more activities have specified a portrait orientation; android.hardware.location.network implied: requested android.permission.ACCESS_COARSE_LOCATION permission and targetSdkVersion &lt; 21; android.hardware.location implied: requested android.permission.ACCESS_COARSE_LOCATION permission and android.permission.ACCESS_FINE_LOCATION permission and requested android.permission.ACCESS_MOCK_LOCATION permission; android.hardware.faketouch implied: default feature for all apps</t>
+  </si>
+  <si>
+    <t>android.hardware.location.gps implied: requested android.permission.ACCESS_FINE_LOCATION permission and targetSdkVersion &lt; 21; android.hardware.bluetooth implied: requested android.permission.BLUETOOTH permission and android.permission.BLUETOOTH_ADMIN permission and targetSdkVersion &gt; 4; android.hardware.microphone implied: requested android.permission.RECORD_AUDIO permission; android.hardware.telephony implied: requested a telephony permission; android.hardware.location implied: requested android.permission.ACCESS_FINE_LOCATION permission; android.hardware.wifi implied: requested android.permission.ACCESS_WIFI_STATE permission and requested android.permission.CHANGE_WIFI_STATE permission; android.hardware.faketouch implied: default feature for all apps</t>
+  </si>
+  <si>
+    <t>android.hardware.bluetooth implied: requested android.permission.BLUETOOTH permission and android.permission.BLUETOOTH_ADMIN permission;  and targetSdkVersion &gt; 4; android.hardware.location implied: requested android.permission.ACCESS_COARSE_LOCATION permission and android.permission.ACCESS_FINE_LOCATION permission; android.hardware.wifi implied: requested android.permission.ACCESS_WIFI_STATE permission and android.permission.CHANGE_WIFI_STATE permission; android.hardware.faketouch implied: default feature for all apps</t>
   </si>
 </sst>
 </file>
@@ -2227,7 +2227,7 @@
   <dimension ref="A1:M48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="J50" sqref="J50"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -2244,7 +2244,8 @@
     <col min="10" max="10" width="20.7265625" customWidth="1"/>
     <col min="11" max="11" width="8.86328125" style="2"/>
     <col min="12" max="12" width="14" style="2" customWidth="1"/>
-    <col min="13" max="16384" width="8.86328125" style="2"/>
+    <col min="13" max="13" width="11.54296875" style="2" customWidth="1"/>
+    <col min="14" max="16384" width="8.86328125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
@@ -2270,22 +2271,22 @@
         <v>129</v>
       </c>
       <c r="H1" s="43" t="s">
+        <v>355</v>
+      </c>
+      <c r="I1" s="43" t="s">
+        <v>360</v>
+      </c>
+      <c r="J1" s="43" t="s">
+        <v>358</v>
+      </c>
+      <c r="K1" s="43" t="s">
         <v>359</v>
       </c>
-      <c r="I1" s="43" t="s">
-        <v>364</v>
-      </c>
-      <c r="J1" s="43" t="s">
-        <v>362</v>
-      </c>
-      <c r="K1" s="43" t="s">
-        <v>363</v>
-      </c>
       <c r="L1" s="43" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="M1" s="44" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.75">
@@ -2320,13 +2321,13 @@
         <v>0</v>
       </c>
       <c r="K2" s="35" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="L2" s="15">
         <v>8</v>
       </c>
       <c r="M2" s="36" t="s">
-        <v>465</v>
+        <v>372</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.75">
@@ -2361,13 +2362,13 @@
         <v>1</v>
       </c>
       <c r="K3" s="34" t="s">
+        <v>363</v>
+      </c>
+      <c r="L3" s="13">
+        <v>1</v>
+      </c>
+      <c r="M3" s="37" t="s">
         <v>367</v>
-      </c>
-      <c r="L3" s="13">
-        <v>1</v>
-      </c>
-      <c r="M3" s="37" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.75">
@@ -2402,13 +2403,13 @@
         <v>1</v>
       </c>
       <c r="K4" s="34" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="L4" s="13">
         <v>22</v>
       </c>
       <c r="M4" s="37" t="s">
-        <v>466</v>
+        <v>373</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.75">
@@ -2443,13 +2444,13 @@
         <v>1</v>
       </c>
       <c r="K5" s="34" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="L5" s="13">
         <v>3</v>
       </c>
       <c r="M5" s="37" t="s">
-        <v>467</v>
+        <v>374</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.75">
@@ -2484,13 +2485,13 @@
         <v>1</v>
       </c>
       <c r="K6" s="34" t="s">
+        <v>363</v>
+      </c>
+      <c r="L6" s="13">
+        <v>1</v>
+      </c>
+      <c r="M6" s="37" t="s">
         <v>367</v>
-      </c>
-      <c r="L6" s="13">
-        <v>1</v>
-      </c>
-      <c r="M6" s="37" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.75">
@@ -2525,13 +2526,13 @@
         <v>5</v>
       </c>
       <c r="K7" s="34" t="s">
-        <v>468</v>
+        <v>499</v>
       </c>
       <c r="L7" s="13">
         <v>4</v>
       </c>
       <c r="M7" s="37" t="s">
-        <v>469</v>
+        <v>375</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.75">
@@ -2566,13 +2567,13 @@
         <v>2</v>
       </c>
       <c r="K8" s="34" t="s">
-        <v>455</v>
+        <v>376</v>
       </c>
       <c r="L8" s="13">
         <v>6</v>
       </c>
       <c r="M8" s="37" t="s">
-        <v>470</v>
+        <v>377</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.75">
@@ -2607,13 +2608,13 @@
         <v>0</v>
       </c>
       <c r="K9" s="34" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="L9" s="13">
         <v>4</v>
       </c>
       <c r="M9" s="37" t="s">
-        <v>471</v>
+        <v>378</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.75">
@@ -2648,13 +2649,13 @@
         <v>1</v>
       </c>
       <c r="K10" s="34" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="L10" s="13">
         <v>3</v>
       </c>
       <c r="M10" s="37" t="s">
-        <v>472</v>
+        <v>379</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.75">
@@ -2689,13 +2690,13 @@
         <v>1</v>
       </c>
       <c r="K11" s="34" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="L11" s="13">
         <v>6</v>
       </c>
       <c r="M11" s="37" t="s">
-        <v>473</v>
+        <v>380</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.75">
@@ -2730,13 +2731,13 @@
         <v>3</v>
       </c>
       <c r="K12" s="34" t="s">
-        <v>474</v>
+        <v>495</v>
       </c>
       <c r="L12" s="13">
         <v>7</v>
       </c>
       <c r="M12" s="37" t="s">
-        <v>475</v>
+        <v>381</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.75">
@@ -2771,13 +2772,13 @@
         <v>1</v>
       </c>
       <c r="K13" s="34" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="L13" s="13">
         <v>3</v>
       </c>
       <c r="M13" s="37" t="s">
-        <v>472</v>
+        <v>379</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.75">
@@ -2812,13 +2813,13 @@
         <v>2</v>
       </c>
       <c r="K14" s="34" t="s">
-        <v>476</v>
+        <v>382</v>
       </c>
       <c r="L14" s="13">
         <v>5</v>
       </c>
       <c r="M14" s="37" t="s">
-        <v>477</v>
+        <v>383</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.75">
@@ -2853,13 +2854,13 @@
         <v>2</v>
       </c>
       <c r="K15" s="34" t="s">
-        <v>478</v>
+        <v>384</v>
       </c>
       <c r="L15" s="13">
         <v>1</v>
       </c>
       <c r="M15" s="37" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.75">
@@ -2894,13 +2895,13 @@
         <v>1</v>
       </c>
       <c r="K16" s="34" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="L16" s="13">
         <v>3</v>
       </c>
       <c r="M16" s="37" t="s">
-        <v>472</v>
+        <v>379</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.75">
@@ -2935,13 +2936,13 @@
         <v>0</v>
       </c>
       <c r="K17" s="34" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="L17" s="13">
         <v>0</v>
       </c>
       <c r="M17" s="37" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.75">
@@ -2976,13 +2977,13 @@
         <v>2</v>
       </c>
       <c r="K18" s="34" t="s">
-        <v>476</v>
+        <v>382</v>
       </c>
       <c r="L18" s="13">
         <v>8</v>
       </c>
       <c r="M18" s="37" t="s">
-        <v>479</v>
+        <v>385</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.75">
@@ -3017,13 +3018,13 @@
         <v>2</v>
       </c>
       <c r="K19" s="34" t="s">
-        <v>455</v>
+        <v>376</v>
       </c>
       <c r="L19" s="13">
         <v>4</v>
       </c>
       <c r="M19" s="37" t="s">
-        <v>480</v>
+        <v>386</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.75">
@@ -3136,7 +3137,7 @@
         <v>1</v>
       </c>
       <c r="M22" s="42" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.75">
@@ -3171,13 +3172,13 @@
         <v>1</v>
       </c>
       <c r="K23" s="34" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="L23" s="13">
         <v>1</v>
       </c>
       <c r="M23" s="37" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.75">
@@ -3212,13 +3213,13 @@
         <v>1</v>
       </c>
       <c r="K24" s="34" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="L24" s="13">
         <v>7</v>
       </c>
       <c r="M24" s="37" t="s">
-        <v>481</v>
+        <v>387</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.75">
@@ -3253,13 +3254,13 @@
         <v>3</v>
       </c>
       <c r="K25" s="34" t="s">
-        <v>482</v>
+        <v>388</v>
       </c>
       <c r="L25" s="13">
         <v>8</v>
       </c>
       <c r="M25" s="37" t="s">
-        <v>483</v>
+        <v>389</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.75">
@@ -3294,13 +3295,13 @@
         <v>2</v>
       </c>
       <c r="K26" s="34" t="s">
-        <v>455</v>
+        <v>376</v>
       </c>
       <c r="L26" s="13">
         <v>4</v>
       </c>
       <c r="M26" s="37" t="s">
-        <v>480</v>
+        <v>386</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.75">
@@ -3335,13 +3336,13 @@
         <v>1</v>
       </c>
       <c r="K27" s="34" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="L27" s="13">
         <v>4</v>
       </c>
       <c r="M27" s="37" t="s">
-        <v>484</v>
+        <v>390</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.75">
@@ -3376,13 +3377,13 @@
         <v>3</v>
       </c>
       <c r="K28" s="34" t="s">
-        <v>485</v>
+        <v>496</v>
       </c>
       <c r="L28" s="13">
         <v>4</v>
       </c>
       <c r="M28" s="37" t="s">
-        <v>486</v>
+        <v>391</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.75">
@@ -3417,13 +3418,13 @@
         <v>1</v>
       </c>
       <c r="K29" s="34" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="L29" s="13">
         <v>2</v>
       </c>
       <c r="M29" s="37" t="s">
-        <v>487</v>
+        <v>392</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.75">
@@ -3458,13 +3459,13 @@
         <v>2</v>
       </c>
       <c r="K30" s="34" t="s">
-        <v>476</v>
+        <v>382</v>
       </c>
       <c r="L30" s="13">
         <v>7</v>
       </c>
       <c r="M30" s="37" t="s">
-        <v>488</v>
+        <v>393</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.75">
@@ -3499,13 +3500,13 @@
         <v>1</v>
       </c>
       <c r="K31" s="34" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="L31" s="13">
         <v>1</v>
       </c>
       <c r="M31" s="37" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.75">
@@ -3540,13 +3541,13 @@
         <v>1</v>
       </c>
       <c r="K32" s="34" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="L32" s="13">
         <v>3</v>
       </c>
       <c r="M32" s="37" t="s">
-        <v>489</v>
+        <v>394</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.75">
@@ -3581,13 +3582,13 @@
         <v>2</v>
       </c>
       <c r="K33" s="34" t="s">
-        <v>426</v>
+        <v>395</v>
       </c>
       <c r="L33" s="13">
         <v>5</v>
       </c>
       <c r="M33" s="37" t="s">
-        <v>490</v>
+        <v>396</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.75">
@@ -3622,13 +3623,13 @@
         <v>1</v>
       </c>
       <c r="K34" s="34" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="L34" s="13">
         <v>7</v>
       </c>
       <c r="M34" s="37" t="s">
-        <v>491</v>
+        <v>397</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.75">
@@ -3663,13 +3664,13 @@
         <v>3</v>
       </c>
       <c r="K35" s="34" t="s">
-        <v>492</v>
+        <v>497</v>
       </c>
       <c r="L35" s="13">
         <v>22</v>
       </c>
       <c r="M35" s="37" t="s">
-        <v>493</v>
+        <v>398</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.75">
@@ -3708,7 +3709,7 @@
         <v>2</v>
       </c>
       <c r="M36" s="42" t="s">
-        <v>500</v>
+        <v>399</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.75">
@@ -3743,13 +3744,13 @@
         <v>2</v>
       </c>
       <c r="K37" s="34" t="s">
-        <v>381</v>
+        <v>400</v>
       </c>
       <c r="L37" s="13">
         <v>6</v>
       </c>
       <c r="M37" s="37" t="s">
-        <v>494</v>
+        <v>401</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.75">
@@ -3784,13 +3785,13 @@
         <v>7</v>
       </c>
       <c r="K38" s="34" t="s">
-        <v>495</v>
+        <v>500</v>
       </c>
       <c r="L38" s="13">
         <v>25</v>
       </c>
       <c r="M38" s="37" t="s">
-        <v>496</v>
+        <v>402</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.75">
@@ -3860,13 +3861,13 @@
         <v>0</v>
       </c>
       <c r="K40" s="34" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="L40" s="13">
         <v>0</v>
       </c>
       <c r="M40" s="37" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.75">
@@ -3938,13 +3939,13 @@
         <v>2</v>
       </c>
       <c r="K42" s="34" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="L42" s="13">
         <v>7</v>
       </c>
       <c r="M42" s="37" t="s">
-        <v>498</v>
+        <v>403</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.75">
@@ -3983,7 +3984,7 @@
         <v>7</v>
       </c>
       <c r="M43" s="13" t="s">
-        <v>501</v>
+        <v>404</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.75">
@@ -4055,13 +4056,13 @@
         <v>2</v>
       </c>
       <c r="K45" s="34" t="s">
-        <v>379</v>
+        <v>405</v>
       </c>
       <c r="L45" s="13">
         <v>3</v>
       </c>
       <c r="M45" s="37" t="s">
-        <v>472</v>
+        <v>379</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.75">
@@ -4096,13 +4097,13 @@
         <v>1</v>
       </c>
       <c r="K46" s="34" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="L46" s="13">
         <v>0</v>
       </c>
       <c r="M46" s="37" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.75">
@@ -4137,13 +4138,13 @@
         <v>1</v>
       </c>
       <c r="K47" s="34" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="L47" s="13">
         <v>0</v>
       </c>
       <c r="M47" s="37" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="48" spans="1:13" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
@@ -4178,13 +4179,13 @@
         <v>0</v>
       </c>
       <c r="K48" s="38" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="L48" s="14">
         <v>5</v>
       </c>
       <c r="M48" s="39" t="s">
-        <v>499</v>
+        <v>406</v>
       </c>
     </row>
   </sheetData>
@@ -4201,8 +4202,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B385612B-4AB7-4533-A5E4-09CD735EBEA7}">
   <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="87" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView topLeftCell="C1" zoomScale="87" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -4245,22 +4246,22 @@
         <v>129</v>
       </c>
       <c r="H1" s="31" t="s">
+        <v>354</v>
+      </c>
+      <c r="I1" s="31" t="s">
+        <v>354</v>
+      </c>
+      <c r="J1" s="31" t="s">
         <v>358</v>
       </c>
-      <c r="I1" s="31" t="s">
-        <v>358</v>
-      </c>
-      <c r="J1" s="31" t="s">
-        <v>362</v>
-      </c>
       <c r="K1" s="31" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="L1" s="31" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="M1" s="32" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.75">
@@ -4295,13 +4296,13 @@
         <v>2</v>
       </c>
       <c r="K2" s="35" t="s">
-        <v>455</v>
+        <v>376</v>
       </c>
       <c r="L2" s="15">
         <v>1</v>
       </c>
       <c r="M2" s="36" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.75">
@@ -4336,13 +4337,13 @@
         <v>1</v>
       </c>
       <c r="K3" s="34" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="L3" s="13">
         <v>1</v>
       </c>
       <c r="M3" s="37" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.75">
@@ -4377,13 +4378,13 @@
         <v>1</v>
       </c>
       <c r="K4" s="34" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="L4" s="13">
         <v>0</v>
       </c>
       <c r="M4" s="37" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.75">
@@ -4418,13 +4419,13 @@
         <v>1</v>
       </c>
       <c r="K5" s="34" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="L5" s="13">
         <v>5</v>
       </c>
       <c r="M5" s="37" t="s">
-        <v>461</v>
+        <v>407</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.75">
@@ -4459,13 +4460,13 @@
         <v>0</v>
       </c>
       <c r="K6" s="34" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="L6" s="13">
         <v>6</v>
       </c>
       <c r="M6" s="37" t="s">
-        <v>457</v>
+        <v>408</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.75">
@@ -4500,13 +4501,13 @@
         <v>4</v>
       </c>
       <c r="K7" s="34" t="s">
-        <v>452</v>
+        <v>501</v>
       </c>
       <c r="L7" s="13">
         <v>17</v>
       </c>
       <c r="M7" s="37" t="s">
-        <v>453</v>
+        <v>409</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.75">
@@ -4541,13 +4542,13 @@
         <v>3</v>
       </c>
       <c r="K8" s="34" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="L8" s="13">
         <v>9</v>
       </c>
       <c r="M8" s="37" t="s">
-        <v>456</v>
+        <v>411</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.75">
@@ -4582,13 +4583,13 @@
         <v>2</v>
       </c>
       <c r="K9" s="34" t="s">
-        <v>381</v>
+        <v>400</v>
       </c>
       <c r="L9" s="13">
         <v>5</v>
       </c>
       <c r="M9" s="37" t="s">
-        <v>454</v>
+        <v>412</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.75">
@@ -4623,13 +4624,13 @@
         <v>1</v>
       </c>
       <c r="K10" s="34" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="L10" s="13">
         <v>5</v>
       </c>
       <c r="M10" s="37" t="s">
-        <v>459</v>
+        <v>413</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.75">
@@ -4664,13 +4665,13 @@
         <v>1</v>
       </c>
       <c r="K11" s="34" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="L11" s="13">
         <v>1</v>
       </c>
       <c r="M11" s="37" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.75">
@@ -4705,13 +4706,13 @@
         <v>0</v>
       </c>
       <c r="K12" s="34" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="L12" s="13">
         <v>12</v>
       </c>
       <c r="M12" s="37" t="s">
-        <v>458</v>
+        <v>414</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.75">
@@ -4746,13 +4747,13 @@
         <v>1</v>
       </c>
       <c r="K13" s="34" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="L13" s="13">
         <v>20</v>
       </c>
       <c r="M13" s="37" t="s">
-        <v>460</v>
+        <v>415</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.75">
@@ -4787,13 +4788,13 @@
         <v>0</v>
       </c>
       <c r="K14" s="34" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="L14" s="13">
         <v>15</v>
       </c>
       <c r="M14" s="37" t="s">
-        <v>462</v>
+        <v>416</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
@@ -4828,13 +4829,13 @@
         <v>1</v>
       </c>
       <c r="K15" s="38" t="s">
-        <v>463</v>
+        <v>417</v>
       </c>
       <c r="L15" s="14">
         <v>20</v>
       </c>
       <c r="M15" s="39" t="s">
-        <v>464</v>
+        <v>418</v>
       </c>
     </row>
   </sheetData>
@@ -4857,8 +4858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BADE359F-D744-4042-8AB1-E2120DD4E375}">
   <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView topLeftCell="G17" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -4886,13 +4887,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="D1" s="21" t="s">
         <v>189</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="F1" s="22" t="s">
         <v>190</v>
@@ -4901,22 +4902,22 @@
         <v>129</v>
       </c>
       <c r="H1" s="40" t="s">
+        <v>354</v>
+      </c>
+      <c r="I1" s="40" t="s">
+        <v>371</v>
+      </c>
+      <c r="J1" s="40" t="s">
         <v>358</v>
       </c>
-      <c r="I1" s="40" t="s">
-        <v>451</v>
-      </c>
-      <c r="J1" s="40" t="s">
-        <v>362</v>
-      </c>
       <c r="K1" s="40" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="L1" s="40" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="M1" s="41" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.75">
@@ -4933,7 +4934,7 @@
         <v>194</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="F2" s="18">
         <v>4</v>
@@ -4951,13 +4952,13 @@
         <v>3</v>
       </c>
       <c r="K2" s="35" t="s">
-        <v>448</v>
+        <v>419</v>
       </c>
       <c r="L2" s="15">
         <v>66</v>
       </c>
       <c r="M2" s="36" t="s">
-        <v>449</v>
+        <v>420</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.75">
@@ -4974,7 +4975,7 @@
         <v>198</v>
       </c>
       <c r="E3" s="25" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="F3" s="25">
         <v>36</v>
@@ -4992,13 +4993,13 @@
         <v>4</v>
       </c>
       <c r="K3" s="34" t="s">
-        <v>437</v>
+        <v>476</v>
       </c>
       <c r="L3" s="13">
         <v>43</v>
       </c>
       <c r="M3" s="37" t="s">
-        <v>438</v>
+        <v>421</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.75">
@@ -5015,7 +5016,7 @@
         <v>201</v>
       </c>
       <c r="E4" s="25" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="F4" s="25">
         <v>25</v>
@@ -5033,13 +5034,13 @@
         <v>1</v>
       </c>
       <c r="K4" s="34" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="L4" s="13">
         <v>46</v>
       </c>
       <c r="M4" s="37" t="s">
-        <v>410</v>
+        <v>422</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.75">
@@ -5056,7 +5057,7 @@
         <v>201</v>
       </c>
       <c r="E5" s="25" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F5" s="25">
         <v>6</v>
@@ -5074,13 +5075,13 @@
         <v>2</v>
       </c>
       <c r="K5" s="34" t="s">
-        <v>443</v>
+        <v>487</v>
       </c>
       <c r="L5" s="13">
         <v>43</v>
       </c>
       <c r="M5" s="37" t="s">
-        <v>444</v>
+        <v>423</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.75">
@@ -5097,7 +5098,7 @@
         <v>206</v>
       </c>
       <c r="E6" s="25" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="F6" s="25">
         <v>53</v>
@@ -5115,13 +5116,13 @@
         <v>4</v>
       </c>
       <c r="K6" s="34" t="s">
-        <v>400</v>
+        <v>477</v>
       </c>
       <c r="L6" s="13">
         <v>25</v>
       </c>
       <c r="M6" s="37" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.75">
@@ -5138,7 +5139,7 @@
         <v>210</v>
       </c>
       <c r="E7" s="25" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="F7" s="25">
         <v>23</v>
@@ -5156,13 +5157,13 @@
         <v>6</v>
       </c>
       <c r="K7" s="34" t="s">
-        <v>431</v>
+        <v>488</v>
       </c>
       <c r="L7" s="13">
         <v>35</v>
       </c>
       <c r="M7" s="37" t="s">
-        <v>445</v>
+        <v>425</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.75">
@@ -5179,7 +5180,7 @@
         <v>213</v>
       </c>
       <c r="E8" s="25" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="F8" s="25">
         <v>17</v>
@@ -5197,13 +5198,13 @@
         <v>2</v>
       </c>
       <c r="K8" s="34" t="s">
-        <v>379</v>
+        <v>405</v>
       </c>
       <c r="L8" s="13">
         <v>41</v>
       </c>
       <c r="M8" s="37" t="s">
-        <v>380</v>
+        <v>426</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.75">
@@ -5220,7 +5221,7 @@
         <v>219</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="F9" s="25">
         <v>8</v>
@@ -5238,13 +5239,13 @@
         <v>5</v>
       </c>
       <c r="K9" s="34" t="s">
-        <v>408</v>
+        <v>478</v>
       </c>
       <c r="L9" s="13">
         <v>25</v>
       </c>
       <c r="M9" s="37" t="s">
-        <v>409</v>
+        <v>427</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.75">
@@ -5261,7 +5262,7 @@
         <v>216</v>
       </c>
       <c r="E10" s="25" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="F10" s="25">
         <v>8</v>
@@ -5279,13 +5280,13 @@
         <v>4</v>
       </c>
       <c r="K10" s="34" t="s">
-        <v>391</v>
+        <v>428</v>
       </c>
       <c r="L10" s="13">
         <v>40</v>
       </c>
       <c r="M10" s="37" t="s">
-        <v>392</v>
+        <v>429</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.75">
@@ -5302,7 +5303,7 @@
         <v>223</v>
       </c>
       <c r="E11" s="25" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="F11" s="25">
         <v>20</v>
@@ -5314,13 +5315,13 @@
         <v>14</v>
       </c>
       <c r="I11" s="13">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J11" s="13">
         <v>4</v>
       </c>
       <c r="K11" s="34" t="s">
-        <v>429</v>
+        <v>489</v>
       </c>
       <c r="L11" s="13">
         <v>116</v>
@@ -5343,7 +5344,7 @@
         <v>226</v>
       </c>
       <c r="E12" s="25" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="F12" s="25">
         <v>51</v>
@@ -5361,13 +5362,13 @@
         <v>1</v>
       </c>
       <c r="K12" s="34" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="L12" s="13">
         <v>34</v>
       </c>
       <c r="M12" s="37" t="s">
-        <v>399</v>
+        <v>431</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.75">
@@ -5384,7 +5385,7 @@
         <v>229</v>
       </c>
       <c r="E13" s="25" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="F13" s="25">
         <v>32</v>
@@ -5402,30 +5403,30 @@
         <v>2</v>
       </c>
       <c r="K13" s="34" t="s">
-        <v>381</v>
+        <v>400</v>
       </c>
       <c r="L13" s="13">
         <v>38</v>
       </c>
       <c r="M13" s="37" t="s">
-        <v>382</v>
+        <v>432</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A14" s="23" t="s">
+        <v>433</v>
+      </c>
+      <c r="B14" s="24" t="s">
         <v>230</v>
-      </c>
-      <c r="B14" s="24" t="s">
-        <v>231</v>
       </c>
       <c r="C14" s="24" t="s">
         <v>222</v>
       </c>
       <c r="D14" s="24" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E14" s="25" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="F14" s="25">
         <v>31</v>
@@ -5443,30 +5444,30 @@
         <v>3</v>
       </c>
       <c r="K14" s="34" t="s">
-        <v>389</v>
+        <v>434</v>
       </c>
       <c r="L14" s="13">
         <v>16</v>
       </c>
       <c r="M14" s="37" t="s">
-        <v>390</v>
+        <v>435</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A15" s="23" t="s">
+        <v>232</v>
+      </c>
+      <c r="B15" s="24" t="s">
         <v>233</v>
-      </c>
-      <c r="B15" s="24" t="s">
-        <v>234</v>
       </c>
       <c r="C15" s="24" t="s">
         <v>222</v>
       </c>
       <c r="D15" s="24" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E15" s="25" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="F15" s="25">
         <v>15</v>
@@ -5484,21 +5485,21 @@
         <v>5</v>
       </c>
       <c r="K15" s="34" t="s">
-        <v>419</v>
+        <v>479</v>
       </c>
       <c r="L15" s="13">
         <v>66</v>
       </c>
       <c r="M15" s="37" t="s">
-        <v>420</v>
+        <v>436</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A16" s="23" t="s">
+        <v>235</v>
+      </c>
+      <c r="B16" s="24" t="s">
         <v>236</v>
-      </c>
-      <c r="B16" s="24" t="s">
-        <v>237</v>
       </c>
       <c r="C16" s="24" t="s">
         <v>222</v>
@@ -5507,7 +5508,7 @@
         <v>213</v>
       </c>
       <c r="E16" s="25" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="F16" s="25">
         <v>2</v>
@@ -5525,30 +5526,30 @@
         <v>2</v>
       </c>
       <c r="K16" s="34" t="s">
-        <v>426</v>
+        <v>395</v>
       </c>
       <c r="L16" s="13">
         <v>11</v>
       </c>
       <c r="M16" s="37" t="s">
-        <v>427</v>
+        <v>437</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A17" s="23" t="s">
+        <v>237</v>
+      </c>
+      <c r="B17" s="24" t="s">
         <v>238</v>
       </c>
-      <c r="B17" s="24" t="s">
+      <c r="C17" s="24" t="s">
         <v>239</v>
       </c>
-      <c r="C17" s="24" t="s">
+      <c r="D17" s="24" t="s">
         <v>240</v>
       </c>
-      <c r="D17" s="24" t="s">
-        <v>241</v>
-      </c>
       <c r="E17" s="25" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="F17" s="25">
         <v>73</v>
@@ -5566,33 +5567,33 @@
         <v>7</v>
       </c>
       <c r="K17" s="34" t="s">
-        <v>387</v>
+        <v>490</v>
       </c>
       <c r="L17" s="13">
         <v>46</v>
       </c>
       <c r="M17" s="37" t="s">
-        <v>388</v>
+        <v>438</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A18" s="23" t="s">
+        <v>245</v>
+      </c>
+      <c r="B18" s="24" t="s">
         <v>246</v>
       </c>
-      <c r="B18" s="24" t="s">
+      <c r="C18" s="24" t="s">
+        <v>242</v>
+      </c>
+      <c r="D18" s="24" t="s">
         <v>247</v>
-      </c>
-      <c r="C18" s="24" t="s">
-        <v>243</v>
-      </c>
-      <c r="D18" s="24" t="s">
-        <v>248</v>
       </c>
       <c r="E18" s="25">
         <v>3.4</v>
       </c>
       <c r="F18" s="25" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G18" s="24">
         <v>17</v>
@@ -5607,33 +5608,33 @@
         <v>4</v>
       </c>
       <c r="K18" s="34" t="s">
-        <v>385</v>
+        <v>480</v>
       </c>
       <c r="L18" s="13">
         <v>42</v>
       </c>
       <c r="M18" s="37" t="s">
-        <v>386</v>
+        <v>439</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A19" s="23" t="s">
+        <v>241</v>
+      </c>
+      <c r="B19" s="26" t="s">
+        <v>352</v>
+      </c>
+      <c r="C19" s="24" t="s">
         <v>242</v>
       </c>
-      <c r="B19" s="26" t="s">
-        <v>356</v>
-      </c>
-      <c r="C19" s="24" t="s">
+      <c r="D19" s="24" t="s">
         <v>243</v>
       </c>
-      <c r="D19" s="24" t="s">
+      <c r="E19" s="25" t="s">
+        <v>329</v>
+      </c>
+      <c r="F19" s="25" t="s">
         <v>244</v>
-      </c>
-      <c r="E19" s="25" t="s">
-        <v>333</v>
-      </c>
-      <c r="F19" s="25" t="s">
-        <v>245</v>
       </c>
       <c r="G19" s="24">
         <v>16</v>
@@ -5648,30 +5649,30 @@
         <v>8</v>
       </c>
       <c r="K19" s="34" t="s">
-        <v>393</v>
+        <v>491</v>
       </c>
       <c r="L19" s="13">
         <v>15</v>
       </c>
       <c r="M19" s="37" t="s">
-        <v>394</v>
+        <v>440</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A20" s="23" t="s">
+        <v>248</v>
+      </c>
+      <c r="B20" s="24" t="s">
         <v>249</v>
       </c>
-      <c r="B20" s="24" t="s">
+      <c r="C20" s="24" t="s">
+        <v>242</v>
+      </c>
+      <c r="D20" s="24" t="s">
         <v>250</v>
       </c>
-      <c r="C20" s="24" t="s">
-        <v>243</v>
-      </c>
-      <c r="D20" s="24" t="s">
-        <v>251</v>
-      </c>
       <c r="E20" s="25" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="F20" s="25">
         <v>70</v>
@@ -5689,30 +5690,30 @@
         <v>5</v>
       </c>
       <c r="K20" s="34" t="s">
-        <v>406</v>
+        <v>481</v>
       </c>
       <c r="L20" s="13">
         <v>25</v>
       </c>
       <c r="M20" s="37" t="s">
-        <v>407</v>
+        <v>441</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A21" s="23" t="s">
+        <v>442</v>
+      </c>
+      <c r="B21" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="C21" s="24" t="s">
+        <v>242</v>
+      </c>
+      <c r="D21" s="24" t="s">
         <v>252</v>
       </c>
-      <c r="B21" s="24" t="s">
-        <v>253</v>
-      </c>
-      <c r="C21" s="24" t="s">
-        <v>243</v>
-      </c>
-      <c r="D21" s="24" t="s">
-        <v>254</v>
-      </c>
       <c r="E21" s="25" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="F21" s="25">
         <v>68</v>
@@ -5730,30 +5731,30 @@
         <v>4</v>
       </c>
       <c r="K21" s="34" t="s">
-        <v>400</v>
+        <v>477</v>
       </c>
       <c r="L21" s="13">
         <v>21</v>
       </c>
       <c r="M21" s="37" t="s">
-        <v>401</v>
+        <v>443</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A22" s="23" t="s">
+        <v>253</v>
+      </c>
+      <c r="B22" s="24" t="s">
+        <v>254</v>
+      </c>
+      <c r="C22" s="24" t="s">
+        <v>242</v>
+      </c>
+      <c r="D22" s="24" t="s">
         <v>255</v>
       </c>
-      <c r="B22" s="24" t="s">
-        <v>256</v>
-      </c>
-      <c r="C22" s="24" t="s">
-        <v>243</v>
-      </c>
-      <c r="D22" s="24" t="s">
-        <v>257</v>
-      </c>
       <c r="E22" s="25" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="F22" s="25">
         <v>1</v>
@@ -5771,30 +5772,30 @@
         <v>1</v>
       </c>
       <c r="K22" s="34" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="L22" s="13">
         <v>16</v>
       </c>
       <c r="M22" s="37" t="s">
-        <v>439</v>
+        <v>444</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A23" s="23" t="s">
+        <v>256</v>
+      </c>
+      <c r="B23" s="24" t="s">
+        <v>257</v>
+      </c>
+      <c r="C23" s="24" t="s">
+        <v>242</v>
+      </c>
+      <c r="D23" s="24" t="s">
         <v>258</v>
       </c>
-      <c r="B23" s="24" t="s">
-        <v>259</v>
-      </c>
-      <c r="C23" s="24" t="s">
-        <v>243</v>
-      </c>
-      <c r="D23" s="24" t="s">
-        <v>260</v>
-      </c>
       <c r="E23" s="25" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="F23" s="25">
         <v>64</v>
@@ -5812,24 +5813,24 @@
         <v>4</v>
       </c>
       <c r="K23" s="34" t="s">
-        <v>440</v>
+        <v>482</v>
       </c>
       <c r="L23" s="13">
         <v>23</v>
       </c>
       <c r="M23" s="37" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A24" s="23" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B24" s="24" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D24" s="24" t="s">
         <v>226</v>
@@ -5853,27 +5854,27 @@
         <v>4</v>
       </c>
       <c r="K24" s="34" t="s">
-        <v>423</v>
+        <v>446</v>
       </c>
       <c r="L24" s="13">
         <v>15</v>
       </c>
       <c r="M24" s="37" t="s">
-        <v>424</v>
+        <v>447</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A25" s="23" t="s">
-        <v>263</v>
+        <v>448</v>
       </c>
       <c r="B25" s="24" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C25" s="24" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D25" s="24" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="E25" s="25">
         <v>240</v>
@@ -5894,30 +5895,30 @@
         <v>4</v>
       </c>
       <c r="K25" s="34" t="s">
-        <v>400</v>
+        <v>477</v>
       </c>
       <c r="L25" s="13">
         <v>22</v>
       </c>
       <c r="M25" s="37" t="s">
-        <v>442</v>
+        <v>449</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A26" s="23" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B26" s="24" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C26" s="24" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D26" s="24" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="E26" s="25" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="F26" s="25">
         <v>19</v>
@@ -5935,30 +5936,30 @@
         <v>4</v>
       </c>
       <c r="K26" s="34" t="s">
-        <v>433</v>
+        <v>450</v>
       </c>
       <c r="L26" s="13">
         <v>20</v>
       </c>
       <c r="M26" s="37" t="s">
-        <v>434</v>
+        <v>451</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A27" s="23" t="s">
-        <v>269</v>
+        <v>452</v>
       </c>
       <c r="B27" s="24" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="C27" s="24" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D27" s="24" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="E27" s="25" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F27" s="25">
         <v>1</v>
@@ -5976,30 +5977,30 @@
         <v>3</v>
       </c>
       <c r="K27" s="34" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="L27" s="13">
         <v>16</v>
       </c>
       <c r="M27" s="37" t="s">
-        <v>412</v>
+        <v>453</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A28" s="23" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="B28" s="24" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="C28" s="24" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="D28" s="24" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="E28" s="25" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="F28" s="25">
         <v>14</v>
@@ -6017,33 +6018,33 @@
         <v>5</v>
       </c>
       <c r="K28" s="34" t="s">
-        <v>415</v>
+        <v>483</v>
       </c>
       <c r="L28" s="13">
         <v>22</v>
       </c>
       <c r="M28" s="37" t="s">
-        <v>416</v>
+        <v>454</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A29" s="23" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B29" s="24" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="C29" s="24" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="D29" s="24" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="E29" s="25" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="F29" s="25" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G29" s="24">
         <v>125</v>
@@ -6058,27 +6059,27 @@
         <v>3</v>
       </c>
       <c r="K29" s="34" t="s">
-        <v>404</v>
+        <v>484</v>
       </c>
       <c r="L29" s="13">
         <v>39</v>
       </c>
       <c r="M29" s="37" t="s">
-        <v>405</v>
+        <v>455</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A30" s="23" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B30" s="24" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="C30" s="24" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="D30" s="24" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="E30" s="25">
         <v>23.9</v>
@@ -6099,30 +6100,30 @@
         <v>6</v>
       </c>
       <c r="K30" s="34" t="s">
-        <v>431</v>
+        <v>488</v>
       </c>
       <c r="L30" s="13">
         <v>26</v>
       </c>
       <c r="M30" s="37" t="s">
-        <v>432</v>
+        <v>456</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A31" s="23" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="B31" s="24" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="C31" s="24" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="D31" s="24" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E31" s="25" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="F31" s="25">
         <v>3</v>
@@ -6140,33 +6141,33 @@
         <v>4</v>
       </c>
       <c r="K31" s="34" t="s">
-        <v>391</v>
+        <v>428</v>
       </c>
       <c r="L31" s="13">
         <v>38</v>
       </c>
       <c r="M31" s="37" t="s">
-        <v>450</v>
+        <v>457</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A32" s="23" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="B32" s="24" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C32" s="24" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="D32" s="24" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="E32" s="25" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="F32" s="25" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G32" s="24">
         <v>60</v>
@@ -6181,30 +6182,30 @@
         <v>4</v>
       </c>
       <c r="K32" s="34" t="s">
-        <v>383</v>
+        <v>458</v>
       </c>
       <c r="L32" s="13">
         <v>15</v>
       </c>
       <c r="M32" s="37" t="s">
-        <v>384</v>
+        <v>459</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A33" s="23" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="B33" s="24" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C33" s="24" t="s">
+        <v>281</v>
+      </c>
+      <c r="D33" s="24" t="s">
         <v>285</v>
       </c>
-      <c r="D33" s="24" t="s">
-        <v>289</v>
-      </c>
       <c r="E33" s="25" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="F33" s="25">
         <v>93</v>
@@ -6222,30 +6223,30 @@
         <v>5</v>
       </c>
       <c r="K33" s="34" t="s">
-        <v>417</v>
+        <v>492</v>
       </c>
       <c r="L33" s="13">
         <v>58</v>
       </c>
       <c r="M33" s="37" t="s">
-        <v>418</v>
+        <v>460</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A34" s="23" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="B34" s="24" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="C34" s="24" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="D34" s="24" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="E34" s="25" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="F34" s="25">
         <v>74</v>
@@ -6263,30 +6264,30 @@
         <v>5</v>
       </c>
       <c r="K34" s="34" t="s">
-        <v>413</v>
+        <v>485</v>
       </c>
       <c r="L34" s="13">
         <v>39</v>
       </c>
       <c r="M34" s="37" t="s">
-        <v>414</v>
+        <v>461</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A35" s="23" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B35" s="24" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="C35" s="24" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="D35" s="24" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="E35" s="25" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="F35" s="25">
         <v>55</v>
@@ -6304,30 +6305,30 @@
         <v>4</v>
       </c>
       <c r="K35" s="34" t="s">
-        <v>375</v>
+        <v>462</v>
       </c>
       <c r="L35" s="13">
         <v>17</v>
       </c>
       <c r="M35" s="37" t="s">
-        <v>376</v>
+        <v>463</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A36" s="23" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="B36" s="24" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="C36" s="24" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="D36" s="24" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E36" s="25" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="F36" s="25">
         <v>53</v>
@@ -6345,30 +6346,30 @@
         <v>4</v>
       </c>
       <c r="K36" s="34" t="s">
-        <v>377</v>
+        <v>493</v>
       </c>
       <c r="L36" s="13">
         <v>27</v>
       </c>
       <c r="M36" s="37" t="s">
-        <v>378</v>
+        <v>464</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A37" s="23" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B37" s="24" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C37" s="24" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="D37" s="24" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="E37" s="25" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="F37" s="25">
         <v>27</v>
@@ -6386,30 +6387,30 @@
         <v>3</v>
       </c>
       <c r="K37" s="34" t="s">
-        <v>402</v>
+        <v>465</v>
       </c>
       <c r="L37" s="13">
         <v>18</v>
       </c>
       <c r="M37" s="37" t="s">
-        <v>403</v>
+        <v>466</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A38" s="23" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B38" s="24" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="C38" s="24" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="D38" s="24" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="E38" s="25" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="F38" s="25">
         <v>5</v>
@@ -6427,33 +6428,33 @@
         <v>5</v>
       </c>
       <c r="K38" s="34" t="s">
-        <v>397</v>
+        <v>467</v>
       </c>
       <c r="L38" s="13">
         <v>35</v>
       </c>
       <c r="M38" s="37" t="s">
-        <v>398</v>
+        <v>468</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A39" s="23" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="B39" s="24" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="C39" s="24" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="D39" s="24" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="E39" s="25" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="F39" s="25" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G39" s="24">
         <v>32</v>
@@ -6468,33 +6469,33 @@
         <v>4</v>
       </c>
       <c r="K39" s="34" t="s">
-        <v>400</v>
+        <v>477</v>
       </c>
       <c r="L39" s="13">
         <v>22</v>
       </c>
       <c r="M39" s="37" t="s">
-        <v>428</v>
+        <v>469</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A40" s="23" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="B40" s="24" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="C40" s="24" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="D40" s="24" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="E40" s="25" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="F40" s="25" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G40" s="24">
         <v>15</v>
@@ -6509,33 +6510,33 @@
         <v>5</v>
       </c>
       <c r="K40" s="34" t="s">
-        <v>435</v>
+        <v>486</v>
       </c>
       <c r="L40" s="13">
         <v>18</v>
       </c>
       <c r="M40" s="37" t="s">
-        <v>436</v>
+        <v>470</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A41" s="23" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="B41" s="24" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="C41" s="24" t="s">
+        <v>301</v>
+      </c>
+      <c r="D41" s="24" t="s">
         <v>305</v>
       </c>
-      <c r="D41" s="24" t="s">
-        <v>309</v>
-      </c>
       <c r="E41" s="25" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="F41" s="25" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G41" s="24">
         <v>17</v>
@@ -6550,30 +6551,30 @@
         <v>3</v>
       </c>
       <c r="K41" s="34" t="s">
-        <v>446</v>
+        <v>471</v>
       </c>
       <c r="L41" s="13">
         <v>16</v>
       </c>
       <c r="M41" s="37" t="s">
-        <v>447</v>
+        <v>472</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A42" s="23" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="B42" s="24" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="C42" s="24" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="D42" s="24" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E42" s="25" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="F42" s="25">
         <v>102</v>
@@ -6591,30 +6592,30 @@
         <v>3</v>
       </c>
       <c r="K42" s="34" t="s">
-        <v>395</v>
+        <v>473</v>
       </c>
       <c r="L42" s="13">
         <v>13</v>
       </c>
       <c r="M42" s="37" t="s">
-        <v>396</v>
+        <v>474</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A43" s="27" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="B43" s="28" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="C43" s="28" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="D43" s="28" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="E43" s="29" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="F43" s="29">
         <v>14</v>
@@ -6632,13 +6633,13 @@
         <v>6</v>
       </c>
       <c r="K43" s="38" t="s">
-        <v>421</v>
+        <v>494</v>
       </c>
       <c r="L43" s="14">
         <v>27</v>
       </c>
       <c r="M43" s="39" t="s">
-        <v>422</v>
+        <v>475</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating tables to contain all info
</commit_message>
<xml_diff>
--- a/assets/data/BenchInfo.xlsx
+++ b/assets/data/BenchInfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fariakn\Research\resess.github.io\artifacts\MobileCoverage\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF31AEB-C2B9-4049-88FA-DC5EB744700C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DABA38E-83A8-4F20-8EA6-1070EA9EFEF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" xr2:uid="{2D0D9300-A13D-45F3-88AA-A9A4F06330F2}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="502">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="502">
   <si>
     <t>App name</t>
   </si>
@@ -2226,19 +2226,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{570D0CD3-3FB1-4EBA-8F90-C94D00E6CE1D}">
   <dimension ref="A1:M48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="90" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="26.76953125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="36.31640625" style="2" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="17.453125" style="2" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="26.2265625" style="2" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="19" style="2" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="25.54296875" style="2" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="22.08984375" style="2" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="17.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.04296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.6796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.453125" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.58984375" customWidth="1"/>
     <col min="9" max="9" width="12.31640625" customWidth="1"/>
     <col min="10" max="10" width="20.7265625" customWidth="1"/>
@@ -2625,7 +2625,7 @@
         <v>136</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>138</v>
@@ -2675,7 +2675,7 @@
         <v>2012</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="G11" s="4">
         <v>4</v>
@@ -3914,8 +3914,8 @@
       <c r="B42" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="C42" s="4" t="s">
-        <v>137</v>
+      <c r="C42" s="4">
+        <v>2.2000000000000002</v>
       </c>
       <c r="D42" s="4">
         <v>2.2000000000000002</v>

</xml_diff>